<commit_message>
Created 3 utility modules to better organize functions
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!$A$1:$B$48</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$G$22</definedName>
     <definedName name="cLastDataDate">Parameters!#REF!</definedName>
     <definedName name="clEntryLimit">Parameters!$B$5</definedName>
     <definedName name="cLineUpURL">Parameters!$B$2</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="452">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -50,9 +50,6 @@
     <t>script_name_0</t>
   </si>
   <si>
-    <t>test.py</t>
-  </si>
-  <si>
     <t>script_path_0</t>
   </si>
   <si>
@@ -74,27 +71,12 @@
     <t>C:\Users\Cole\Desktop\FanduelV2\fanduel\modules\gameday\build_all.py</t>
   </si>
   <si>
-    <t>C:\Users\Cole\Desktop\FanduelV2\fanduel\modules\test.py</t>
-  </si>
-  <si>
-    <t>data_scrapping.py</t>
-  </si>
-  <si>
-    <t>C:\Users\Cole\Desktop\FanduelV2\fanduel\modules\data_scrapping.py</t>
-  </si>
-  <si>
     <t>script_name_2</t>
   </si>
   <si>
     <t>script_path_2</t>
   </si>
   <si>
-    <t>database_operations.py</t>
-  </si>
-  <si>
-    <t>C:\Users\Cole\Desktop\FanduelV2\fanduel\modules\database_operations.py</t>
-  </si>
-  <si>
     <t>script_name_3</t>
   </si>
   <si>
@@ -104,9 +86,6 @@
     <t>main.py</t>
   </si>
   <si>
-    <t>C:\Users\Cole\Desktop\FanduelV2\fanduel\modules\main.py</t>
-  </si>
-  <si>
     <t>script_name_4</t>
   </si>
   <si>
@@ -1407,6 +1386,18 @@
   </si>
   <si>
     <t>Education</t>
+  </si>
+  <si>
+    <t>CS 258 - Software testing</t>
+  </si>
+  <si>
+    <t>CS 212 - Design of computer programs</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>C:\Users\Cole\Desktop\FanDuel\fanduel\modules\main.py</t>
   </si>
 </sst>
 </file>
@@ -2066,11 +2057,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="209605376"/>
-        <c:axId val="209606912"/>
+        <c:axId val="209404672"/>
+        <c:axId val="209406208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="209605376"/>
+        <c:axId val="209404672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209606912"/>
+        <c:crossAx val="209406208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2087,7 +2078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209606912"/>
+        <c:axId val="209406208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209605376"/>
+        <c:crossAx val="209404672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2211,11 +2202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209635200"/>
-        <c:axId val="209636736"/>
+        <c:axId val="209434496"/>
+        <c:axId val="209436032"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="209635200"/>
+        <c:axId val="209434496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209636736"/>
+        <c:crossAx val="209436032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2232,7 +2223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209636736"/>
+        <c:axId val="209436032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209635200"/>
+        <c:crossAx val="209434496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2378,11 +2369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210038784"/>
-        <c:axId val="210040320"/>
+        <c:axId val="210186240"/>
+        <c:axId val="210187776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210038784"/>
+        <c:axId val="210186240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2392,12 +2383,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210040320"/>
+        <c:crossAx val="210187776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210040320"/>
+        <c:axId val="210187776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2408,7 +2399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210038784"/>
+        <c:crossAx val="210186240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3091,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3099,79 +3090,79 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3203,34 +3194,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3238,7 +3229,7 @@
         <v>42015</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C2" s="5">
         <v>723.2</v>
@@ -3250,7 +3241,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G2">
         <v>1.8</v>
@@ -3263,7 +3254,7 @@
         <v>0.33750000000000002</v>
       </c>
       <c r="J2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3271,7 +3262,7 @@
         <v>42015</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C3" s="5">
         <v>1096.8</v>
@@ -3283,7 +3274,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G3" s="5">
         <v>3.6</v>
@@ -3296,7 +3287,7 @@
         <v>0.375</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3304,7 +3295,7 @@
         <v>42015</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C4" s="5">
         <v>1716.5</v>
@@ -3316,7 +3307,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G4" s="5">
         <v>9</v>
@@ -3329,7 +3320,7 @@
         <v>0.35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3337,7 +3328,7 @@
         <v>42015</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C5" s="5">
         <v>933.8</v>
@@ -3349,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G5" s="5">
         <v>1.8</v>
@@ -3362,7 +3353,7 @@
         <v>0.3</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3370,7 +3361,7 @@
         <v>42020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C6" s="5">
         <v>657.45</v>
@@ -3382,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G6" s="5">
         <v>1.8</v>
@@ -3395,7 +3386,7 @@
         <v>0.23749999999999999</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3403,7 +3394,7 @@
         <v>42020</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C7" s="5">
         <v>538</v>
@@ -3415,7 +3406,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G7">
         <v>9</v>
@@ -3428,7 +3419,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3436,7 +3427,7 @@
         <v>42020</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C8" s="5">
         <v>699.95</v>
@@ -3448,7 +3439,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G8">
         <v>1.8</v>
@@ -3461,7 +3452,7 @@
         <v>0.26250000000000001</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3469,7 +3460,7 @@
         <v>42021</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="C9" s="5">
         <v>2493.6999999999998</v>
@@ -3481,7 +3472,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3494,7 +3485,7 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3502,7 +3493,7 @@
         <v>42024</v>
       </c>
       <c r="B10" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="C10" s="5">
         <v>1750.3</v>
@@ -3514,10 +3505,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3525,7 +3516,7 @@
         <v>42024</v>
       </c>
       <c r="B11" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="C11" s="5">
         <v>3036</v>
@@ -3537,10 +3528,10 @@
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3548,7 +3539,7 @@
         <v>42024</v>
       </c>
       <c r="B12" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C12" s="5">
         <v>1702.55</v>
@@ -3560,10 +3551,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3571,7 +3562,7 @@
         <v>42024</v>
       </c>
       <c r="B13" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C13" s="5">
         <v>1733.4</v>
@@ -3583,10 +3574,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3609,10 +3600,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,376 +3616,391 @@
     <col min="6" max="6" width="31.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="D6" s="6">
         <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D7" s="6">
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6">
         <v>3</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D9" s="6">
         <v>3</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D10" s="6">
         <v>3</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6">
         <v>4</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D12" s="6">
         <v>5</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D14" s="6">
         <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D15" s="6">
         <v>4</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D16" s="6">
         <v>4</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D17" s="6">
         <v>5</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D18" s="6">
         <v>6</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="D20" s="6">
         <v>4</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F13">
-    <sortState ref="A2:F14">
-      <sortCondition ref="D1:D14"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4024,19 +4030,19 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="M2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -4050,7 +4056,7 @@
         <v>-1</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="M3" s="14">
         <v>-1</v>
@@ -4058,7 +4064,7 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C4" s="14">
         <v>-10</v>
@@ -4067,7 +4073,7 @@
         <v>-1</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="M4" s="14">
         <v>-1</v>
@@ -4096,22 +4102,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3">
         <v>696</v>
@@ -4119,15 +4125,15 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -4135,7 +4141,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B6">
         <v>10000</v>
@@ -4194,15 +4200,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -4210,7 +4216,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -4218,7 +4224,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -4226,7 +4232,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B5">
         <v>16</v>
@@ -4234,7 +4240,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>17</v>
@@ -4242,7 +4248,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B7">
         <v>18</v>
@@ -4250,7 +4256,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -4258,7 +4264,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -4266,7 +4272,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B10">
         <v>21</v>
@@ -4274,7 +4280,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B11" s="5">
         <v>22</v>
@@ -4282,7 +4288,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B12" s="5">
         <v>23</v>
@@ -4290,7 +4296,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B13" s="5">
         <v>24</v>
@@ -4298,7 +4304,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B14" s="5">
         <v>25</v>
@@ -4306,7 +4312,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B15" s="5">
         <v>26</v>
@@ -4314,7 +4320,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B16" s="5">
         <v>27</v>
@@ -4322,7 +4328,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B17" s="5">
         <v>28</v>
@@ -4330,7 +4336,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B18" s="5">
         <v>29</v>
@@ -4338,7 +4344,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B19" s="5">
         <v>30</v>
@@ -4346,7 +4352,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B20" s="5">
         <v>31</v>
@@ -4354,7 +4360,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B21" s="5">
         <v>32</v>
@@ -4362,7 +4368,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B22" s="5">
         <v>33</v>
@@ -4370,7 +4376,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B23" s="5">
         <v>34</v>
@@ -4378,7 +4384,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B24" s="5">
         <v>35</v>
@@ -4386,7 +4392,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B25" s="5">
         <v>36</v>
@@ -4394,7 +4400,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B26" s="5">
         <v>37</v>
@@ -4402,7 +4408,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B27" s="5">
         <v>38</v>
@@ -4410,7 +4416,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B28" s="5">
         <v>39</v>
@@ -4418,7 +4424,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B29" s="5">
         <v>40</v>
@@ -4426,7 +4432,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B30" s="5">
         <v>41</v>
@@ -4434,7 +4440,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B31" s="5">
         <v>42</v>
@@ -4473,1623 +4479,1623 @@
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="G2" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="H2" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="I2" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J2" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="K2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C6" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D6" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B7" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F7" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G7" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E8" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C9" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D9" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="E9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B10" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D10" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D11" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="E11" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F11" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G11" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H11" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I11" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C13" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E13" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F13" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G13" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B14" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C14" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D14" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B15" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F15" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="G15" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H15" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I15" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D16" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E17" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="F17" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="G17" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H17" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="I17" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="J17" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="K17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B18" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="D18" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E18" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G18" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C19" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D19" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E19" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C20" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D20" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E20" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C21" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B22" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C22" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D22" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B23" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D23" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E23" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F23" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="G23" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="B24" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D24" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E24" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C25" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="B26" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="B27" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C27" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E27" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F27" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="G27" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H27" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I27" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J27" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C28" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D28" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E28" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F28" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G28" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H28" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I28" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J28" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C29" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D29" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E29" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="F29" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="G29" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H29" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="I29" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="J29" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B30" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C30" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="D30" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E30" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F30" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B31" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C31" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E31" t="s">
+        <v>238</v>
+      </c>
+      <c r="F31" t="s">
+        <v>239</v>
+      </c>
+      <c r="G31" t="s">
+        <v>240</v>
+      </c>
+      <c r="H31" t="s">
+        <v>241</v>
+      </c>
+      <c r="I31" t="s">
+        <v>242</v>
+      </c>
+      <c r="J31" t="s">
         <v>243</v>
-      </c>
-      <c r="D31" t="s">
-        <v>244</v>
-      </c>
-      <c r="E31" t="s">
-        <v>245</v>
-      </c>
-      <c r="F31" t="s">
-        <v>246</v>
-      </c>
-      <c r="G31" t="s">
-        <v>247</v>
-      </c>
-      <c r="H31" t="s">
-        <v>248</v>
-      </c>
-      <c r="I31" t="s">
-        <v>249</v>
-      </c>
-      <c r="J31" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B32" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C32" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C33" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D33" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E33" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B34" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C34" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E34" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F34" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="G34" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H34" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="B35" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C35" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E35" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="F35" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G35" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B36" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="C36" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D36" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E36" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F36" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G36" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B37" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="C37" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="D37" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E37" t="s">
+        <v>208</v>
+      </c>
+      <c r="F37" t="s">
+        <v>250</v>
+      </c>
+      <c r="G37" t="s">
         <v>215</v>
-      </c>
-      <c r="F37" t="s">
-        <v>257</v>
-      </c>
-      <c r="G37" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B38" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C38" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D38" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E38" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F38" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G38" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D39" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D40" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E40" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F40" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G40" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="B41" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="C41" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D41" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E41" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F41" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="G41" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="H41" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B42" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B43" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="C43" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D43" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="E43" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F43" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="G43" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B44" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E44" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F44" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G44" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B45" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C45" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D45" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E45" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>234</v>
+      </c>
+      <c r="B46" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" t="s">
+        <v>237</v>
+      </c>
+      <c r="E46" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" t="s">
+        <v>239</v>
+      </c>
+      <c r="G46" t="s">
+        <v>240</v>
+      </c>
+      <c r="H46" t="s">
+        <v>300</v>
+      </c>
+      <c r="I46" t="s">
         <v>241</v>
       </c>
-      <c r="B46" t="s">
+      <c r="J46" t="s">
         <v>242</v>
       </c>
-      <c r="C46" t="s">
+      <c r="K46" t="s">
         <v>243</v>
-      </c>
-      <c r="D46" t="s">
-        <v>244</v>
-      </c>
-      <c r="E46" t="s">
-        <v>245</v>
-      </c>
-      <c r="F46" t="s">
-        <v>246</v>
-      </c>
-      <c r="G46" t="s">
-        <v>247</v>
-      </c>
-      <c r="H46" t="s">
-        <v>307</v>
-      </c>
-      <c r="I46" t="s">
-        <v>248</v>
-      </c>
-      <c r="J46" t="s">
-        <v>249</v>
-      </c>
-      <c r="K46" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B47" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="C47" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D47" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E47" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F47" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G47" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D48" t="s">
+        <v>238</v>
+      </c>
+      <c r="E48" t="s">
+        <v>239</v>
+      </c>
+      <c r="F48" t="s">
+        <v>240</v>
+      </c>
+      <c r="G48" t="s">
+        <v>241</v>
+      </c>
+      <c r="H48" t="s">
+        <v>242</v>
+      </c>
+      <c r="I48" t="s">
         <v>243</v>
-      </c>
-      <c r="C48" t="s">
-        <v>244</v>
-      </c>
-      <c r="D48" t="s">
-        <v>245</v>
-      </c>
-      <c r="E48" t="s">
-        <v>246</v>
-      </c>
-      <c r="F48" t="s">
-        <v>247</v>
-      </c>
-      <c r="G48" t="s">
-        <v>248</v>
-      </c>
-      <c r="H48" t="s">
-        <v>249</v>
-      </c>
-      <c r="I48" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B49" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C49" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D49" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E49" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B50" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C50" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D50" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="E50" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B51" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C51" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D51" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E51" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F51" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G51" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B52" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="C52" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D52" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="E52" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B53" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="D53" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E53" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B54" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C54" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="D54" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B55" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C55" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="D55" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E55" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="F55" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="B56" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="D56" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E56" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B57" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C57" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D57" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E57" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B58" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C58" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D58" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B59" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C59" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D59" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="B60" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C60" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E60" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B61" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D61" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B62" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C62" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D62" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E62" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B63" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B64" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B65" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C65" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B66" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C66" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D66" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B67" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C67" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D67" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="E67" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B68" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B70" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C70" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B72" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C72" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D72" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B73" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C73" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D73" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E73" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F73" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G73" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C74" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D74" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B75" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C75" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D75" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B76" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C77" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D77" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="E77" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F77" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G77" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="B78" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C78" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D78" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="B79" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B80" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C80" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D80" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B81" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C81" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D81" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B82" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C82" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D82" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E82" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B83" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C83" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B84" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C84" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D84" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B85" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C85" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D85" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B86" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C86" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D86" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E86" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B87" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C87" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="B88" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C88" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="D88" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="E88" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="F88" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B89" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C89" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="D89" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E89" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B90" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C90" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D90" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="E90" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6114,170 +6120,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -6304,30 +6310,30 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D2" s="10">
         <v>637.32000000000005</v>
@@ -6344,13 +6350,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D3" s="10">
         <v>699.12</v>
@@ -6367,13 +6373,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D4" s="10">
         <v>717.35416666699996</v>
@@ -6390,13 +6396,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B5" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D5" s="10">
         <v>593.9</v>
@@ -6413,13 +6419,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B6" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D6" s="10">
         <v>793.3125</v>
@@ -6436,13 +6442,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B7" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D7" s="10">
         <v>832.125</v>
@@ -6459,13 +6465,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B8" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D8" s="10">
         <v>824.72500000000002</v>
@@ -6482,13 +6488,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B9" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D9" s="10">
         <v>-569.35913249999999</v>
@@ -6505,13 +6511,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B10" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D10" s="10">
         <v>409.64</v>
@@ -6563,21 +6569,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B2">
         <v>3403.3</v>
@@ -6591,7 +6597,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="B3">
         <v>1913.05</v>
@@ -6605,7 +6611,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B4">
         <v>1943.25</v>
@@ -6619,7 +6625,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B5">
         <v>1733.4</v>

</xml_diff>

<commit_message>
updated database connection to be function call
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -2057,11 +2057,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="209404672"/>
-        <c:axId val="209406208"/>
+        <c:axId val="217797376"/>
+        <c:axId val="217798912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="209404672"/>
+        <c:axId val="217797376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,7 +2070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209406208"/>
+        <c:crossAx val="217798912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2078,7 +2078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209406208"/>
+        <c:axId val="217798912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2089,7 +2089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209404672"/>
+        <c:crossAx val="217797376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2202,11 +2202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209434496"/>
-        <c:axId val="209436032"/>
+        <c:axId val="217827200"/>
+        <c:axId val="217828736"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="209434496"/>
+        <c:axId val="217827200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209436032"/>
+        <c:crossAx val="217828736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2223,7 +2223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209436032"/>
+        <c:axId val="217828736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209434496"/>
+        <c:crossAx val="217827200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2369,11 +2369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210186240"/>
-        <c:axId val="210187776"/>
+        <c:axId val="218234880"/>
+        <c:axId val="218236416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210186240"/>
+        <c:axId val="218234880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,12 +2383,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210187776"/>
+        <c:crossAx val="218236416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210187776"/>
+        <c:axId val="218236416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2399,7 +2399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210186240"/>
+        <c:crossAx val="218234880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3602,7 +3602,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4002,6 +4002,7 @@
   </sheetData>
   <autoFilter ref="A1:G22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4090,7 +4091,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 'table' to db write to modularize extend function call to parameterize table write
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -2057,11 +2057,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="217797376"/>
-        <c:axId val="217798912"/>
+        <c:axId val="221664000"/>
+        <c:axId val="221665536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217797376"/>
+        <c:axId val="221664000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,7 +2070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217798912"/>
+        <c:crossAx val="221665536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2078,7 +2078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217798912"/>
+        <c:axId val="221665536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2089,7 +2089,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217797376"/>
+        <c:crossAx val="221664000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2202,11 +2202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217827200"/>
-        <c:axId val="217828736"/>
+        <c:axId val="221697920"/>
+        <c:axId val="221699456"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="217827200"/>
+        <c:axId val="221697920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217828736"/>
+        <c:crossAx val="221699456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2223,7 +2223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217828736"/>
+        <c:axId val="221699456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217827200"/>
+        <c:crossAx val="221697920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2369,11 +2369,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218234880"/>
-        <c:axId val="218236416"/>
+        <c:axId val="222101504"/>
+        <c:axId val="222103040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218234880"/>
+        <c:axId val="222101504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,12 +2383,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218236416"/>
+        <c:crossAx val="222103040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218236416"/>
+        <c:axId val="222103040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2399,7 +2399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218234880"/>
+        <c:crossAx val="222101504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>

<commit_message>
refactored dbo, column definitions now accept functions parsed by python eval
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Performance Monitoring" sheetId="13" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!$A$1:$B$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$G$22</definedName>
     <definedName name="cLastDataDate">Parameters!#REF!</definedName>
     <definedName name="clEntryLimit">Parameters!$B$5</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="380">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -530,9 +530,6 @@
     <t>Lineups Cache</t>
   </si>
   <si>
-    <t>Patrick Kane</t>
-  </si>
-  <si>
     <t>Matt Carle</t>
   </si>
   <si>
@@ -563,9 +560,6 @@
     <t>Max Avg Wins Threshold</t>
   </si>
   <si>
-    <t>Brent Seabrook</t>
-  </si>
-  <si>
     <t>Contest Date</t>
   </si>
   <si>
@@ -632,18 +626,9 @@
     <t>Ryan Carter</t>
   </si>
   <si>
-    <t>Matt Stajan</t>
-  </si>
-  <si>
     <t>Pascal Dupuis</t>
   </si>
   <si>
-    <t>Mark Fayne</t>
-  </si>
-  <si>
-    <t>Liam O'Brien</t>
-  </si>
-  <si>
     <t>Patrick Dwyer</t>
   </si>
   <si>
@@ -671,15 +656,6 @@
     <t>Andrew Cogliano</t>
   </si>
   <si>
-    <t>Kyle Quincey</t>
-  </si>
-  <si>
-    <t>Kyle Turris</t>
-  </si>
-  <si>
-    <t>Kyle Palmieri</t>
-  </si>
-  <si>
     <t>Dmitry Orlov</t>
   </si>
   <si>
@@ -695,12 +671,6 @@
     <t>Patric Hornqvist</t>
   </si>
   <si>
-    <t>Patrick Maroon</t>
-  </si>
-  <si>
-    <t>Troy Brouwer</t>
-  </si>
-  <si>
     <t>Nathan Gerbe</t>
   </si>
   <si>
@@ -722,27 +692,12 @@
     <t>Carl Hagelin</t>
   </si>
   <si>
-    <t>Jason Garrison</t>
-  </si>
-  <si>
-    <t>Anthony Duclair</t>
-  </si>
-  <si>
-    <t>Anthony Peluso</t>
-  </si>
-  <si>
-    <t>Blake Comeau</t>
-  </si>
-  <si>
     <t>Matthew Lombardi</t>
   </si>
   <si>
     <t>Matt Dumba</t>
   </si>
   <si>
-    <t>Brian Gibbons</t>
-  </si>
-  <si>
     <t>Brian Elliott</t>
   </si>
   <si>
@@ -776,15 +731,6 @@
     <t>Chris Kelly</t>
   </si>
   <si>
-    <t>Jared Cowen</t>
-  </si>
-  <si>
-    <t>Ian Cole</t>
-  </si>
-  <si>
-    <t>Emerson Etem</t>
-  </si>
-  <si>
     <t>Jamie Benn</t>
   </si>
   <si>
@@ -797,9 +743,6 @@
     <t>Colin Wilson</t>
   </si>
   <si>
-    <t>Olli Maatta</t>
-  </si>
-  <si>
     <t>Calvin de Haan</t>
   </si>
   <si>
@@ -842,18 +785,6 @@
     <t>Jordan Eberle</t>
   </si>
   <si>
-    <t>Jeff Zatkoff</t>
-  </si>
-  <si>
-    <t>Jeff Carter</t>
-  </si>
-  <si>
-    <t>Scott Hartnell</t>
-  </si>
-  <si>
-    <t>Scott Hannan</t>
-  </si>
-  <si>
     <t>Tomas Vokoun</t>
   </si>
   <si>
@@ -869,36 +800,12 @@
     <t>Keith Aulie</t>
   </si>
   <si>
-    <t>Justin Peters</t>
-  </si>
-  <si>
-    <t>Justin Abdelkader</t>
-  </si>
-  <si>
-    <t>Justin Fontaine</t>
-  </si>
-  <si>
-    <t>Justin Braun</t>
-  </si>
-  <si>
     <t>Jason Demers</t>
   </si>
   <si>
-    <t>Martin St. Louis</t>
-  </si>
-  <si>
-    <t>Bryan Bickell</t>
-  </si>
-  <si>
     <t>Kris Letang</t>
   </si>
   <si>
-    <t>Derrick Pouliot</t>
-  </si>
-  <si>
-    <t>Lubomir Visnovsky</t>
-  </si>
-  <si>
     <t>S119446122</t>
   </si>
   <si>
@@ -929,63 +836,24 @@
     <t>Luke Schenn</t>
   </si>
   <si>
-    <t>Patrick Eaves</t>
-  </si>
-  <si>
-    <t>Patrik Elias</t>
-  </si>
-  <si>
-    <t>Patrick Kaleta</t>
-  </si>
-  <si>
-    <t>Patrick Sharp</t>
-  </si>
-  <si>
-    <t>Dion Phaneuf</t>
-  </si>
-  <si>
     <t>Chris Neil</t>
   </si>
   <si>
-    <t>Chris Phillips</t>
-  </si>
-  <si>
     <t>Chris Kunitz</t>
   </si>
   <si>
-    <t>Chris VandeVelde</t>
-  </si>
-  <si>
-    <t>Martin Erat</t>
-  </si>
-  <si>
-    <t>Keith Yandle</t>
-  </si>
-  <si>
     <t>Joey MacDonald</t>
   </si>
   <si>
     <t>Andrew MacDonald</t>
   </si>
   <si>
-    <t>Joe Thornton</t>
-  </si>
-  <si>
-    <t>John Moore</t>
-  </si>
-  <si>
-    <t>Marcus Johansson</t>
-  </si>
-  <si>
     <t>Andrei Vasilevskii</t>
   </si>
   <si>
     <t>Matt Ellis</t>
   </si>
   <si>
-    <t>Matt Read</t>
-  </si>
-  <si>
     <t>Maxime Fortunus</t>
   </si>
   <si>
@@ -1019,18 +887,6 @@
     <t>Rich Peverley</t>
   </si>
   <si>
-    <t>Mikael Granlund</t>
-  </si>
-  <si>
-    <t>Mikael Backlund</t>
-  </si>
-  <si>
-    <t>Markus Granlund</t>
-  </si>
-  <si>
-    <t>Michael Grabner</t>
-  </si>
-  <si>
     <t>Josh Harding</t>
   </si>
   <si>
@@ -1040,21 +896,9 @@
     <t>Josh Bailey</t>
   </si>
   <si>
-    <t>Brian Flynn</t>
-  </si>
-  <si>
-    <t>Brian Boyle</t>
-  </si>
-  <si>
     <t>Kristers Gudlevskis</t>
   </si>
   <si>
-    <t>Andrew Ladd</t>
-  </si>
-  <si>
-    <t>Andrew Shaw</t>
-  </si>
-  <si>
     <t>Oliver Lauridsen</t>
   </si>
   <si>
@@ -1070,39 +914,12 @@
     <t>Alexei Emelin</t>
   </si>
   <si>
-    <t>David Moss</t>
-  </si>
-  <si>
-    <t>David Pastrnak</t>
-  </si>
-  <si>
-    <t>David Jones</t>
-  </si>
-  <si>
-    <t>Stu Bickel</t>
-  </si>
-  <si>
     <t>Mathew Dumba</t>
   </si>
   <si>
-    <t>Radko Gudas</t>
-  </si>
-  <si>
-    <t>Jakub Kindl</t>
-  </si>
-  <si>
     <t>Quinton Howden</t>
   </si>
   <si>
-    <t>Johan Franzen</t>
-  </si>
-  <si>
-    <t>Jannik Hansen</t>
-  </si>
-  <si>
-    <t>Marcus Kruger</t>
-  </si>
-  <si>
     <t>Jason Williams</t>
   </si>
   <si>
@@ -1118,36 +935,6 @@
     <t>Stefan Elliott</t>
   </si>
   <si>
-    <t>Mark Pysyk</t>
-  </si>
-  <si>
-    <t>Alex Grant</t>
-  </si>
-  <si>
-    <t>Alex Tanguay</t>
-  </si>
-  <si>
-    <t>Alex Killorn</t>
-  </si>
-  <si>
-    <t>Alex Pietrangelo</t>
-  </si>
-  <si>
-    <t>Alex Chiasson</t>
-  </si>
-  <si>
-    <t>Brett Sutter</t>
-  </si>
-  <si>
-    <t>Brandon Sutter</t>
-  </si>
-  <si>
-    <t>Brett Ritchie</t>
-  </si>
-  <si>
-    <t>Brent Burns</t>
-  </si>
-  <si>
     <t>Ryan Callahan</t>
   </si>
   <si>
@@ -1235,18 +1022,6 @@
     <t>Bobby Butler</t>
   </si>
   <si>
-    <t>Andrew Ebbett</t>
-  </si>
-  <si>
-    <t>Andre Benoit</t>
-  </si>
-  <si>
-    <t>Artem Anisimov</t>
-  </si>
-  <si>
-    <t>Karri Ramo</t>
-  </si>
-  <si>
     <t>Patrice Cormier</t>
   </si>
   <si>
@@ -1259,12 +1034,6 @@
     <t>John Carlson</t>
   </si>
   <si>
-    <t>Eric Brewer</t>
-  </si>
-  <si>
-    <t>Eric Fehr</t>
-  </si>
-  <si>
     <t>Nathan Horton</t>
   </si>
   <si>
@@ -1277,12 +1046,6 @@
     <t>John Klingberg</t>
   </si>
   <si>
-    <t>Jason LaBarbera</t>
-  </si>
-  <si>
-    <t>Jason Chimera</t>
-  </si>
-  <si>
     <t>Brad Winchester</t>
   </si>
   <si>
@@ -1298,12 +1061,6 @@
     <t>Chad LaRose</t>
   </si>
   <si>
-    <t>Marcus Foligno</t>
-  </si>
-  <si>
-    <t>Nick Foligno</t>
-  </si>
-  <si>
     <t>Ray Whitney</t>
   </si>
   <si>
@@ -1319,12 +1076,6 @@
     <t>Ryan Ellis</t>
   </si>
   <si>
-    <t>Boone Jenner</t>
-  </si>
-  <si>
-    <t>Matt Donovan</t>
-  </si>
-  <si>
     <t>Brad Thiessen</t>
   </si>
   <si>
@@ -1334,9 +1085,6 @@
     <t>Sheldon Brookbank</t>
   </si>
   <si>
-    <t>Reto Berra</t>
-  </si>
-  <si>
     <t>Andrei Loktionov</t>
   </si>
   <si>
@@ -1349,21 +1097,12 @@
     <t>Josh Jooris</t>
   </si>
   <si>
-    <t>Brian Gionta</t>
-  </si>
-  <si>
-    <t>Brian Strait</t>
-  </si>
-  <si>
     <t>Danny Taylor</t>
   </si>
   <si>
     <t>Manny Malhotra</t>
   </si>
   <si>
-    <t>Grant Clitsome</t>
-  </si>
-  <si>
     <t>Matthew Hackett</t>
   </si>
   <si>
@@ -1404,6 +1143,45 @@
   </si>
   <si>
     <t>C:\Users\Cole\Desktop\FanDuel\fanduel\modules\database_operations.py</t>
+  </si>
+  <si>
+    <t>Mat Clark</t>
+  </si>
+  <si>
+    <t>Johan Larsson</t>
+  </si>
+  <si>
+    <t>Patrick Bordeleau</t>
+  </si>
+  <si>
+    <t>Josh Manson</t>
+  </si>
+  <si>
+    <t>Shawn Thornton</t>
+  </si>
+  <si>
+    <t>Andrei Vasilevskiy</t>
+  </si>
+  <si>
+    <t>Andrew Campbell</t>
+  </si>
+  <si>
+    <t>Chris Porter</t>
+  </si>
+  <si>
+    <t>Cory Conacher</t>
+  </si>
+  <si>
+    <t>Chris Tierney</t>
+  </si>
+  <si>
+    <t>Tomas Vincour</t>
+  </si>
+  <si>
+    <t>Jesse Blacker</t>
+  </si>
+  <si>
+    <t>Brian Dumoulin</t>
   </si>
 </sst>
 </file>
@@ -1853,7 +1631,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1866,9 +1644,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2063,11 +1838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="208757504"/>
-        <c:axId val="208759040"/>
+        <c:axId val="216687360"/>
+        <c:axId val="216688896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="208757504"/>
+        <c:axId val="216687360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,7 +1851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208759040"/>
+        <c:crossAx val="216688896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2084,7 +1859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208759040"/>
+        <c:axId val="216688896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2095,7 +1870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208757504"/>
+        <c:crossAx val="216687360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2208,11 +1983,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="208787328"/>
-        <c:axId val="208788864"/>
+        <c:axId val="216717184"/>
+        <c:axId val="216718720"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="208787328"/>
+        <c:axId val="216717184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2221,7 +1996,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208788864"/>
+        <c:crossAx val="216718720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2229,7 +2004,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208788864"/>
+        <c:axId val="216718720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,7 +2015,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208787328"/>
+        <c:crossAx val="216717184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2375,11 +2150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209190912"/>
-        <c:axId val="209192448"/>
+        <c:axId val="218431488"/>
+        <c:axId val="218433024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209190912"/>
+        <c:axId val="218431488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2389,12 +2164,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209192448"/>
+        <c:crossAx val="218433024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209192448"/>
+        <c:axId val="218433024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2405,7 +2180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209190912"/>
+        <c:crossAx val="218431488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3096,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>452</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +2879,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>453</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,7 +2895,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>451</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3200,7 +2975,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
         <v>125</v>
@@ -3215,27 +2990,27 @@
         <v>127</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G1" t="s">
         <v>128</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>42015</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C2" s="5">
         <v>723.2</v>
@@ -3247,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G2">
         <v>1.8</v>
@@ -3260,15 +3035,15 @@
         <v>0.33750000000000002</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>42015</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" s="5">
         <v>1096.8</v>
@@ -3280,7 +3055,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G3" s="5">
         <v>3.6</v>
@@ -3293,15 +3068,15 @@
         <v>0.375</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>42015</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" s="5">
         <v>1716.5</v>
@@ -3313,7 +3088,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G4" s="5">
         <v>9</v>
@@ -3326,15 +3101,15 @@
         <v>0.35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <v>42015</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C5" s="5">
         <v>933.8</v>
@@ -3346,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G5" s="5">
         <v>1.8</v>
@@ -3359,15 +3134,15 @@
         <v>0.3</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>42020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="C6" s="5">
         <v>657.45</v>
@@ -3379,7 +3154,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G6" s="5">
         <v>1.8</v>
@@ -3392,15 +3167,15 @@
         <v>0.23749999999999999</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>42020</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="C7" s="5">
         <v>538</v>
@@ -3412,7 +3187,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G7">
         <v>9</v>
@@ -3425,15 +3200,15 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>42020</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="C8" s="5">
         <v>699.95</v>
@@ -3445,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G8">
         <v>1.8</v>
@@ -3458,15 +3233,15 @@
         <v>0.26250000000000001</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>42021</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>370</v>
+        <v>299</v>
       </c>
       <c r="C9" s="5">
         <v>2493.6999999999998</v>
@@ -3478,7 +3253,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3491,15 +3266,15 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>42024</v>
       </c>
       <c r="B10" t="s">
-        <v>383</v>
+        <v>312</v>
       </c>
       <c r="C10" s="5">
         <v>1750.3</v>
@@ -3511,18 +3286,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>42024</v>
       </c>
       <c r="B11" t="s">
-        <v>384</v>
+        <v>313</v>
       </c>
       <c r="C11" s="5">
         <v>3036</v>
@@ -3534,18 +3309,18 @@
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>42024</v>
       </c>
       <c r="B12" t="s">
-        <v>385</v>
+        <v>314</v>
       </c>
       <c r="C12" s="5">
         <v>1702.55</v>
@@ -3557,18 +3332,18 @@
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>42024</v>
       </c>
       <c r="B13" t="s">
-        <v>386</v>
+        <v>315</v>
       </c>
       <c r="C13" s="5">
         <v>1733.4</v>
@@ -3580,10 +3355,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3642,7 +3417,7 @@
         <v>23</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>450</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3662,7 +3437,7 @@
         <v>51</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>387</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3844,7 +3619,7 @@
         <v>50</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>388</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3969,18 +3744,18 @@
         <v>32</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>389</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>445</v>
+        <v>358</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>446</v>
+        <v>359</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>447</v>
+        <v>360</v>
       </c>
       <c r="D20" s="6">
         <v>4</v>
@@ -3991,18 +3766,18 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>448</v>
+        <v>361</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>447</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>449</v>
+        <v>362</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>447</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4036,53 +3811,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>179</v>
       </c>
       <c r="M2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>42015</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <v>-10</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>-1</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="M3" s="14">
+      <c r="L3" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" s="13">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="13">
         <v>-10</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>-1</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="M4" s="14">
+      <c r="L4" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="M4" s="13">
         <v>-1</v>
       </c>
     </row>
@@ -4097,7 +3872,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -4135,12 +3910,12 @@
         <v>161</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>379</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -4148,7 +3923,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6">
         <v>10000</v>
@@ -4464,90 +4239,76 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A63" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>390</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
         <v>191</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H2" t="s">
+        <v>321</v>
+      </c>
+      <c r="I2" t="s">
+        <v>322</v>
+      </c>
+      <c r="J2" t="s">
         <v>192</v>
       </c>
-      <c r="D2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
         <v>193</v>
-      </c>
-      <c r="F2" t="s">
-        <v>391</v>
-      </c>
-      <c r="G2" t="s">
-        <v>392</v>
-      </c>
-      <c r="H2" t="s">
-        <v>393</v>
-      </c>
-      <c r="I2" t="s">
-        <v>194</v>
-      </c>
-      <c r="J2" t="s">
-        <v>195</v>
-      </c>
-      <c r="K2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" t="s">
-        <v>224</v>
-      </c>
-      <c r="E3" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
-        <v>395</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="D4" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="E4" t="s">
         <v>78</v>
@@ -4555,225 +4316,156 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" t="s">
         <v>194</v>
-      </c>
-      <c r="D5" t="s">
-        <v>195</v>
-      </c>
-      <c r="E5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>396</v>
-      </c>
-      <c r="B6" t="s">
-        <v>293</v>
-      </c>
-      <c r="C6" t="s">
-        <v>371</v>
-      </c>
-      <c r="D6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E6" t="s">
-        <v>78</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>397</v>
+        <v>260</v>
       </c>
       <c r="B7" t="s">
-        <v>398</v>
+        <v>368</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D7" t="s">
-        <v>297</v>
-      </c>
-      <c r="E7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F7" t="s">
-        <v>298</v>
-      </c>
-      <c r="G7" t="s">
-        <v>200</v>
-      </c>
-      <c r="H7" t="s">
-        <v>217</v>
-      </c>
-      <c r="I7" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>399</v>
+        <v>261</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>262</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>300</v>
       </c>
       <c r="D8" t="s">
-        <v>332</v>
-      </c>
-      <c r="E8" t="s">
-        <v>333</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>327</v>
       </c>
       <c r="C9" t="s">
-        <v>371</v>
+        <v>208</v>
       </c>
       <c r="D9" t="s">
-        <v>294</v>
+        <v>195</v>
       </c>
       <c r="E9" t="s">
-        <v>202</v>
+        <v>196</v>
+      </c>
+      <c r="F9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>292</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>293</v>
+        <v>199</v>
       </c>
       <c r="C10" t="s">
-        <v>371</v>
+        <v>200</v>
       </c>
       <c r="D10" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>295</v>
+        <v>328</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>329</v>
       </c>
       <c r="C11" t="s">
-        <v>162</v>
+        <v>368</v>
       </c>
       <c r="D11" t="s">
-        <v>297</v>
+        <v>212</v>
       </c>
       <c r="E11" t="s">
-        <v>202</v>
+        <v>370</v>
       </c>
       <c r="F11" t="s">
-        <v>298</v>
+        <v>230</v>
       </c>
       <c r="G11" t="s">
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="H11" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>400</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D12" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C13" t="s">
-        <v>260</v>
-      </c>
-      <c r="D13" t="s">
-        <v>248</v>
-      </c>
-      <c r="E13" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" t="s">
-        <v>250</v>
-      </c>
-      <c r="G13" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>330</v>
       </c>
       <c r="B14" t="s">
-        <v>261</v>
+        <v>371</v>
       </c>
       <c r="C14" t="s">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="D14" t="s">
-        <v>341</v>
+        <v>209</v>
+      </c>
+      <c r="E14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G14" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>401</v>
+        <v>332</v>
       </c>
       <c r="B15" t="s">
-        <v>402</v>
+        <v>333</v>
       </c>
       <c r="C15" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E15" t="s">
-        <v>202</v>
-      </c>
-      <c r="F15" t="s">
-        <v>222</v>
-      </c>
-      <c r="G15" t="s">
-        <v>200</v>
-      </c>
-      <c r="H15" t="s">
-        <v>217</v>
-      </c>
-      <c r="I15" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4783,168 +4475,90 @@
       <c r="B16" t="s">
         <v>267</v>
       </c>
-      <c r="C16" t="s">
-        <v>304</v>
-      </c>
-      <c r="D16" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>334</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>335</v>
       </c>
       <c r="C17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D17" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" t="s">
-        <v>301</v>
-      </c>
-      <c r="F17" t="s">
-        <v>302</v>
-      </c>
-      <c r="G17" t="s">
-        <v>236</v>
-      </c>
-      <c r="H17" t="s">
-        <v>303</v>
-      </c>
-      <c r="I17" t="s">
-        <v>237</v>
-      </c>
-      <c r="J17" t="s">
-        <v>238</v>
-      </c>
-      <c r="K17" t="s">
-        <v>67</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>403</v>
-      </c>
-      <c r="B18" t="s">
-        <v>404</v>
-      </c>
-      <c r="C18" t="s">
-        <v>222</v>
-      </c>
-      <c r="D18" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18" t="s">
-        <v>249</v>
-      </c>
-      <c r="F18" t="s">
-        <v>250</v>
-      </c>
-      <c r="G18" t="s">
-        <v>215</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>338</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D19" t="s">
-        <v>224</v>
-      </c>
-      <c r="E19" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>339</v>
       </c>
       <c r="B20" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="C20" t="s">
-        <v>309</v>
-      </c>
-      <c r="D20" t="s">
-        <v>201</v>
-      </c>
-      <c r="E20" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>268</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" t="s">
-        <v>299</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>405</v>
+        <v>216</v>
       </c>
       <c r="B22" t="s">
-        <v>406</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>218</v>
-      </c>
-      <c r="D22" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>407</v>
+        <v>270</v>
       </c>
       <c r="B23" t="s">
-        <v>408</v>
-      </c>
-      <c r="C23" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" t="s">
-        <v>220</v>
-      </c>
-      <c r="E23" t="s">
-        <v>221</v>
-      </c>
-      <c r="F23" t="s">
-        <v>222</v>
-      </c>
-      <c r="G23" t="s">
-        <v>215</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>409</v>
+        <v>342</v>
       </c>
       <c r="B24" t="s">
-        <v>410</v>
+        <v>343</v>
       </c>
       <c r="C24" t="s">
-        <v>223</v>
+        <v>269</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
+        <v>271</v>
       </c>
       <c r="E24" t="s">
-        <v>225</v>
+        <v>218</v>
+      </c>
+      <c r="F24" t="s">
+        <v>272</v>
+      </c>
+      <c r="G24" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -4952,1157 +4566,329 @@
         <v>274</v>
       </c>
       <c r="B25" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="C25" t="s">
-        <v>331</v>
+        <v>373</v>
+      </c>
+      <c r="D25" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>411</v>
+        <v>277</v>
       </c>
       <c r="B26" t="s">
-        <v>412</v>
-      </c>
-      <c r="C26" t="s">
-        <v>226</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>350</v>
+        <v>219</v>
       </c>
       <c r="B27" t="s">
-        <v>351</v>
+        <v>374</v>
       </c>
       <c r="C27" t="s">
-        <v>309</v>
+        <v>220</v>
       </c>
       <c r="D27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E27" t="s">
-        <v>221</v>
+        <v>375</v>
       </c>
       <c r="F27" t="s">
+        <v>376</v>
+      </c>
+      <c r="G27" t="s">
         <v>222</v>
       </c>
-      <c r="G27" t="s">
-        <v>240</v>
-      </c>
       <c r="H27" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="I27" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="J27" t="s">
-        <v>243</v>
+        <v>225</v>
+      </c>
+      <c r="K27" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>306</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>307</v>
+        <v>344</v>
+      </c>
+      <c r="B28" t="s">
+        <v>345</v>
       </c>
       <c r="C28" t="s">
-        <v>320</v>
-      </c>
-      <c r="D28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E28" t="s">
-        <v>193</v>
-      </c>
-      <c r="F28" t="s">
-        <v>240</v>
-      </c>
-      <c r="G28" t="s">
-        <v>241</v>
-      </c>
-      <c r="H28" t="s">
-        <v>242</v>
-      </c>
-      <c r="I28" t="s">
-        <v>243</v>
-      </c>
-      <c r="J28" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>246</v>
-      </c>
-      <c r="B29" t="s">
-        <v>322</v>
-      </c>
-      <c r="C29" t="s">
-        <v>239</v>
-      </c>
-      <c r="D29" t="s">
-        <v>301</v>
-      </c>
-      <c r="E29" t="s">
-        <v>302</v>
-      </c>
-      <c r="F29" t="s">
-        <v>236</v>
-      </c>
-      <c r="G29" t="s">
-        <v>303</v>
-      </c>
-      <c r="H29" t="s">
-        <v>237</v>
-      </c>
-      <c r="I29" t="s">
-        <v>238</v>
-      </c>
-      <c r="J29" t="s">
-        <v>67</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>413</v>
-      </c>
-      <c r="B30" t="s">
-        <v>414</v>
-      </c>
-      <c r="C30" t="s">
-        <v>415</v>
-      </c>
-      <c r="D30" t="s">
-        <v>280</v>
-      </c>
-      <c r="E30" t="s">
-        <v>244</v>
-      </c>
-      <c r="F30" t="s">
-        <v>245</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>370</v>
       </c>
       <c r="C31" t="s">
-        <v>236</v>
+        <v>350</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="E31" t="s">
-        <v>238</v>
-      </c>
-      <c r="F31" t="s">
-        <v>239</v>
-      </c>
-      <c r="G31" t="s">
-        <v>240</v>
-      </c>
-      <c r="H31" t="s">
-        <v>241</v>
-      </c>
-      <c r="I31" t="s">
-        <v>242</v>
-      </c>
-      <c r="J31" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>229</v>
+        <v>347</v>
       </c>
       <c r="B32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>348</v>
+      </c>
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" t="s">
+        <v>349</v>
+      </c>
+      <c r="D33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>301</v>
+      </c>
+      <c r="B35" t="s">
+        <v>302</v>
+      </c>
+      <c r="C35" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>285</v>
+      </c>
+      <c r="B36" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>287</v>
+      </c>
+      <c r="B37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C37" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>290</v>
+      </c>
+      <c r="B38" t="s">
+        <v>217</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B39" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>351</v>
+      </c>
+      <c r="B40" t="s">
         <v>352</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" t="s">
+        <v>238</v>
+      </c>
+      <c r="D43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>240</v>
+      </c>
+      <c r="B44" t="s">
+        <v>241</v>
+      </c>
+      <c r="C44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D44" t="s">
+        <v>243</v>
+      </c>
+      <c r="E44" t="s">
+        <v>244</v>
+      </c>
+      <c r="F44" t="s">
+        <v>245</v>
+      </c>
+      <c r="G44" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>292</v>
+      </c>
+      <c r="B45" t="s">
+        <v>293</v>
+      </c>
+      <c r="C45" t="s">
+        <v>252</v>
+      </c>
+      <c r="D45" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>295</v>
+      </c>
+      <c r="B46" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>283</v>
-      </c>
-      <c r="B33" t="s">
-        <v>273</v>
-      </c>
-      <c r="C33" t="s">
-        <v>327</v>
-      </c>
-      <c r="D33" t="s">
-        <v>328</v>
-      </c>
-      <c r="E33" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>416</v>
-      </c>
-      <c r="B34" t="s">
-        <v>330</v>
-      </c>
-      <c r="C34" t="s">
-        <v>331</v>
-      </c>
-      <c r="D34" t="s">
-        <v>222</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="C46" t="s">
+        <v>227</v>
+      </c>
+      <c r="D46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>353</v>
+      </c>
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>296</v>
+      </c>
+      <c r="B48" t="s">
+        <v>218</v>
+      </c>
+      <c r="C48" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>355</v>
+      </c>
+      <c r="B49" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>247</v>
+      </c>
+      <c r="B50" t="s">
+        <v>377</v>
+      </c>
+      <c r="C50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" t="s">
         <v>248</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F50" t="s">
         <v>249</v>
       </c>
-      <c r="G34" t="s">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>356</v>
+      </c>
+      <c r="B51" t="s">
+        <v>357</v>
+      </c>
+      <c r="C51" t="s">
+        <v>379</v>
+      </c>
+      <c r="D51" t="s">
         <v>250</v>
       </c>
-      <c r="H34" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>417</v>
-      </c>
-      <c r="B35" t="s">
-        <v>215</v>
-      </c>
-      <c r="C35" t="s">
-        <v>366</v>
-      </c>
-      <c r="D35" t="s">
-        <v>173</v>
-      </c>
-      <c r="E35" t="s">
-        <v>367</v>
-      </c>
-      <c r="F35" t="s">
-        <v>250</v>
-      </c>
-      <c r="G35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>418</v>
-      </c>
-      <c r="B36" t="s">
-        <v>419</v>
-      </c>
-      <c r="C36" t="s">
-        <v>310</v>
-      </c>
-      <c r="D36" t="s">
-        <v>248</v>
-      </c>
-      <c r="E36" t="s">
-        <v>249</v>
-      </c>
-      <c r="F36" t="s">
-        <v>250</v>
-      </c>
-      <c r="G36" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>420</v>
-      </c>
-      <c r="B37" t="s">
-        <v>421</v>
-      </c>
-      <c r="C37" t="s">
-        <v>422</v>
-      </c>
-      <c r="D37" t="s">
-        <v>336</v>
-      </c>
-      <c r="E37" t="s">
-        <v>208</v>
-      </c>
-      <c r="F37" t="s">
-        <v>250</v>
-      </c>
-      <c r="G37" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>311</v>
-      </c>
-      <c r="B38" t="s">
-        <v>338</v>
-      </c>
-      <c r="C38" t="s">
-        <v>310</v>
-      </c>
-      <c r="D38" t="s">
-        <v>248</v>
-      </c>
-      <c r="E38" t="s">
-        <v>249</v>
-      </c>
-      <c r="F38" t="s">
-        <v>250</v>
-      </c>
-      <c r="G38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>230</v>
-      </c>
-      <c r="B39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" t="s">
-        <v>231</v>
-      </c>
-      <c r="D39" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>314</v>
-      </c>
-      <c r="B40" t="s">
-        <v>112</v>
-      </c>
-      <c r="C40" t="s">
-        <v>207</v>
-      </c>
-      <c r="D40" t="s">
-        <v>341</v>
-      </c>
-      <c r="E40" t="s">
-        <v>263</v>
-      </c>
-      <c r="F40" t="s">
-        <v>264</v>
-      </c>
-      <c r="G40" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>423</v>
-      </c>
-      <c r="B41" t="s">
-        <v>424</v>
-      </c>
-      <c r="C41" t="s">
-        <v>312</v>
-      </c>
-      <c r="D41" t="s">
-        <v>315</v>
-      </c>
-      <c r="E41" t="s">
-        <v>233</v>
-      </c>
-      <c r="F41" t="s">
-        <v>316</v>
-      </c>
-      <c r="G41" t="s">
-        <v>317</v>
-      </c>
-      <c r="H41" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>425</v>
-      </c>
-      <c r="B42" t="s">
-        <v>282</v>
-      </c>
-      <c r="C42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D42" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>318</v>
-      </c>
-      <c r="B43" t="s">
-        <v>319</v>
-      </c>
-      <c r="C43" t="s">
-        <v>320</v>
-      </c>
-      <c r="D43" t="s">
-        <v>315</v>
-      </c>
-      <c r="E43" t="s">
-        <v>233</v>
-      </c>
-      <c r="F43" t="s">
-        <v>316</v>
-      </c>
-      <c r="G43" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>321</v>
-      </c>
-      <c r="B44" t="s">
-        <v>322</v>
-      </c>
-      <c r="C44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" t="s">
-        <v>262</v>
-      </c>
-      <c r="E44" t="s">
-        <v>263</v>
-      </c>
-      <c r="F44" t="s">
-        <v>264</v>
-      </c>
-      <c r="G44" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>426</v>
-      </c>
-      <c r="B45" t="s">
-        <v>231</v>
-      </c>
-      <c r="C45" t="s">
-        <v>192</v>
-      </c>
-      <c r="D45" t="s">
-        <v>196</v>
-      </c>
-      <c r="E45" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>234</v>
-      </c>
-      <c r="B46" t="s">
-        <v>235</v>
-      </c>
-      <c r="C46" t="s">
-        <v>236</v>
-      </c>
-      <c r="D46" t="s">
-        <v>237</v>
-      </c>
-      <c r="E46" t="s">
-        <v>238</v>
-      </c>
-      <c r="F46" t="s">
-        <v>239</v>
-      </c>
-      <c r="G46" t="s">
-        <v>240</v>
-      </c>
-      <c r="H46" t="s">
-        <v>300</v>
-      </c>
-      <c r="I46" t="s">
-        <v>241</v>
-      </c>
-      <c r="J46" t="s">
-        <v>242</v>
-      </c>
-      <c r="K46" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>427</v>
-      </c>
-      <c r="B47" t="s">
-        <v>428</v>
-      </c>
-      <c r="C47" t="s">
-        <v>323</v>
-      </c>
-      <c r="D47" t="s">
-        <v>196</v>
-      </c>
-      <c r="E47" t="s">
-        <v>193</v>
-      </c>
-      <c r="F47" t="s">
-        <v>264</v>
-      </c>
-      <c r="G47" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>324</v>
-      </c>
-      <c r="B48" t="s">
-        <v>236</v>
-      </c>
-      <c r="C48" t="s">
-        <v>237</v>
-      </c>
-      <c r="D48" t="s">
-        <v>238</v>
-      </c>
-      <c r="E48" t="s">
-        <v>239</v>
-      </c>
-      <c r="F48" t="s">
-        <v>240</v>
-      </c>
-      <c r="G48" t="s">
-        <v>241</v>
-      </c>
-      <c r="H48" t="s">
-        <v>242</v>
-      </c>
-      <c r="I48" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>429</v>
-      </c>
-      <c r="B49" t="s">
-        <v>256</v>
-      </c>
-      <c r="C49" t="s">
-        <v>257</v>
-      </c>
-      <c r="D49" t="s">
-        <v>258</v>
-      </c>
-      <c r="E49" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>325</v>
-      </c>
-      <c r="B50" t="s">
-        <v>326</v>
-      </c>
-      <c r="C50" t="s">
-        <v>327</v>
-      </c>
-      <c r="D50" t="s">
-        <v>328</v>
-      </c>
-      <c r="E50" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>430</v>
-      </c>
-      <c r="B51" t="s">
-        <v>260</v>
-      </c>
-      <c r="C51" t="s">
-        <v>261</v>
-      </c>
-      <c r="D51" t="s">
-        <v>262</v>
-      </c>
       <c r="E51" t="s">
-        <v>263</v>
-      </c>
-      <c r="F51" t="s">
-        <v>264</v>
-      </c>
-      <c r="G51" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>329</v>
-      </c>
-      <c r="B52" t="s">
-        <v>434</v>
-      </c>
-      <c r="C52" t="s">
-        <v>330</v>
-      </c>
-      <c r="D52" t="s">
-        <v>331</v>
-      </c>
-      <c r="E52" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>431</v>
-      </c>
-      <c r="B53" t="s">
-        <v>207</v>
-      </c>
-      <c r="C53" t="s">
-        <v>208</v>
-      </c>
-      <c r="D53" t="s">
-        <v>278</v>
-      </c>
-      <c r="E53" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>432</v>
-      </c>
-      <c r="B54" t="s">
-        <v>219</v>
-      </c>
-      <c r="C54" t="s">
-        <v>433</v>
-      </c>
-      <c r="D54" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>435</v>
-      </c>
-      <c r="B55" t="s">
-        <v>233</v>
-      </c>
-      <c r="C55" t="s">
-        <v>436</v>
-      </c>
-      <c r="D55" t="s">
-        <v>332</v>
-      </c>
-      <c r="E55" t="s">
-        <v>333</v>
-      </c>
-      <c r="F55" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>334</v>
-      </c>
-      <c r="B56" t="s">
-        <v>233</v>
-      </c>
-      <c r="C56" t="s">
-        <v>436</v>
-      </c>
-      <c r="D56" t="s">
-        <v>332</v>
-      </c>
-      <c r="E56" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>372</v>
-      </c>
-      <c r="B57" t="s">
-        <v>373</v>
-      </c>
-      <c r="C57" t="s">
-        <v>308</v>
-      </c>
-      <c r="D57" t="s">
-        <v>309</v>
-      </c>
-      <c r="E57" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>337</v>
-      </c>
-      <c r="B58" t="s">
-        <v>338</v>
-      </c>
-      <c r="C58" t="s">
-        <v>268</v>
-      </c>
-      <c r="D58" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>339</v>
-      </c>
-      <c r="B59" t="s">
-        <v>340</v>
-      </c>
-      <c r="C59" t="s">
-        <v>207</v>
-      </c>
-      <c r="D59" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>345</v>
-      </c>
-      <c r="B60" t="s">
-        <v>281</v>
-      </c>
-      <c r="C60" t="s">
-        <v>366</v>
-      </c>
-      <c r="D60" t="s">
-        <v>173</v>
-      </c>
-      <c r="E60" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>232</v>
-      </c>
-      <c r="B61" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" t="s">
-        <v>207</v>
-      </c>
-      <c r="D61" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>284</v>
-      </c>
-      <c r="B62" t="s">
-        <v>281</v>
-      </c>
-      <c r="C62" t="s">
-        <v>335</v>
-      </c>
-      <c r="D62" t="s">
-        <v>336</v>
-      </c>
-      <c r="E62" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>346</v>
-      </c>
-      <c r="B63" t="s">
-        <v>231</v>
-      </c>
-      <c r="C63" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>347</v>
-      </c>
-      <c r="B64" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
         <v>251</v>
-      </c>
-      <c r="B65" t="s">
-        <v>231</v>
-      </c>
-      <c r="C65" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>348</v>
-      </c>
-      <c r="B66" t="s">
-        <v>340</v>
-      </c>
-      <c r="C66" t="s">
-        <v>207</v>
-      </c>
-      <c r="D66" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>252</v>
-      </c>
-      <c r="B67" t="s">
-        <v>253</v>
-      </c>
-      <c r="C67" t="s">
-        <v>342</v>
-      </c>
-      <c r="D67" t="s">
-        <v>343</v>
-      </c>
-      <c r="E67" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>437</v>
-      </c>
-      <c r="B68" t="s">
-        <v>438</v>
-      </c>
-      <c r="C68" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>349</v>
-      </c>
-      <c r="B69" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>439</v>
-      </c>
-      <c r="B70" t="s">
-        <v>438</v>
-      </c>
-      <c r="C70" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>255</v>
-      </c>
-      <c r="B72" t="s">
-        <v>256</v>
-      </c>
-      <c r="C72" t="s">
-        <v>257</v>
-      </c>
-      <c r="D72" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>259</v>
-      </c>
-      <c r="B73" t="s">
-        <v>260</v>
-      </c>
-      <c r="C73" t="s">
-        <v>261</v>
-      </c>
-      <c r="D73" t="s">
-        <v>262</v>
-      </c>
-      <c r="E73" t="s">
-        <v>263</v>
-      </c>
-      <c r="F73" t="s">
-        <v>264</v>
-      </c>
-      <c r="G73" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>353</v>
-      </c>
-      <c r="B74" t="s">
-        <v>354</v>
-      </c>
-      <c r="C74" t="s">
-        <v>279</v>
-      </c>
-      <c r="D74" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>356</v>
-      </c>
-      <c r="B75" t="s">
-        <v>256</v>
-      </c>
-      <c r="C75" t="s">
-        <v>257</v>
-      </c>
-      <c r="D75" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>199</v>
-      </c>
-      <c r="B76" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>440</v>
-      </c>
-      <c r="B77" t="s">
-        <v>118</v>
-      </c>
-      <c r="C77" t="s">
-        <v>441</v>
-      </c>
-      <c r="D77" t="s">
-        <v>262</v>
-      </c>
-      <c r="E77" t="s">
-        <v>263</v>
-      </c>
-      <c r="F77" t="s">
-        <v>264</v>
-      </c>
-      <c r="G77" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>357</v>
-      </c>
-      <c r="B78" t="s">
-        <v>233</v>
-      </c>
-      <c r="C78" t="s">
-        <v>315</v>
-      </c>
-      <c r="D78" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>358</v>
-      </c>
-      <c r="B79" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>442</v>
-      </c>
-      <c r="B80" t="s">
-        <v>256</v>
-      </c>
-      <c r="C80" t="s">
-        <v>257</v>
-      </c>
-      <c r="D80" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>270</v>
-      </c>
-      <c r="B81" t="s">
-        <v>262</v>
-      </c>
-      <c r="C81" t="s">
-        <v>263</v>
-      </c>
-      <c r="D81" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>364</v>
-      </c>
-      <c r="B82" t="s">
-        <v>365</v>
-      </c>
-      <c r="C82" t="s">
-        <v>366</v>
-      </c>
-      <c r="D82" t="s">
-        <v>173</v>
-      </c>
-      <c r="E82" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>443</v>
-      </c>
-      <c r="B83" t="s">
-        <v>444</v>
-      </c>
-      <c r="C83" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>442</v>
-      </c>
-      <c r="B84" t="s">
-        <v>354</v>
-      </c>
-      <c r="C84" t="s">
-        <v>279</v>
-      </c>
-      <c r="D84" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>270</v>
-      </c>
-      <c r="B85" t="s">
-        <v>262</v>
-      </c>
-      <c r="C85" t="s">
-        <v>263</v>
-      </c>
-      <c r="D85" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>364</v>
-      </c>
-      <c r="B86" t="s">
-        <v>365</v>
-      </c>
-      <c r="C86" t="s">
-        <v>366</v>
-      </c>
-      <c r="D86" t="s">
-        <v>173</v>
-      </c>
-      <c r="E86" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>443</v>
-      </c>
-      <c r="B87" t="s">
-        <v>444</v>
-      </c>
-      <c r="C87" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>359</v>
-      </c>
-      <c r="B88" t="s">
-        <v>340</v>
-      </c>
-      <c r="C88" t="s">
-        <v>360</v>
-      </c>
-      <c r="D88" t="s">
-        <v>361</v>
-      </c>
-      <c r="E88" t="s">
-        <v>362</v>
-      </c>
-      <c r="F88" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>364</v>
-      </c>
-      <c r="B89" t="s">
-        <v>365</v>
-      </c>
-      <c r="C89" t="s">
-        <v>366</v>
-      </c>
-      <c r="D89" t="s">
-        <v>173</v>
-      </c>
-      <c r="E89" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>275</v>
-      </c>
-      <c r="B90" t="s">
-        <v>276</v>
-      </c>
-      <c r="C90" t="s">
-        <v>277</v>
-      </c>
-      <c r="D90" t="s">
-        <v>278</v>
-      </c>
-      <c r="E90" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6126,10 +4912,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6287,7 +5073,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" t="s">
         <v>118</v>
@@ -6317,32 +5103,32 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>368</v>
+        <v>297</v>
       </c>
       <c r="B2" t="s">
-        <v>374</v>
+        <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" s="10">
+        <v>165</v>
+      </c>
+      <c r="D2" s="9">
         <v>637.32000000000005</v>
       </c>
       <c r="E2">
@@ -6357,15 +5143,15 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>369</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s">
-        <v>374</v>
+        <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" s="10">
+        <v>163</v>
+      </c>
+      <c r="D3" s="9">
         <v>699.12</v>
       </c>
       <c r="E3">
@@ -6380,15 +5166,15 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>375</v>
+        <v>304</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="10">
+        <v>163</v>
+      </c>
+      <c r="D4" s="9">
         <v>717.35416666699996</v>
       </c>
       <c r="E4">
@@ -6403,15 +5189,15 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>375</v>
+        <v>304</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="10">
+        <v>166</v>
+      </c>
+      <c r="D5" s="9">
         <v>593.9</v>
       </c>
       <c r="E5">
@@ -6426,15 +5212,15 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>302</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" s="10">
+        <v>164</v>
+      </c>
+      <c r="D6" s="9">
         <v>793.3125</v>
       </c>
       <c r="E6">
@@ -6449,15 +5235,15 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>377</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D7" s="10">
+        <v>165</v>
+      </c>
+      <c r="D7" s="9">
         <v>832.125</v>
       </c>
       <c r="E7">
@@ -6472,15 +5258,15 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="10">
+        <v>166</v>
+      </c>
+      <c r="D8" s="9">
         <v>824.72500000000002</v>
       </c>
       <c r="E8">
@@ -6495,15 +5281,15 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>309</v>
       </c>
       <c r="B9" t="s">
-        <v>381</v>
+        <v>310</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="10">
+        <v>167</v>
+      </c>
+      <c r="D9" s="9">
         <v>-569.35913249999999</v>
       </c>
       <c r="E9">
@@ -6518,15 +5304,15 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>382</v>
+        <v>311</v>
       </c>
       <c r="B10" t="s">
-        <v>378</v>
+        <v>307</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="10">
+        <v>164</v>
+      </c>
+      <c r="D10" s="9">
         <v>409.64</v>
       </c>
       <c r="E10">
@@ -6540,7 +5326,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <f>SUM(D2:D10)</f>
         <v>4938.1375341670009</v>
       </c>
@@ -6590,7 +5376,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>384</v>
+        <v>313</v>
       </c>
       <c r="B2">
         <v>3403.3</v>
@@ -6604,7 +5390,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>385</v>
+        <v>314</v>
       </c>
       <c r="B3">
         <v>1913.05</v>
@@ -6618,7 +5404,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>386</v>
+        <v>315</v>
       </c>
       <c r="B4">
         <v>1943.25</v>
@@ -6632,7 +5418,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>386</v>
+        <v>315</v>
       </c>
       <c r="B5">
         <v>1733.4</v>

</xml_diff>

<commit_message>
Updated best contest to take game start parameter, simplified to report all contest under limit sort smallest avg wins to largest
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$H$22</definedName>
     <definedName name="cLastDataDate">Parameters!#REF!</definedName>
     <definedName name="clEntryLimit">Parameters!$B$5</definedName>
     <definedName name="cLineUpURL">Parameters!$B$2</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="371">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -599,18 +596,6 @@
     <t>Place</t>
   </si>
   <si>
-    <t>S116326603</t>
-  </si>
-  <si>
-    <t>S116301544</t>
-  </si>
-  <si>
-    <t>S116301404</t>
-  </si>
-  <si>
-    <t>S116301270</t>
-  </si>
-  <si>
     <t>Matt Calvert</t>
   </si>
   <si>
@@ -629,48 +614,21 @@
     <t>Pascal Dupuis</t>
   </si>
   <si>
-    <t>Patrick Dwyer</t>
-  </si>
-  <si>
-    <t>Patrick Wiercioch</t>
-  </si>
-  <si>
     <t>Patrick Marleau</t>
   </si>
   <si>
-    <t>Philipp Grubauer</t>
-  </si>
-  <si>
-    <t>Philip Varone</t>
-  </si>
-  <si>
-    <t>Philip Samuelsson</t>
-  </si>
-  <si>
-    <t>Filip Forsberg</t>
-  </si>
-  <si>
     <t>Andrei Markov</t>
   </si>
   <si>
     <t>Andrew Cogliano</t>
   </si>
   <si>
-    <t>Dmitry Orlov</t>
-  </si>
-  <si>
-    <t>Dmitry Kulikov</t>
-  </si>
-  <si>
     <t>Jacob Markstrom</t>
   </si>
   <si>
     <t>Chad Johnson</t>
   </si>
   <si>
-    <t>Patric Hornqvist</t>
-  </si>
-  <si>
     <t>Nathan Gerbe</t>
   </si>
   <si>
@@ -683,27 +641,12 @@
     <t>Jonathan Ericsson</t>
   </si>
   <si>
-    <t>Carl Soderberg</t>
-  </si>
-  <si>
-    <t>Karl Alzner</t>
-  </si>
-  <si>
-    <t>Carl Hagelin</t>
-  </si>
-  <si>
-    <t>Matthew Lombardi</t>
-  </si>
-  <si>
     <t>Matt Dumba</t>
   </si>
   <si>
     <t>Brian Elliott</t>
   </si>
   <si>
-    <t>Chris Conner</t>
-  </si>
-  <si>
     <t>Chris Terry</t>
   </si>
   <si>
@@ -722,12 +665,6 @@
     <t>Charlie Coyle</t>
   </si>
   <si>
-    <t>Chris Thorburn</t>
-  </si>
-  <si>
-    <t>Erik Condra</t>
-  </si>
-  <si>
     <t>Chris Kelly</t>
   </si>
   <si>
@@ -743,33 +680,15 @@
     <t>Colin Wilson</t>
   </si>
   <si>
-    <t>Calvin de Haan</t>
-  </si>
-  <si>
     <t>Calvin de_Haan</t>
   </si>
   <si>
-    <t>Harry Zolnierczyk</t>
-  </si>
-  <si>
-    <t>Steven Oleksy</t>
-  </si>
-  <si>
-    <t>Steven Stamkos</t>
-  </si>
-  <si>
     <t>Steve Ott</t>
   </si>
   <si>
     <t>Stephen Weiss</t>
   </si>
   <si>
-    <t>Tomas Kaberle</t>
-  </si>
-  <si>
-    <t>Tomas Hertl</t>
-  </si>
-  <si>
     <t>Tomas Tatar</t>
   </si>
   <si>
@@ -800,198 +719,39 @@
     <t>Keith Aulie</t>
   </si>
   <si>
-    <t>Jason Demers</t>
-  </si>
-  <si>
     <t>Kris Letang</t>
   </si>
   <si>
-    <t>S119446122</t>
-  </si>
-  <si>
-    <t>S119468134</t>
-  </si>
-  <si>
-    <t>S119440314</t>
-  </si>
-  <si>
-    <t>Richard Bachman</t>
-  </si>
-  <si>
-    <t>Richard Panik</t>
-  </si>
-  <si>
     <t>Tye McGinn</t>
   </si>
   <si>
-    <t>Jonas Gustavsson</t>
-  </si>
-  <si>
-    <t>Mike McKenna</t>
-  </si>
-  <si>
-    <t>Mike Green</t>
-  </si>
-  <si>
-    <t>Luke Schenn</t>
-  </si>
-  <si>
     <t>Chris Neil</t>
   </si>
   <si>
     <t>Chris Kunitz</t>
   </si>
   <si>
-    <t>Joey MacDonald</t>
-  </si>
-  <si>
-    <t>Andrew MacDonald</t>
-  </si>
-  <si>
-    <t>Andrei Vasilevskii</t>
-  </si>
-  <si>
     <t>Matt Ellis</t>
   </si>
   <si>
-    <t>Maxime Fortunus</t>
-  </si>
-  <si>
-    <t>Sean Collins</t>
-  </si>
-  <si>
-    <t>Dylan Olsen</t>
-  </si>
-  <si>
-    <t>Dan Hamhuis</t>
-  </si>
-  <si>
-    <t>Jack Campbell</t>
-  </si>
-  <si>
-    <t>Brian Campbell</t>
-  </si>
-  <si>
-    <t>Gregory Campbell</t>
-  </si>
-  <si>
-    <t>Andy Miele</t>
-  </si>
-  <si>
-    <t>Andy Greene</t>
-  </si>
-  <si>
-    <t>Brad Boyes</t>
-  </si>
-  <si>
-    <t>Rich Peverley</t>
-  </si>
-  <si>
-    <t>Josh Harding</t>
-  </si>
-  <si>
     <t>Josh Gorges</t>
   </si>
   <si>
     <t>Josh Bailey</t>
   </si>
   <si>
-    <t>Kristers Gudlevskis</t>
-  </si>
-  <si>
-    <t>Oliver Lauridsen</t>
-  </si>
-  <si>
-    <t>Oliver Ekman-Larsson</t>
-  </si>
-  <si>
-    <t>Alexei Marchenko</t>
-  </si>
-  <si>
-    <t>Alex Galchenyuk</t>
-  </si>
-  <si>
     <t>Alexei Emelin</t>
   </si>
   <si>
-    <t>Mathew Dumba</t>
-  </si>
-  <si>
-    <t>Quinton Howden</t>
-  </si>
-  <si>
-    <t>Jason Williams</t>
-  </si>
-  <si>
-    <t>Justin Williams</t>
-  </si>
-  <si>
-    <t>Jason Pominville</t>
-  </si>
-  <si>
-    <t>Allan York</t>
-  </si>
-  <si>
     <t>Stefan Elliott</t>
   </si>
   <si>
     <t>Ryan Callahan</t>
   </si>
   <si>
-    <t>Valtteri Filppula</t>
-  </si>
-  <si>
-    <t>S120331303</t>
-  </si>
-  <si>
-    <t>Mike Weaver</t>
-  </si>
-  <si>
-    <t>Thomas McCollum</t>
-  </si>
-  <si>
-    <t>Tom McCollum</t>
-  </si>
-  <si>
-    <t>['TBL', 'TBL', 'TBL', 'TBL', 'TBL']</t>
-  </si>
-  <si>
-    <t>['MTL', 'MTL', 'MTL', 'MTL']</t>
-  </si>
-  <si>
-    <t>['PIT', 'PIT', 'PIT', 'PIT']</t>
-  </si>
-  <si>
     <t>David Perron</t>
   </si>
   <si>
-    <t>['DET', 'DET', 'DET', 'DET', 'DET']</t>
-  </si>
-  <si>
-    <t>{u'MIN': [['Zach Parise', 'Mikko Koivu', 'Jason Pominville'], ['Jason Zucker', 'Erik Haula', 'Thomas Vanek'], ['Ryan Carter', 'Charlie Coyle', 'Nino Niederreiter'], ['Matt Cooke', 'Kyle Brodziak', 'Justin Fontaine'], ['Ryan Suter', 'Jonas Brodin'], ['Jared Spurgeon', 'Mathew Dumba'], ['Marco Scandella', 'Christian Folin'], ['Zach Parise', 'Mikko Koivu', 'Thomas Vanek', 'Ryan Suter', 'Jason Pominville'], ['Jason Zucker', 'Charlie Coyle', 'Nino Niederreiter', 'Jared Spurgeon', 'Jonas Brodin']], u'TOR': [['James van Riemsdyk', 'Nazem Kadri', 'Phil Kessel'], ['Daniel Winnik', 'Tyler Bozak', 'David Clarkson'], ['Richard Panik', 'Mike Santorelli', 'Josh Leivo'], ['David Booth', 'Trevor Smith', 'Matt Frattin'], ['Dion Phaneuf', 'Cody Franson'], ['Morgan Rielly', 'Roman Polak'], ['Jake Gardiner', 'Korbinian Holzer'], ['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel', 'Dion Phaneuf', 'Cody Franson'], ['Richard Panik', 'Nazem Kadri', 'David Clarkson', 'Jake Gardiner', 'Morgan Rielly']], u'CAR': [['Eric Staal', 'Jordan Staal', 'Jiri Tlusty'], ['Jeff Skinner', 'Victor Rask', 'Elias Lindholm'], ['Nathan Gerbe', 'Riley Nash', 'Chris Terry'], ['Brad Malone', 'Jay McClement', 'Pat Dwyer'], ['Andrej Sekera', 'Justin Faulk'], ['Tim Gleason', 'John-Michael Liles'], ['Ron Hainsey', 'Brett Bellemore'], ['Eric Staal', 'Jordan Staal', 'Jiri Tlusty', 'Andrej Sekera', 'John-Michael Liles'], ['Jeff Skinner', 'Riley Nash', 'Victor Rask', 'Elias Lindholm', 'Justin Faulk']], u'BOS': [['Milan Lucic', 'David Krejci', 'David Pastrnak'], ['Daniel Paille', 'Patrice Bergeron', 'Reilly Smith'], ['Chris Kelly', 'Carl Soderberg', 'Loui Eriksson'], ['Jordan Caron', 'Gregory Campbell', 'Craig Cunningham'], ['Zdeno Chara', 'Dougie Hamilton'], ['Dennis Seidenberg', 'Adam McQuaid'], ['Torey Krug', 'Kevan Miller'], ['Loui Eriksson', 'Patrice Bergeron', 'Reilly Smith', 'Carl Soderberg', 'Dougie Hamilton'], ['Milan Lucic', 'David Krejci', 'David Pastrnak', 'Zdeno Chara', 'Torey Krug']], u'DET': [['Gustav Nyquist', 'Henrik Zetterberg', 'Justin Abdelkader'], ['Tomas Tatar', 'Pavel Datsyuk', 'Darren Helm'], ['Luke Glendening', 'Riley Sheahan', 'Drew Miller'], ['Stephen Weiss', 'Joakim Andersson', 'Teemu Pulkkinen'], ['Jonathan Ericsson', 'Niklas Kronwall'], ['Kyle Quincey', 'Dan DeKeyser'], ['Brendan Smith', 'Xavier Ouellet'], ['Gustav Nyquist', 'Henrik Zetterberg', 'Justin Abdelkader', 'Teemu Pulkkinen', 'Niklas Kronwall'], ['Tomas Tatar', 'Pavel Datsyuk', 'Riley Sheahan', 'Stephen Weiss', 'Dan DeKeyser']], u'NAS': [['Filip Forsberg', 'Mike Ribeiro', 'Craig Smith'], ['Colin Wilson', 'Mike Fisher', 'James Neal'], ['Gabriel Bourque', 'Calle Jarnkrok', 'Matt Cullen'], ['Eric Nystrom', 'Paul Gaustad', 'Olli Jokinen'], ['Roman Josi', 'Shea Weber'], ['Victor Bartley', 'Seth Jones'], ['Mattias Ekholm', 'Anthony Bitetto'], ['Filip Forsberg', 'Mike Fisher', 'James Neal', 'Roman Josi', 'Shea Weber'], ['Colin Wilson', 'Mike Ribeiro', 'Craig Smith', 'Seth Jones', 'Mattias Ekholm']], u'NYI': [['Josh Bailey', 'John Tavares', 'Kyle Okposo'], ['Anders Lee', 'Frans Nielsen', 'Ryan Strome'], ['Michael Grabner', 'Brock Nelson', 'Nikolay Kulemin'], ['Matt Martin', 'Casey Cizikas', 'Cal Clutterbuck'], ['Calvin de Haan', 'Travis Hamonic'], ['Nick Leddy', 'Johnny Boychuk'], ['Thomas Hickey', 'Brian Strait'], ['Brock Nelson', 'John Tavares', 'Kyle Okposo', 'Frans Nielsen', 'Johnny Boychuk'], ['Anders Lee', 'Ryan Strome', 'Josh Bailey', 'Nick Leddy', 'Travis Hamonic']], u'FLA': [['Jonathan Huberdeau', 'Aleksander Barkov', 'Brad Boyes'], ['Jimmy Hayes', 'Nick Bjugstad', 'Brandon Pirri'], ['Jussi Jokinen', 'Dave Bolland', 'Tomas Fleischmann'], ['Tomas Kopecky', 'Derek MacKenzie', 'Scottie Upshall'], ['Brian Campbell', 'Aaron Ekblad'], ['Willie Mitchell', 'Dmitry Kulikov'], ['Erik Gudbranson', 'Dylan Olsen'], ['Jonathan Huberdeau', 'Nick Bjugstad', 'Aleksander Barkov', 'Brian Campbell', 'Aaron Ekblad'], ['Tomas Fleischmann', 'Dave Bolland', 'Jussi Jokinen', 'Dylan Olsen', 'Dmitry Kulikov']], u'COL': [['Gabriel Landeskog', "Ryan O'Reilly", 'Nathan Mackinnon'], ['Alex Tanguay', 'Matt Duchene', 'Jarome Iginla'], ['Dennis Everberg', 'John Mitchell', 'Cody McLeod'], ['Marc-Andre Cliche', 'Max Talbot', 'Danny Briere'], ['Jan Hejda', 'Erik Johnson'], ['Nate Guenin', 'Tyson Barrie'], ['Brad Stuart', 'Nick Holden'], ['Gabriel Landeskog', 'Matt Duchene', 'Nathan Mackinnon', 'Jarome Iginla', 'Erik Johnson'], ['Alex Tanguay', "Ryan O'Reilly", 'Cody McLeod', 'Nick Holden', 'Tyson Barrie']], u'NJD': [['Adam Henrique', 'Scott Gomez', 'Steve Bernier'], ['Patrik Elias', 'Travis Zajac', 'Martin Havlat'], ['Dainius Zubrus', 'Michael Cammalleri', 'Michael Ryder'], ['Joe Whitney', 'Tim Sestito', 'Jordin Tootoo'], ['Andy Greene', 'Adam Larsson'], ['Mark Fraser', 'Marek Zidlicky'], ['Jon Merrill', ''], ['Michael Ryder', 'Travis Zajac', 'Martin Havlat', 'Patrik Elias', 'Marek Zidlicky'], ['Adam Henrique', 'Scott Gomez', 'Michael Cammalleri', 'Jon Merrill', 'Eric Gelinas']], u'DAL': [['Jamie Benn', 'Tyler Seguin', 'Colton Sceviour'], ['Erik Cole', 'Jason Spezza', 'Ales Hemsky'], ['Antoine Roussel', 'Cody Eakin', 'Ryan Garbutt'], ['Shawn Horcoff', 'Vernon Fiddler', 'Travis Moen'], ['Alex Goligoski', 'John Klingberg'], ['Jordie Benn', 'Jason Demers'], ['Jyrki Jokipakka', 'Jamie Oleksiak'], ['Jamie Benn', 'Tyler Seguin', 'Cody Eakin', 'John Klingberg', 'Jason Spezza'], ['Erik Cole', 'Shawn Horcoff', 'Ales Hemsky', 'Alex Goligoski', 'Jason Demers']], u'CGY': [['Johnny Gaudreau', 'Mikael Backlund', 'Jiri Hudler'], ['Lance Bouma', 'Sean Monahan', 'David Jones'], ['Mason Raymond', 'Markus Granlund', 'Joe Colborne'], ['Brandon Bollig', 'Matt Stajan', 'Paul Byron'], ['Mark Giordano', 'T.J. Brodie'], ['Kris Russell', 'Dennis Wideman'], ['Ladislav Smid', 'Deryk Engelland'], ['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler', 'T.J. Brodie', 'Mark Giordano'], ['Mason Raymond', 'Mikael Backlund', 'Joe Colborne', 'Kris Russell', 'Dennis Wideman']], u'NYR': [['Rick Nash', 'Derick Brassard', 'Mats Zuccarello'], ['Chris Kreider', 'Derek Stepan', 'Martin St. Louis'], ['Carl Hagelin', 'Kevin Hayes', 'Jesper Fast'], ['J.T. Miller', 'Dominic Moore', 'Lee Stempniak'], ['Ryan McDonagh', 'Dan Girardi'], ['Marc Staal', 'Dan Boyle'], ['Kevin Klein', 'Matt Hunwick'], ['Rick Nash', 'Derick Brassard', 'Martin St. Louis', 'Derek Stepan', 'Dan Boyle'], ['Chris Kreider', 'J.T. Miller', 'Mats Zuccarello', 'Ryan McDonagh', 'Dan Girardi']], u'SJS': [['Melker Karlsson', 'Joe Thornton', 'Joe Pavelski'], ['Patrick Marleau', 'Logan Couture', 'Tommy Wingels'], ['Matthew Nieto', 'Tomas Hertl', 'Tyler Kennedy'], ['Andrew Desjardins', 'James Sheppard', 'Tye McGinn'], ['Marc-Edouard Vlasic', 'Brent Burns'], ['Brenden Dillon', 'Justin Braun'], ['Matt Irwin', 'Scott Hannan'], ['Patrick Marleau', 'Joe Thornton', 'Logan Couture', 'Joe Pavelski', 'Brent Burns'], ['Melker Karlsson', 'Tomas Hertl', 'Tyler Kennedy', 'Marc-Edouard Vlasic', 'Matt Irwin']], u'PIT': [['Chris Kunitz', 'Sidney Crosby', 'David Perron'], ['Nick Spaling', 'Evgeni Malkin', 'Beau Bennett'], ['Mark Arcobello', 'Brandon Sutter', 'Steve Downie'], ['Bobby Farnham', 'Zach Sill', 'Craig Adams'], ['Paul Martin', 'Kris Letang'], ['Rob Scuderi', 'Christian Ehrhoff'], ['Robert Bortuzzo', 'Simon Despres'], ['Chris Kunitz', 'Sidney Crosby', 'David Perron', 'Evgeni Malkin', 'Kris Letang'], ['Beau Bennett', 'Brandon Sutter', 'Steve Downie', 'Christian Ehrhoff', 'Paul Martin']], u'VAN': [['Daniel Sedin', 'Henrik Sedin', 'Radim Vrbata'], ['Chris Higgins', 'Linden Vey', 'Alexandre Burrows'], ['Shawn Matthias', 'Nick Bonino', 'Zack Kassian'], ['Derek Dorsett', 'Bo Horvat', 'Jannik Hansen'], ['Alexander Edler', 'Chris Tanev'], ['Ryan Stanton', 'Kevin Bieksa'], ['Dan Hamhuis', 'Luca Sbisa'], ['Daniel Sedin', 'Henrik Sedin', 'Radim Vrbata', 'Alexander Edler', 'Alexandre Burrows'], ['Derek Dorsett', 'Nick Bonino', 'Linden Vey', 'Chris Higgins', 'Kevin Bieksa']], u'STL': [['Alex Steen', 'David Backes', 'T.J. Oshie'], ['Patrik Berglund', 'Jori Lehtera', 'Vladimir Tarasenko'], ['Jaden Schwartz', 'Paul Stastny', 'Dmitrij Jaskin'], ['Steve Ott', 'Maxim Lapierre', 'Ryan Reaves'], ['Jay Bouwmeester', 'Alex Pietrangelo'], ['Carl Gunnarsson', 'Kevin Shattenkirk'], ['Barret Jackman', 'Ian Cole'], ['David Backes', 'Paul Stastny', 'T.J. Oshie', 'Alex Steen', 'Kevin Shattenkirk'], ['Jaden Schwartz', 'Jori Lehtera', 'Vladimir Tarasenko', 'Jay Bouwmeester', 'Alex Pietrangelo']], u'CHI': [['Brandon Saad', 'Jonathan Toews', 'Marian Hossa'], ['Bryan Bickell', 'Brad Richards', 'Patrick Kane'], ['Patrick Sharp', 'Teuvo Teravainen', 'Andrew Shaw'], ['Joakim Nordstrom', 'Marcus Kruger', 'Ben Smith'], ['Duncan Keith', 'Brent Seabrook'], ['Niklas Hjalmarsson', 'Johnny Oduya'], ['Michal Rozsival', 'David Rundblad'], ['Andrew Shaw', 'Jonathan Toews', 'Patrick Kane', 'Duncan Keith', 'Brad Richards'], ['Bryan Bickell', 'Brandon Saad', 'Marian Hossa', 'Patrick Sharp', 'Brent Seabrook']], u'MTL': [['Max Pacioretty', 'Tomas Plekanec', 'Dale Weise'], ['Alex Galchenyuk', 'David Desharnais', 'Brendan Gallagher'], ['Jiri Sekac', 'Lars Eller', 'Christian Thomas'], ['Michael Bournival', 'Manny Malhotra', 'Brandon Prust'], ['Andrei Markov', 'P.K. Subban'], ['Nathan Beaulieu', 'Sergei Gonchar'], ['Alexei Emelin', 'Tom Gilbert'], ['Max Pacioretty', 'Tomas Plekanec', 'Brendan Gallagher', 'Andrei Markov', 'P.K. Subban'], ['Jiri Sekac', 'David Desharnais', 'Alex Galchenyuk', 'Nathan Beaulieu', 'Sergei Gonchar']], u'PHI': [['Brayden Schenn', 'Claude Giroux', 'Jakub Voracek'], ['R.J. Umberger', 'Sean Couturier', 'Matt Read'], ['Zac Rinaldo', 'Michael Raffl', 'Wayne Simmonds'], ['Chris VandeVelde', 'Vincent Lecavalier'], ['Mark Streit', 'Andrew MacDonald'], ['Michael Del Zotto', 'Luke Schenn'], ['Brandon Manning', 'Oliver Lauridsen'], ['Brayden Schenn', 'Claude Giroux', 'Wayne Simmonds', 'Jakub Voracek', 'Mark Streit'], ['R.J. Umberger', 'Sean Couturier', 'Vincent Lecavalier', 'Matt Read', 'Michael Del Zotto']], u'ANA': [['Patrick Maroon', 'Ryan Getzlaf', 'Corey Perry'], ['Matt Beleskey', 'Ryan Kesler', 'Kyle Palmieri'], ['Andrew Cogliano', 'Rickard Rakell', 'Jakob Silfverberg'], ['Devante Smith-Pelly', 'Nate Thompson', 'Tim Jackman'], ['Francois Beauchemin', 'Hampus Lindholm'], ['Cam Fowler', 'Ben Lovejoy'], ['Clayton Stoner', 'Sami Vatanen'], ['Patrick Maroon', 'Ryan Getzlaf', 'Corey Perry', 'Cam Fowler', 'Sami Vatanen'], ['Rickard Rakell', 'Ryan Kesler', 'Kyle Palmieri', 'Francois Beauchemin', 'Hampus Lindholm']], u'LAK': [['Marian Gaborik', 'Anze Kopitar', 'Justin Williams'], ['Kyle Clifford', 'Nick Shore', 'Jeff Carter'], ['Dustin Brown', 'Jarret Stoll', 'Trevor Lewis'], ['Dwight King', 'Mike Richards', 'Jordan Nolan'], ['Jake Muzzin', 'Drew Doughty'], ['Brayden McNabb', 'Matt Greene'], ['Robyn Regehr', 'Alec Martinez'], ['Marian Gaborik', 'Anze Kopitar', 'Jeff Carter', 'Jake Muzzin', 'Drew Doughty'], ['Dustin Brown', 'Jarret Stoll', 'Justin Williams', 'Brayden McNabb', 'Alec Martinez']], u'CBJ': [['Nick Foligno', 'Ryan Johansen', 'Jeremy Morin'], ['Scott Hartnell', 'Brandon Dubinsky', 'Josh  Anderson'], ['Matt Calvert', 'Alexander Wennberg', 'Cam Atkinson'], ['Corey Tropp', 'Mark Letestu', 'Jack Skille'], ['Jack Johnson', 'David Savard'], ['Kevin Connauton', 'James Wisniewski'], ['Fedor Tyutin', 'Dalton Prout'], ['Scott Hartnell', 'Ryan Johansen', 'Nick Foligno', 'Jack Johnson', 'James Wisniewski'], ['Alexander Wennberg', 'Brandon Dubinsky', 'Cam Atkinson', 'Kevin Connauton', 'David Savard']], u'BUF': [['Brian Flynn', 'Zemgus  Girgensons', 'Chris Stewart'], ['Matt Moulson', 'Torrey Mitchell', 'Tyler Ennis'], ['Cody Hodgson', 'Phil Varone', 'Drew Stafford'], ['Nicolas Deslauriers', 'Matt Ellis', 'Patrick Kaleta'], ['Tyler Myers', 'Josh Gorges'], ['Nikita Zadorov', 'Tyson Strachan'], ['Andre Benoit', 'Andrej Meszaros'], ['Chris Stewart', 'Zemgus  Girgensons', 'Tyler Ennis', 'Nikita Zadorov', 'Tyler Myers'], ['Matt Moulson', 'Brian Flynn', 'Nicolas Deslauriers', 'Andre Benoit', 'Andrej Meszaros']], u'EDM': [['Taylor Hall', 'Ryan Nugent-Hopkins', 'Jordan Eberle'], ['Benoit Pouliot', 'Derek Roy', 'Nail Yakupov'], ['Matt Fraser', 'Anton Lander', 'Teddy Purcell'], ['Matt Hendricks', 'Boyd Gordon', 'Rob Klinkhammer'], ['Oscar Klefbom', 'Justin Schultz'], ['Andrew Ference', 'Jeff Petry'], ['Nikita Nikitin', 'Mark Fayne'], ['Benoit Pouliot', 'Ryan Nugent-Hopkins', 'Jordan Eberle', 'Taylor Hall', 'Justin Schultz'], ['Nail Yakupov', 'Anton Lander', 'Teddy Purcell', 'Derek Roy', 'Jeff Petry']], u'TBL': [['Valtteri Filppula', 'Steven Stamkos', 'Ryan Callahan'], ['Ondrej Palat', 'Tyler Johnson', 'Nikita Kucherov'], ['Alex Killorn', 'Cedric Paquette', 'Brett Connolly'], ['Brenden Morrow', 'Brian Boyle', 'Jonathan Drouin'], ['Victor Hedman', 'Andrej Sustr'], ['Jason Garrison', 'Anton Stralman'], ['Luke Witkowski', 'Nikita Nesterov'], ['Ondrej Palat', 'Steven Stamkos', 'Nikita Kucherov', 'Tyler Johnson', 'Anton Stralman'], ['Brett Connolly', 'Alex Killorn', 'Ryan Callahan', 'Victor Hedman', 'Valtteri Filppula']], u'WIN': [['Andrew Ladd', 'Bryan Little', 'Blake Wheeler'], ['Evander Kane', 'Mark Scheifele', 'Michael Frolik'], ['Chris Thorburn', 'Adam Lowry', 'Matt Halischuk'], ['T.J. Galiardi', 'Jim Slater', 'Anthony Peluso'], ['Ben Chiarot', 'Dustin Byfuglien'], ['Tobias Enstrom', 'Zach Bogosian'], ['Mark Stuart', 'Jay Harrison'], ['Andrew Ladd', 'Bryan Little', 'Blake Wheeler', 'Tobias Enstrom', 'Dustin Byfuglien'], ['Adam Lowry', 'Mark Scheifele', 'Michael Frolik', 'Evander Kane', 'Zach Bogosian']], u'ARI': [['Tobias Rieder', 'Antoine Vermette', 'Shane Doan'], ['Lauri Korpikoski', 'Martin Hanzal', 'Sam Gagner'], ['Brandon McMillan', 'Kyle Chipchura', 'David Moss'], ['Lucas Lessio', 'Joe Vitale', 'B.J. Crombeen'], ['Oliver Ekman-Larsson', 'Michael Stone'], ['Keith Yandle', 'Connor Murphy'], ['Philip Samuelsson', 'Brandon Gormley'], ['Sam Gagner', 'Antoine Vermette', 'Shane Doan', 'Oliver Ekman-Larsson', 'Keith Yandle'], ['Tobias Rieder', 'Martin Hanzal', 'Lauri Korpikoski', 'Michael Stone', 'Brandon Gormley']], u'OTT': [['Clarke MacArthur', 'Kyle Turris', 'Mark Stone'], ['Mike Hoffman', 'Mika Zibanejad', 'Bobby Ryan'], ['Milan Michalek', 'Jean-Gabriel Pageau', 'Alex Chiasson'], ['Erik Condra', 'David Legwand', 'Chris Neil'], ['Marc Methot', 'Erik Karlsson'], ['Jared Cowen', 'Cody Ceci'], ['Chris Phillips', 'Eric Gryba'], ['Alex Chiasson', 'Mika Zibanejad', 'Bobby Ryan', 'Milan Michalek', 'Erik Karlsson'], ['Clarke MacArthur', 'David Legwand', 'Mark Stone', 'Kyle Turris', 'Cody Ceci']]}</t>
-  </si>
-  <si>
-    <t>Braden Holtby</t>
-  </si>
-  <si>
-    <t>['WSH', 'WSH', 'WSH', 'WSH']</t>
-  </si>
-  <si>
-    <t>Darren Helm</t>
-  </si>
-  <si>
-    <t>https://www.fanduel.com/e/Game/11476?tableId=9922292&amp;fromLobby=true</t>
-  </si>
-  <si>
-    <t>https://www.fanduel.com/e/Game/11476?tableId=9923099&amp;fromLobby=true</t>
-  </si>
-  <si>
-    <t>https://www.fanduel.com/e/Game/11476?tableId=9922574&amp;fromLobby=true</t>
-  </si>
-  <si>
-    <t>https://www.fanduel.com/e/Game/11476?tableId=9923154&amp;fromLobby=true</t>
-  </si>
-  <si>
     <t>Implemented process, continous effort. Needs to be implemented for player lineups</t>
   </si>
   <si>
@@ -1001,9 +761,6 @@
     <t>Store in local text file?</t>
   </si>
   <si>
-    <t>Matt Carkner</t>
-  </si>
-  <si>
     <t>Matt Greene</t>
   </si>
   <si>
@@ -1016,36 +773,12 @@
     <t>Jamie McGinn</t>
   </si>
   <si>
-    <t>Jamie McBain</t>
-  </si>
-  <si>
-    <t>Bobby Butler</t>
-  </si>
-  <si>
-    <t>Patrice Cormier</t>
-  </si>
-  <si>
-    <t>Patrice Bergeron</t>
-  </si>
-  <si>
     <t>John Gibson</t>
   </si>
   <si>
     <t>John Carlson</t>
   </si>
   <si>
-    <t>Nathan Horton</t>
-  </si>
-  <si>
-    <t>Jonathan Drouin</t>
-  </si>
-  <si>
-    <t>Carl Klingberg</t>
-  </si>
-  <si>
-    <t>John Klingberg</t>
-  </si>
-  <si>
     <t>Brad Winchester</t>
   </si>
   <si>
@@ -1055,36 +788,12 @@
     <t>Brad Richardson</t>
   </si>
   <si>
-    <t>Peter Budaj</t>
-  </si>
-  <si>
     <t>Chad LaRose</t>
   </si>
   <si>
-    <t>Ray Whitney</t>
-  </si>
-  <si>
-    <t>Joe Whitney</t>
-  </si>
-  <si>
-    <t>Ray Emery</t>
-  </si>
-  <si>
-    <t>Dan Ellis</t>
-  </si>
-  <si>
     <t>Ryan Ellis</t>
   </si>
   <si>
-    <t>Brad Thiessen</t>
-  </si>
-  <si>
-    <t>Frans Nielsen</t>
-  </si>
-  <si>
-    <t>Sheldon Brookbank</t>
-  </si>
-  <si>
     <t>Andrei Loktionov</t>
   </si>
   <si>
@@ -1094,15 +803,6 @@
     <t>Nathan Beaulieu</t>
   </si>
   <si>
-    <t>Josh Jooris</t>
-  </si>
-  <si>
-    <t>Danny Taylor</t>
-  </si>
-  <si>
-    <t>Manny Malhotra</t>
-  </si>
-  <si>
     <t>Matthew Hackett</t>
   </si>
   <si>
@@ -1148,27 +848,12 @@
     <t>Mat Clark</t>
   </si>
   <si>
-    <t>Johan Larsson</t>
-  </si>
-  <si>
     <t>Patrick Bordeleau</t>
   </si>
   <si>
     <t>Josh Manson</t>
   </si>
   <si>
-    <t>Shawn Thornton</t>
-  </si>
-  <si>
-    <t>Andrei Vasilevskiy</t>
-  </si>
-  <si>
-    <t>Andrew Campbell</t>
-  </si>
-  <si>
-    <t>Chris Porter</t>
-  </si>
-  <si>
     <t>Cory Conacher</t>
   </si>
   <si>
@@ -1178,10 +863,298 @@
     <t>Tomas Vincour</t>
   </si>
   <si>
-    <t>Jesse Blacker</t>
-  </si>
-  <si>
     <t>Brian Dumoulin</t>
+  </si>
+  <si>
+    <t>{u'MIN': [['Zach Parise', 'Mikael Granlund', 'Thomas Vanek'], ['Jason Zucker', 'Mikko Koivu', 'Jason Pominville'], ['Ryan Carter', 'Charlie Coyle', 'Nino Niederreiter'], ['Matt Cooke', 'Kyle Brodziak', 'Justin Fontaine'], ['Ryan Suter', 'Jonas Brodin'], ['Jared Spurgeon', 'Marco Scandella'], ['Nate Prosser', 'Mathew Dumba'], ['Zach Parise', 'Mikko Koivu', 'Thomas Vanek', 'Ryan Suter', 'Jason Pominville'], ['Nino Niederreiter', 'Mikael Granlund', 'Charlie Coyle', 'Jared Spurgeon', 'Mathew Dumba']], u'TOR': [['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel'], ['Daniel Winnik', 'Nazem Kadri', 'Mike Santorelli'], ['Leo Komarov', 'Peter Holland', 'David Clarkson'], ['David Booth', 'Trevor Smith', 'Joffrey Lupul'], ['Korbinian Holzer', 'Cody Franson'], ['Morgan Rielly', 'Roman Polak'], ['Jake Gardiner', 'Petter Granberg'], ['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel', 'Peter Holland', 'Cody Franson'], ['Joffrey Lupul', 'Nazem Kadri', 'David Clarkson', 'Morgan Rielly', 'Jake Gardiner']], u'CAR': [['Eric Staal', 'Jordan Staal', 'Jiri Tlusty'], ['Nathan Gerbe', 'Victor Rask', 'Elias Lindholm'], ['Jeff Skinner', 'Riley Nash', 'Chris Terry'], ['Brad Malone', 'Jay McClement', 'Pat Dwyer'], ['Andrej Sekera', 'Justin Faulk'], ['Ryan Murphy', 'Tim Gleason'], ['Ron Hainsey', 'Brett Bellemore'], ['Eric Staal', 'Jordan Staal', 'Riley Nash', 'Ryan Murphy', 'Jeff Skinner'], ['Jiri Tlusty', 'Victor Rask', 'Nathan Gerbe', 'Elias Lindholm', 'Justin Faulk']], u'BOS': [['Milan Lucic', 'David Krejci', 'Reilly Smith'], ['Brad Marchand', 'Patrice Bergeron', 'Loui Eriksson'], ['Chris Kelly', 'Carl Soderberg', 'David Pastrnak'], ['Daniel Paille', 'Gregory Campbell', 'Craig Cunningham'], ['Zdeno Chara', 'Dougie Hamilton'], ['Dennis Seidenberg', 'Adam McQuaid'], ['Torey Krug', 'Kevan Miller'], ['Loui Eriksson', 'Patrice Bergeron', 'Carl Soderberg', 'Reilly Smith', 'Dougie Hamilton'], ['Milan Lucic', 'David Krejci', 'David Pastrnak', 'Zdeno Chara', 'Torey Krug']], u'DET': [['Gustav Nyquist', 'Henrik Zetterberg', 'Justin Abdelkader'], ['Tomas Tatar', 'Pavel Datsyuk', 'Darren Helm'], ['Stephen Weiss', 'Riley Sheahan', 'Luke Glendening'], ['Drew Miller', 'Joakim Andersson', 'Tomas Jurco'], ['Jonathan Ericsson', 'Niklas Kronwall'], ['Kyle Quincey', 'Dan DeKeyser'], ['Brendan Smith', 'Jakub Kindl'], ['Gustav Nyquist', 'Henrik Zetterberg', 'Justin Abdelkader', 'Stephen Weiss', 'Niklas Kronwall'], ['Tomas Tatar', 'Riley Sheahan', 'Darren Helm', 'Pavel Datsyuk', 'Dan DeKeyser']], u'NAS': [['Filip Forsberg', 'Mike Ribeiro', 'Craig Smith'], ['Colin Wilson', 'Mike Fisher', 'James Neal'], ['Matt Cullen', 'Calle Jarnkrok', 'Gabriel Bourque'], ['Eric Nystrom', 'Paul Gaustad', 'Olli Jokinen'], ['Roman Josi', 'Shea Weber'], ['Victor Bartley', 'Seth Jones'], ['Mattias Ekholm', 'Anton Volchenkov'], ['Filip Forsberg', 'Mike Fisher', 'James Neal', 'Roman Josi', 'Shea Weber'], ['Colin Wilson', 'Mike Ribeiro', 'Craig Smith', 'Seth Jones', 'Mattias Ekholm']], u'NYI': [['Mikhail Grabovski', 'John Tavares', 'Josh Bailey'], ['Anders Lee', 'Frans Nielsen', 'Ryan Strome'], ['Michael Grabner', 'Brock Nelson', 'Nikolay Kulemin'], ['Matt Martin', 'Casey Cizikas', 'Cal Clutterbuck'], ['Calvin de Haan', 'Travis Hamonic'], ['Nick Leddy', 'Johnny Boychuk'], ['Thomas Hickey', 'Brian Strait'], ['Brock Nelson', 'John Tavares', 'Ryan Strome', 'Frans Nielsen', 'Johnny Boychuk'], ['Anders Lee', 'Mikhail Grabovski', 'Josh Bailey', 'Nick Leddy', 'Travis Hamonic']], u'FLA': [['Jonathan Huberdeau', 'Aleksander Barkov', 'Brad Boyes'], ['Brandon Pirri', 'Nick Bjugstad', 'Jimmy Hayes'], ['Sean Bergenheim', 'Dave Bolland', 'Jussi Jokinen'], ['Tomas Kopecky', 'Derek MacKenzie', 'Shawn Thornton'], ['Brian Campbell', 'Aaron Ekblad'], ['Willie Mitchell', 'Erik Gudbranson'], ['Alex Petrovic', 'Dmitry Kulikov'], ['Jonathan Huberdeau', 'Nick Bjugstad', 'Jimmy Hayes', 'Aleksander Barkov', 'Aaron Ekblad'], ['Jussi Jokinen', 'Dave Bolland', 'Brad Boyes', 'Brian Campbell', 'Dmitry Kulikov']], u'COL': [['Gabriel Landeskog', "Ryan O'Reilly", 'Nathan Mackinnon'], ['Alex Tanguay', 'Matt Duchene', 'Jarome Iginla'], ['Cody McLeod', 'John Mitchell', 'Dennis Everberg'], ['Max Talbot', 'Marc-Andre Cliche', 'Danny Briere'], ['Jan Hejda', 'Zach Redmond'], ['Nate Guenin', 'Tyson Barrie'], ['Brad Stuart', 'Nick Holden'], ['Gabriel Landeskog', "Ryan O'Reilly", 'Nathan Mackinnon', 'Nick Holden', 'Tyson Barrie'], ['Cody McLeod', 'Matt Duchene', 'Jarome Iginla', 'Alex Tanguay', 'Zach Redmond']], u'NJD': [['Adam Henrique', 'Scott Gomez', 'Jaromir Jagr'], ['Patrik Elias', 'Travis Zajac', 'Martin Havlat'], ['Dainius Zubrus', 'Michael Cammalleri', 'Steve Bernier'], ['Jordin Tootoo', 'Jacob Josefson', 'Tuomo Ruutu'], ['Andy Greene', 'Adam Larsson'], ['Mark Fraser', 'Marek Zidlicky'], ['Jon Merrill', 'Peter Harrold'], ['Jordin Tootoo', 'Travis Zajac', 'Martin Havlat', 'Patrik Elias', 'Marek Zidlicky'], ['Michael Cammalleri', 'Scott Gomez', 'Jaromir Jagr', 'Andy Greene', 'Steve Bernier']], u'DAL': [['Jamie Benn', 'Tyler Seguin', 'Patrick Eaves'], ['Shawn Horcoff', 'Jason Spezza', 'Ales Hemsky'], ['Antoine Roussel', 'Cody Eakin', 'Ryan Garbutt'], ['Travis Moen', 'Vernon Fiddler', 'Colton Sceviour'], ['Alex Goligoski', 'John Klingberg'], ['Jamie Oleksiak', 'Trevor Daley'], ['David Schlemko', 'Jason Demers'], ['Jamie Benn', 'Jason Spezza', 'Patrick Eaves', 'Tyler Seguin', 'John Klingberg'], ['Colton Sceviour', 'Shawn Horcoff', 'Ales Hemsky', 'Jason Demers', 'Trevor Daley']], u'CGY': [['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler'], ['Mason Raymond', 'Josh Jooris', 'Joe Colborne'], ['Lance Bouma', 'Mikael Backlund', 'David Jones'], ['Brandon Bollig', 'Matt Stajan', 'Paul Byron'], ['Mark Giordano', 'T.J. Brodie'], ['Kris Russell', 'Dennis Wideman'], ['Raphael Diaz', 'Deryk Engelland'], ['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler', 'Dennis Wideman', 'Mark Giordano'], ['Mason Raymond', 'Mikael Backlund', 'Joe Colborne', 'T.J. Brodie', 'Raphael Diaz']], u'NYR': [['Rick Nash', 'Derick Brassard', 'Mats Zuccarello'], ['Chris Kreider', 'Derek Stepan', 'Martin St. Louis'], ['Carl Hagelin', 'Dominic Moore', 'Lee Stempniak'], ['Tanner Glass', 'Kevin Hayes', 'Jesper Fast'], ['Ryan McDonagh', 'Dan Girardi'], ['Marc Staal', 'Kevin Klein'], ['John Moore', 'Dan Boyle'], ['Rick Nash', 'Derick Brassard', 'Martin St. Louis', 'Derek Stepan', 'Dan Boyle'], ['Chris Kreider', 'Mats Zuccarello', 'Lee Stempniak', 'Ryan McDonagh', 'Dan Girardi']], u'SJS': [['Melker Karlsson', 'Joe Thornton', 'Joe Pavelski'], ['Patrick Marleau', 'Logan Couture', 'Matthew Nieto'], ['Tomas Hertl', 'James Sheppard', 'Barclay Goodrow'], ['Tye McGinn', 'Andrew Desjardins', 'John Scott'], ['Marc-Edouard Vlasic', 'Brent Burns'], ['Brenden Dillon', 'Matt Tennyson'], ['Matt Irwin', 'Scott Hannan'], ['Patrick Marleau', 'Joe Thornton', 'Logan Couture', 'Joe Pavelski', 'Brent Burns'], ['Melker Karlsson', 'Tomas Hertl', 'Matthew Nieto', 'Marc-Edouard Vlasic', 'Matt Tennyson']], u'PIT': [['Chris Kunitz', 'Sidney Crosby', 'David Perron'], ['Nick Spaling', 'Brandon Sutter', 'Patric Hornqvist'], ['Mark Arcobello', 'Maxim Lapierre', 'Steve Downie'], ['Zach Sill', 'Andrew Ebbett', 'Craig Adams'], ['Simon Despres', 'Kris Letang'], ['Rob Scuderi', 'Paul Martin'], ['Robert Bortuzzo', 'Scott Harrington'], ['David Perron', 'Sidney Crosby', 'Patric Hornqvist', 'Paul Martin', 'Kris Letang'], ['Chris Kunitz', 'Brandon Sutter', 'Steve Downie', 'Simon Despres', 'Scott Harrington']], u'VAN': [['Daniel Sedin', 'Henrik Sedin', 'Radim Vrbata'], ['Chris Higgins', 'Linden Vey', 'Alexandre Burrows'], ['Shawn Matthias', 'Nick Bonino', 'Jannik Hansen'], ['Derek Dorsett', 'Bo Horvat', 'Zack Kassian'], ['Alexander Edler', 'Luca Sbisa'], ['Dan Hamhuis', 'Frank Corrado'], ['Chris Tanev', 'Yannick Weber'], ['Daniel Sedin', 'Henrik Sedin', 'Radim Vrbata', 'Alexander Edler', 'Nick Bonino'], ['Derek Dorsett', 'Linden Vey', 'Alexandre Burrows', 'Dan Hamhuis', 'Chris Higgins']], u'STL': [['Alex Steen', 'David Backes', 'T.J. Oshie'], ['Jaden Schwartz', 'Paul Stastny', 'Vladimir Tarasenko'], ['Ty Rattie', 'Joakim Lindstrom', 'Dmitrij Jaskin'], ['Steve Ott', 'Marcel Goc', 'Ryan Reaves'], ['Jay Bouwmeester', 'Alex Pietrangelo'], ['Carl Gunnarsson', 'Kevin Shattenkirk'], ['Barret Jackman', 'Ian Cole'], ['Vladimir Tarasenko', 'David Backes', 'T.J. Oshie', 'Alex Steen', 'Kevin Shattenkirk'], ['Jaden Schwartz', 'Paul Stastny', 'Dmitrij Jaskin', 'Jay Bouwmeester', 'Alex Pietrangelo']], u'CHI': [['Brandon Saad', 'Jonathan Toews', 'Marian Hossa'], ['Patrick Sharp', 'Brad Richards', 'Patrick Kane'], ['Bryan Bickell', 'Teuvo Teravainen', 'Andrew Shaw'], ['Joakim Nordstrom', 'Marcus Kruger', 'Ben Smith'], ['Duncan Keith', 'David Rundblad'], ['Niklas Hjalmarsson', 'Brent Seabrook'], ['Michal Rozsival', 'Johnny Oduya'], ['Andrew Shaw', 'Jonathan Toews', 'Patrick Kane', 'Duncan Keith', 'Patrick Sharp'], ['Bryan Bickell', 'Brandon Saad', 'Marian Hossa', 'Brad Richards', 'Brent Seabrook']], u'MTL': [['Max Pacioretty', 'Tomas Plekanec', 'Dale Weise'], ['Alex Galchenyuk', 'David Desharnais', 'Brendan Gallagher'], ['Jiri Sekac', 'Lars Eller', 'Brandon Prust'], ['Michael Bournival', 'Manny Malhotra', 'Christian Thomas'], ['Andrei Markov', 'P.K. Subban'], ['Nathan Beaulieu', 'Sergei Gonchar'], ['Alexei Emelin', 'Tom Gilbert'], ['Max Pacioretty', 'Tomas Plekanec', 'Brendan Gallagher', 'Andrei Markov', 'P.K. Subban'], ['Alex Galchenyuk', 'David Desharnais', 'Jiri Sekac', 'Nathan Beaulieu', 'Sergei Gonchar']], u'PHI': [['Brayden Schenn', 'Claude Giroux', 'Jakub Voracek'], ['Petr Straka', 'Ryan White', 'Wayne Simmonds'], ['R.J. Umberger', 'Sean Couturier', 'Matt Read'], ['Chris VandeVelde', 'Vincent Lecavalier'], ['Nick Schultz', 'Mark Streit'], ['Michael Del Zotto', 'Luke Schenn'], ['Carlo Colaiacovo', 'Andrew MacDonald'], ['Brayden Schenn', 'Claude Giroux', 'Wayne Simmonds', 'Jakub Voracek', 'Mark Streit'], ['R.J. Umberger', 'Sean Couturier', 'Vincent Lecavalier', 'Matt Read', 'Michael Del Zotto']], u'ANA': [['Patrick Maroon', 'Ryan Getzlaf', 'Corey Perry'], ['Kyle Palmieri', 'Ryan Kesler', 'Matt Beleskey'], ['Andrew Cogliano', 'Rickard Rakell', 'Jakob Silfverberg'], ['Rene Bourque', 'Nate Thompson', 'Devante Smith-Pelly'], ['Cam Fowler', 'Ben Lovejoy'], ['Hampus Lindholm', 'Francois Beauchemin'], ['Clayton Stoner', 'Sami Vatanen'], ['Patrick Maroon', 'Ryan Getzlaf', 'Corey Perry', 'Cam Fowler', 'Sami Vatanen'], ['Rickard Rakell', 'Ryan Kesler', 'Kyle Palmieri', 'Francois Beauchemin', 'Hampus Lindholm']], u'LAK': [['Marian Gaborik', 'Anze Kopitar', 'Dustin Brown'], ['Dwight King', 'Jeff Carter', 'Tyler Toffoli'], ['Kyle Clifford', 'Jarret Stoll', 'Justin Williams'], ['Trevor Lewis', 'Nick Shore', 'Jordan Nolan'], ['Jake Muzzin', 'Drew Doughty'], ['Robyn Regehr', 'Alec Martinez'], ['Brayden McNabb', 'Matt Greene'], ['Marian Gaborik', 'Anze Kopitar', 'Justin Williams', 'Jake Muzzin', 'Drew Doughty'], ['Dwight King', 'Jeff Carter', 'Tyler Toffoli', 'Brayden McNabb', 'Alec Martinez']], u'CBJ': [['Nick Foligno', 'Ryan Johansen', 'Cam Atkinson'], ['Scott Hartnell', 'Brandon Dubinsky', 'Corey Tropp'], ['Matt Calvert', 'Artem Anisimov', 'Alexander Wennberg'], ['Jack Skille', 'Mark Letestu', 'Jared Boll'], ['Jack Johnson', 'David Savard'], ['Kevin Connauton', 'James Wisniewski'], ['Fedor Tyutin', 'Dalton Prout'], ['Nick Foligno', 'Ryan Johansen', 'Cam Atkinson', 'Jack Johnson', 'David Savard'], ['Scott Hartnell', 'Artem Anisimov', 'Brandon Dubinsky', 'Kevin Connauton', 'Mark Letestu']], u'BUF': [['Matt Moulson', 'Zemgus  Girgensons', 'Tyler Ennis'], ['Brian Flynn', 'Torrey Mitchell', 'Brian Gionta'], ['Drew Stafford', 'Cody Hodgson', 'Chris Stewart'], ['Nicolas Deslauriers', 'Matt Ellis', 'Patrick Kaleta'], ['Josh Gorges', 'Tyler Myers'], ['Mike Weber', 'Tyson Strachan'], ['Andrej Meszaros', 'Rasmus Ristolainen'], ['Chris Stewart', 'Zemgus  Girgensons', 'Tyler Ennis', 'Rasmus Ristolainen', 'Tyler Myers'], ['Matt Moulson', 'Brian Flynn', 'Drew Stafford', 'Josh Gorges', 'Andrej Meszaros']], u'EDM': [['Benoit Pouliot', 'Ryan Nugent-Hopkins', 'Jordan Eberle'], ['Nail Yakupov', 'Derek Roy', 'Teddy Purcell'], ['Matt Hendricks', 'Boyd Gordon', 'Rob Klinkhammer'], ['Matt Fraser', 'Anton Lander', 'Luke Gazdic'], ['Oscar Klefbom', 'Justin Schultz'], ['Andrew Ference', 'Jeff Petry'], ['Nikita Nikitin', 'Mark Fayne'], ['Benoit Pouliot', 'Ryan Nugent-Hopkins', 'Teddy Purcell', 'Jordan Eberle', 'Justin Schultz'], ['Matt Fraser', 'Derek Roy', 'Anton Lander', 'Nikita Nikitin', 'Nail Yakupov']], u'TBL': [['Valtteri Filppula', 'Steven Stamkos', 'Ryan Callahan'], ['Ondrej Palat', 'Tyler Johnson', 'Nikita Kucherov'], ['Alex Killorn', 'Cedric Paquette', 'Jonathan Drouin'], ['J.T. Brown', 'Brian Boyle', 'Brett Connolly'], ['Andrej Sustr', 'Victor Hedman'], ['Mark Barberio', 'Anton Stralman'], ['Jason Garrison', 'Nikita Nesterov'], ['Jonathan Drouin', 'Steven Stamkos', 'Ryan Callahan', 'Valtteri Filppula', 'Anton Stralman'], ['Ondrej Palat', 'Tyler Johnson', 'Brett Connolly', 'Jason Garrison', 'Nikita Kucherov']], u'WIN': [['Andrew Ladd', 'Bryan Little', 'Blake Wheeler'], ['Mathieu Perreault', 'Mark Scheifele', 'Michael Frolik'], ['Evander Kane', 'Adam Lowry', 'Chris Thorburn'], ['Matt Halischuk', 'Jim Slater', 'Anthony Peluso'], ['Ben Chiarot', 'Dustin Byfuglien'], ['Tobias Enstrom', 'Zach Bogosian'], ['Mark Stuart', 'Jacob Trouba'], ['Evander Kane', 'Mark Scheifele', 'Michael Frolik', 'Mathieu Perreault', 'Dustin Byfuglien'], ['Andrew Ladd', 'Bryan Little', 'Blake Wheeler', 'Tobias Enstrom', 'Jacob Trouba']], u'ARI': [['Tobias Rieder', 'Antoine Vermette', 'Shane Doan'], ['Martin Erat', 'Martin Hanzal', 'Sam Gagner'], ['Lauri Korpikoski', 'Kyle Chipchura', 'David Moss'], ['Lucas Lessio', 'Brendan Shinnimin', 'B.J. Crombeen'], ['Keith Yandle', 'Michael Stone'], ['Oliver Ekman-Larsson', 'Zbynek Michalek'], ['Andrew Campbell', 'Connor Murphy'], ['Sam Gagner', 'Antoine Vermette', 'Shane Doan', 'Oliver Ekman-Larsson', 'Keith Yandle'], ['Tobias Rieder', 'Martin Hanzal', 'Martin Erat', 'Michael Stone', 'Connor Murphy']], u'OTT': [['Clarke MacArthur', 'Mika Zibanejad', 'Bobby Ryan'], ['Mike Hoffman', 'Kyle Turris', 'Curtis Lazar'], ['Milan Michalek', 'David Legwand', 'Mark Stone'], ['Erik Condra', 'Jean-Gabriel Pageau', 'Chris Neil'], ['Marc Methot', 'Erik Karlsson'], ['Jared Cowen', 'Cody Ceci'], ['Eric Gryba', 'Chris Phillips'], ['Clarke MacArthur', 'Mika Zibanejad', 'Bobby Ryan', 'Erik Karlsson', 'Cody Ceci'], ['Milan Michalek', 'Kyle Turris', 'Mark Stone', 'Mike Hoffman', 'Chris Phillips']]}</t>
+  </si>
+  <si>
+    <t>Kyle Cumiskey</t>
+  </si>
+  <si>
+    <t>Kyle Quincey</t>
+  </si>
+  <si>
+    <t>Kyle Turris</t>
+  </si>
+  <si>
+    <t>Kyle Palmieri</t>
+  </si>
+  <si>
+    <t>Eric Brewer</t>
+  </si>
+  <si>
+    <t>Eric Fehr</t>
+  </si>
+  <si>
+    <t>Troy Brouwer</t>
+  </si>
+  <si>
+    <t>Martin Brodeur</t>
+  </si>
+  <si>
+    <t>Martin Jones</t>
+  </si>
+  <si>
+    <t>Martin Erat</t>
+  </si>
+  <si>
+    <t>Martin St. Louis</t>
+  </si>
+  <si>
+    <t>Jason LaBarbera</t>
+  </si>
+  <si>
+    <t>Jason Chimera</t>
+  </si>
+  <si>
+    <t>Jason Garrison</t>
+  </si>
+  <si>
+    <t>Blake Comeau</t>
+  </si>
+  <si>
+    <t>Marcus Foligno</t>
+  </si>
+  <si>
+    <t>Nick Foligno</t>
+  </si>
+  <si>
+    <t>Marcus Johansson</t>
+  </si>
+  <si>
+    <t>Ruslan Fedotenko</t>
+  </si>
+  <si>
+    <t>Ryane Clowe</t>
+  </si>
+  <si>
+    <t>Ryan Strome</t>
+  </si>
+  <si>
+    <t>Ryan Miller</t>
+  </si>
+  <si>
+    <t>Jared Cowen</t>
+  </si>
+  <si>
+    <t>Ian Cole</t>
+  </si>
+  <si>
+    <t>Matt Climie</t>
+  </si>
+  <si>
+    <t>Matt Cullen</t>
+  </si>
+  <si>
+    <t>Matt Read</t>
+  </si>
+  <si>
+    <t>Reto Berra</t>
+  </si>
+  <si>
+    <t>Paul Bissonnette</t>
+  </si>
+  <si>
+    <t>Beau Bennett</t>
+  </si>
+  <si>
+    <t>Paul Byron</t>
+  </si>
+  <si>
+    <t>Emerson Etem</t>
+  </si>
+  <si>
+    <t>Kris Versteeg</t>
+  </si>
+  <si>
+    <t>Peter Mueller</t>
+  </si>
+  <si>
+    <t>Peter Holland</t>
+  </si>
+  <si>
+    <t>Damien Brunner</t>
+  </si>
+  <si>
+    <t>Derrick Pouliot</t>
+  </si>
+  <si>
+    <t>Olli Maatta</t>
+  </si>
+  <si>
+    <t>Jeff Zatkoff</t>
+  </si>
+  <si>
+    <t>Jeff Carter</t>
+  </si>
+  <si>
+    <t>Mark Pysyk</t>
+  </si>
+  <si>
+    <t>Mark Fayne</t>
+  </si>
+  <si>
+    <t>Scott Darling</t>
+  </si>
+  <si>
+    <t>Scott Harrington</t>
+  </si>
+  <si>
+    <t>Scott Hartnell</t>
+  </si>
+  <si>
+    <t>Scott Hannan</t>
+  </si>
+  <si>
+    <t>Damon Severson</t>
+  </si>
+  <si>
+    <t>Kevin Shattenkirk</t>
+  </si>
+  <si>
+    <t>David Backes</t>
+  </si>
+  <si>
+    <t>T.J. Oshie</t>
+  </si>
+  <si>
+    <t>Paul Martin</t>
+  </si>
+  <si>
+    <t>Jake Allen</t>
+  </si>
+  <si>
+    <t>John Mitchell</t>
+  </si>
+  <si>
+    <t>Viktor Stalberg</t>
+  </si>
+  <si>
+    <t>Jack Hillen</t>
+  </si>
+  <si>
+    <t>Jack Skille</t>
+  </si>
+  <si>
+    <t>Jared Boll</t>
+  </si>
+  <si>
+    <t>Calvin Pickard</t>
+  </si>
+  <si>
+    <t>Alexander Steen</t>
+  </si>
+  <si>
+    <t>Alexander Edler</t>
+  </si>
+  <si>
+    <t>Alexander Wennberg</t>
+  </si>
+  <si>
+    <t>Pekka Rinne</t>
+  </si>
+  <si>
+    <t>Miikka Salomaki</t>
+  </si>
+  <si>
+    <t>Andrej Sekera</t>
+  </si>
+  <si>
+    <t>Andrew Desjardins</t>
+  </si>
+  <si>
+    <t>Michael Hutchinson</t>
+  </si>
+  <si>
+    <t>Ryan O'Reilly</t>
+  </si>
+  <si>
+    <t>Ryan White</t>
+  </si>
+  <si>
+    <t>Ryan Stanton</t>
+  </si>
+  <si>
+    <t>Ryan Johansen</t>
+  </si>
+  <si>
+    <t>Ryan Suter</t>
+  </si>
+  <si>
+    <t>Mike Richards</t>
+  </si>
+  <si>
+    <t>Brad Marchand</t>
+  </si>
+  <si>
+    <t>Brad Malone</t>
+  </si>
+  <si>
+    <t>['VAN', 'VAN', 'VAN', 'VAN', 'VAN']</t>
+  </si>
+  <si>
+    <t>['STL', 'STL', 'STL', 'STL']</t>
+  </si>
+  <si>
+    <t>['PIT', 'PIT', 'PIT', 'PIT', 'PIT', 'PIT']</t>
+  </si>
+  <si>
+    <t>Brandon Sutter</t>
+  </si>
+  <si>
+    <t>data_scrapping.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Cole\Desktop\FanDuel\fanduel\modules\data_scrapping.py</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10195041&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10195201&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10195752&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10196255&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10195995&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10195967&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10195565&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>https://www.fanduel.com/e/Game/11536?tableId=10194829&amp;fromLobby=true</t>
+  </si>
+  <si>
+    <t>Analyzed Entries</t>
+  </si>
+  <si>
+    <t>Avg_ToI*Avg_Line_Goals + Vegas</t>
+  </si>
+  <si>
+    <t>Major Category</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Software Testing Course</t>
+  </si>
+  <si>
+    <t>Sublime Text</t>
+  </si>
+  <si>
+    <t>Programming Design Course</t>
   </si>
 </sst>
 </file>
@@ -1838,11 +1811,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="216687360"/>
-        <c:axId val="216688896"/>
+        <c:axId val="199844608"/>
+        <c:axId val="199846144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216687360"/>
+        <c:axId val="199844608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1851,7 +1824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216688896"/>
+        <c:crossAx val="199846144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1859,7 +1832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216688896"/>
+        <c:axId val="199846144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1870,7 +1843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216687360"/>
+        <c:crossAx val="199844608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1983,11 +1956,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216717184"/>
-        <c:axId val="216718720"/>
+        <c:axId val="199874432"/>
+        <c:axId val="199875968"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="216717184"/>
+        <c:axId val="199874432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +1969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216718720"/>
+        <c:crossAx val="199875968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2004,7 +1977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="216718720"/>
+        <c:axId val="199875968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2015,7 +1988,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216717184"/>
+        <c:crossAx val="199874432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2044,160 +2017,6 @@
       </c14:pivotOptions>
     </c:ext>
   </c:extLst>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Performance Monitoring'!$C$2:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>723.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1096.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1716.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>933.8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>657.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>538</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>699.95</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Performance Monitoring'!$I$2:$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.33750000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.23749999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.26250000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="218431488"/>
-        <c:axId val="218433024"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="218431488"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218433024"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="218433024"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218431488"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -2266,45 +2085,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2800349</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Cole MacLean" refreshedDate="42015.695505324074" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="6">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J1048576" sheet="Performance Monitoring"/>
+    <worksheetSource ref="A1:K1048576" sheet="Performance Monitoring"/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Contest Date" numFmtId="0">
@@ -2863,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2871,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2879,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2887,7 +2671,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2895,7 +2679,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>364</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2903,7 +2687,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2911,7 +2695,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2954,10 +2738,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,86 +2751,83 @@
     <col min="3" max="3" width="17" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>126</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
         <v>127</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>42015</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>188</v>
+        <v>42034</v>
+      </c>
+      <c r="B2" t="s">
+        <v>358</v>
       </c>
       <c r="C2" s="5">
-        <v>723.2</v>
+        <v>1329.8</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G2">
-        <v>1.8</v>
-      </c>
-      <c r="H2" s="5">
-        <v>27</v>
-      </c>
-      <c r="I2" s="5">
-        <f>H2/D2</f>
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="J2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>42015</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>187</v>
+        <v>42034</v>
+      </c>
+      <c r="B3" t="s">
+        <v>359</v>
       </c>
       <c r="C3" s="5">
-        <v>1096.8</v>
+        <v>1401.8</v>
       </c>
       <c r="D3">
         <v>40</v>
@@ -3054,32 +2835,25 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="5">
-        <v>3.6</v>
-      </c>
-      <c r="H3" s="5">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" ref="I3:I9" si="0">H3/D3</f>
-        <v>0.375</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="5">
+        <v>21</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>42015</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>186</v>
+        <v>42034</v>
+      </c>
+      <c r="B4" t="s">
+        <v>360</v>
       </c>
       <c r="C4" s="5">
-        <v>1716.5</v>
+        <v>1654.2</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -3087,317 +2861,43 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" s="5">
-        <v>9</v>
-      </c>
-      <c r="H4" s="5">
-        <v>14</v>
-      </c>
-      <c r="I4" s="5">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>42015</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C5" s="5">
-        <v>933.8</v>
-      </c>
-      <c r="D5">
-        <v>80</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="H5" s="5">
-        <v>24</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>42020</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="5">
-        <v>657.45</v>
-      </c>
-      <c r="D6">
-        <v>80</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1.8</v>
-      </c>
-      <c r="H6" s="5">
-        <v>19</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" si="0"/>
-        <v>0.23749999999999999</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>42020</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C7" s="5">
-        <v>538</v>
-      </c>
-      <c r="D7">
-        <v>40</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G7">
-        <v>9</v>
-      </c>
-      <c r="H7" s="5">
-        <v>13</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>42020</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C8" s="5">
-        <v>699.95</v>
-      </c>
-      <c r="D8">
-        <v>80</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8">
-        <v>1.8</v>
-      </c>
-      <c r="H8" s="5">
-        <v>21</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.26250000000000001</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>42021</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2493.6999999999998</v>
-      </c>
-      <c r="D9">
-        <v>40</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>27</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>42024</v>
-      </c>
-      <c r="B10" t="s">
-        <v>312</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1750.3</v>
-      </c>
-      <c r="D10">
-        <v>80</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>42024</v>
-      </c>
-      <c r="B11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C11" s="5">
-        <v>3036</v>
-      </c>
-      <c r="D11">
-        <v>40</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>42024</v>
-      </c>
-      <c r="B12" t="s">
-        <v>314</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1702.55</v>
-      </c>
-      <c r="D12">
-        <v>80</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>42024</v>
-      </c>
-      <c r="B13" t="s">
-        <v>315</v>
-      </c>
-      <c r="C13" s="5">
-        <v>1733.4</v>
-      </c>
-      <c r="D13">
-        <v>80</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>168</v>
+      <c r="F4" s="5">
+        <v>23</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://www.fanduel.com/entry/DEEJTWTWY"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.fanduel.com/entry/CSYJRDAAZ"/>
-    <hyperlink ref="B3" r:id="rId3" display="https://www.fanduel.com/entry/AEQJGHJDX"/>
-    <hyperlink ref="B2" r:id="rId4" display="https://www.fanduel.com/entry/DCOQLQLKB"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://www.fanduel.com/entry/BFXNHPTME"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.fanduel.com/entry/BEVROMGZP"/>
-    <hyperlink ref="B6" r:id="rId7" display="https://www.fanduel.com/entry/EUKTUOFAN"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://www.fanduel.com/entry/CPFDKFGQD"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="82.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="6" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -3405,383 +2905,449 @@
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="6">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="6">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="6">
-        <v>3</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="6">
-        <v>4</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="6">
-        <v>5</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="E14" s="6">
         <v>2</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="F14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="6">
+        <v>4</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="B16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="6">
         <v>4</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="F16" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="6">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D16" s="6">
+      <c r="B18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="6">
+        <v>6</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E20" s="6">
         <v>4</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="6">
-        <v>5</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="6">
-        <v>6</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>358</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="D20" s="6">
-        <v>4</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>361</v>
+        <v>261</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>362</v>
+        <v>262</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>360</v>
+        <v>260</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G22"/>
+  <autoFilter ref="A1:H22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3812,19 +3378,19 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="L2" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
@@ -3838,7 +3404,7 @@
         <v>-1</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M3" s="13">
         <v>-1</v>
@@ -3846,7 +3412,7 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="13">
         <v>-10</v>
@@ -3855,7 +3421,7 @@
         <v>-1</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M4" s="13">
         <v>-1</v>
@@ -3873,7 +3439,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3884,7 +3450,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -3892,41 +3458,38 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3">
-        <v>696</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>308</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6">
-        <v>10000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3982,15 +3545,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2">
         <v>13</v>
@@ -3998,7 +3561,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -4006,7 +3569,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -4014,7 +3577,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5">
         <v>16</v>
@@ -4022,7 +3585,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6">
         <v>17</v>
@@ -4030,7 +3593,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7">
         <v>18</v>
@@ -4038,7 +3601,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -4046,7 +3609,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -4054,7 +3617,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10">
         <v>21</v>
@@ -4062,7 +3625,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="5">
         <v>22</v>
@@ -4070,7 +3633,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="5">
         <v>23</v>
@@ -4078,7 +3641,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13" s="5">
         <v>24</v>
@@ -4086,7 +3649,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" s="5">
         <v>25</v>
@@ -4094,7 +3657,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" s="5">
         <v>26</v>
@@ -4102,7 +3665,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="5">
         <v>27</v>
@@ -4110,7 +3673,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="5">
         <v>28</v>
@@ -4118,7 +3681,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B18" s="5">
         <v>29</v>
@@ -4126,7 +3689,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="5">
         <v>30</v>
@@ -4134,7 +3697,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" s="5">
         <v>31</v>
@@ -4142,7 +3705,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21" s="5">
         <v>32</v>
@@ -4150,7 +3713,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B22" s="5">
         <v>33</v>
@@ -4158,7 +3721,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="5">
         <v>34</v>
@@ -4166,7 +3729,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B24" s="5">
         <v>35</v>
@@ -4174,7 +3737,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="5">
         <v>36</v>
@@ -4182,7 +3745,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" s="5">
         <v>37</v>
@@ -4190,7 +3753,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B27" s="5">
         <v>38</v>
@@ -4198,7 +3761,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B28" s="5">
         <v>39</v>
@@ -4206,7 +3769,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B29" s="5">
         <v>40</v>
@@ -4214,7 +3777,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B30" s="5">
         <v>41</v>
@@ -4222,7 +3785,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B31" s="5">
         <v>42</v>
@@ -4241,7 +3804,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="A63" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -4256,639 +3819,876 @@
     <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G2" t="s">
-        <v>320</v>
+        <v>239</v>
       </c>
       <c r="H2" t="s">
-        <v>321</v>
+        <v>240</v>
       </c>
       <c r="I2" t="s">
-        <v>322</v>
+        <v>241</v>
       </c>
       <c r="J2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>328</v>
       </c>
       <c r="B3" t="s">
-        <v>258</v>
+        <v>327</v>
+      </c>
+      <c r="C3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>323</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>275</v>
+      </c>
+      <c r="B5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>325</v>
+        <v>326</v>
+      </c>
+      <c r="B6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>260</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>368</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B8" t="s">
-        <v>262</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="D8" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>326</v>
+        <v>279</v>
       </c>
       <c r="B9" t="s">
-        <v>327</v>
+        <v>280</v>
       </c>
       <c r="C9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D9" t="s">
+        <v>331</v>
+      </c>
+      <c r="E9" t="s">
         <v>208</v>
       </c>
-      <c r="D9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E9" t="s">
-        <v>196</v>
-      </c>
       <c r="F9" t="s">
-        <v>369</v>
+        <v>268</v>
       </c>
       <c r="G9" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>282</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>283</v>
       </c>
       <c r="C10" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>328</v>
+        <v>286</v>
       </c>
       <c r="B11" t="s">
-        <v>329</v>
+        <v>287</v>
       </c>
       <c r="C11" t="s">
-        <v>368</v>
+        <v>288</v>
       </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="E11" t="s">
-        <v>370</v>
+        <v>269</v>
       </c>
       <c r="F11" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="G11" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="H11" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="I11" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>332</v>
       </c>
       <c r="B12" t="s">
-        <v>205</v>
+        <v>280</v>
+      </c>
+      <c r="C12" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>206</v>
+        <v>245</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>330</v>
+        <v>289</v>
       </c>
       <c r="B14" t="s">
-        <v>371</v>
+        <v>287</v>
       </c>
       <c r="C14" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="D14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="G14" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="B15" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>292</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="E15" t="s">
-        <v>215</v>
+        <v>297</v>
+      </c>
+      <c r="F15" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>246</v>
+      </c>
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" t="s">
         <v>334</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>335</v>
       </c>
-      <c r="C17" t="s">
-        <v>336</v>
+      <c r="E17" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>337</v>
       </c>
+      <c r="B18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D18" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>338</v>
+        <v>242</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>226</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>339</v>
+        <v>294</v>
       </c>
       <c r="B20" t="s">
-        <v>340</v>
+        <v>295</v>
       </c>
       <c r="C20" t="s">
-        <v>341</v>
+        <v>296</v>
+      </c>
+      <c r="D20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" t="s">
+        <v>297</v>
+      </c>
+      <c r="F20" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="B21" t="s">
-        <v>372</v>
+        <v>300</v>
+      </c>
+      <c r="C21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H21" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>302</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>309</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>195</v>
+      </c>
+      <c r="C23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D23" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>342</v>
+        <v>303</v>
       </c>
       <c r="B24" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="C24" t="s">
-        <v>269</v>
+        <v>305</v>
       </c>
       <c r="D24" t="s">
-        <v>271</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F24" t="s">
-        <v>272</v>
+        <v>211</v>
       </c>
       <c r="G24" t="s">
-        <v>273</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>306</v>
       </c>
       <c r="B25" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="C25" t="s">
-        <v>373</v>
+        <v>296</v>
       </c>
       <c r="D25" t="s">
-        <v>276</v>
+        <v>188</v>
+      </c>
+      <c r="E25" t="s">
+        <v>297</v>
+      </c>
+      <c r="F25" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>277</v>
+        <v>307</v>
       </c>
       <c r="B26" t="s">
-        <v>278</v>
+        <v>225</v>
+      </c>
+      <c r="C26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" t="s">
+        <v>185</v>
+      </c>
+      <c r="G26" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="B27" t="s">
-        <v>374</v>
+        <v>309</v>
       </c>
       <c r="C27" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="D27" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="E27" t="s">
-        <v>375</v>
+        <v>270</v>
       </c>
       <c r="F27" t="s">
-        <v>376</v>
+        <v>271</v>
       </c>
       <c r="G27" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="H27" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="I27" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="J27" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="K27" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
       <c r="B28" t="s">
-        <v>345</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
-        <v>279</v>
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
+        <v>338</v>
+      </c>
+      <c r="E28" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>280</v>
+        <v>243</v>
+      </c>
+      <c r="B29" t="s">
+        <v>244</v>
+      </c>
+      <c r="C29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" t="s">
+        <v>210</v>
+      </c>
+      <c r="F29" t="s">
+        <v>211</v>
+      </c>
+      <c r="G29" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>346</v>
+        <v>311</v>
+      </c>
+      <c r="B30" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
       <c r="B31" t="s">
-        <v>370</v>
+        <v>304</v>
       </c>
       <c r="C31" t="s">
-        <v>350</v>
+        <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>282</v>
+        <v>230</v>
       </c>
       <c r="E31" t="s">
-        <v>283</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>347</v>
+        <v>255</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>318</v>
       </c>
       <c r="C32" t="s">
-        <v>203</v>
+        <v>319</v>
+      </c>
+      <c r="D32" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>348</v>
+        <v>249</v>
       </c>
       <c r="B33" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="C33" t="s">
-        <v>349</v>
+        <v>296</v>
       </c>
       <c r="D33" t="s">
-        <v>210</v>
+        <v>341</v>
+      </c>
+      <c r="E33" t="s">
+        <v>234</v>
+      </c>
+      <c r="F33" t="s">
+        <v>200</v>
+      </c>
+      <c r="G33" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>284</v>
+        <v>253</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D34" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="B35" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C35" t="s">
-        <v>377</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>200</v>
+      </c>
+      <c r="C36" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" t="s">
+        <v>209</v>
+      </c>
+      <c r="E36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F36" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>287</v>
+        <v>315</v>
       </c>
       <c r="B37" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="C37" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="D37" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
       <c r="B38" t="s">
-        <v>217</v>
+        <v>318</v>
       </c>
       <c r="C38" t="s">
-        <v>118</v>
+        <v>319</v>
+      </c>
+      <c r="D38" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>233</v>
+        <v>321</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>351</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s">
-        <v>352</v>
+        <v>216</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>217</v>
+      </c>
+      <c r="D40" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>291</v>
+        <v>253</v>
+      </c>
+      <c r="B41" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>313</v>
+      </c>
+      <c r="B42" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B43" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="C43" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="D43" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>240</v>
+        <v>315</v>
       </c>
       <c r="B44" t="s">
-        <v>241</v>
+        <v>316</v>
       </c>
       <c r="C44" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="D44" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="E44" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="F44" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="G44" t="s">
-        <v>246</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>292</v>
+        <v>343</v>
       </c>
       <c r="B45" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>344</v>
       </c>
       <c r="D45" t="s">
-        <v>294</v>
+        <v>345</v>
+      </c>
+      <c r="E45" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
       <c r="B46" t="s">
-        <v>226</v>
+        <v>319</v>
       </c>
       <c r="C46" t="s">
-        <v>227</v>
+        <v>320</v>
       </c>
       <c r="D46" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>353</v>
+        <v>321</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>354</v>
+        <v>254</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>296</v>
+        <v>247</v>
       </c>
       <c r="B48" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="C48" t="s">
-        <v>271</v>
+        <v>346</v>
+      </c>
+      <c r="D48" t="s">
+        <v>347</v>
+      </c>
+      <c r="E48" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>355</v>
+        <v>220</v>
       </c>
       <c r="B49" t="s">
-        <v>378</v>
+        <v>216</v>
+      </c>
+      <c r="C49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>247</v>
+        <v>220</v>
       </c>
       <c r="B50" t="s">
-        <v>377</v>
+        <v>272</v>
       </c>
       <c r="C50" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="D50" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="E50" t="s">
-        <v>248</v>
+        <v>221</v>
       </c>
       <c r="F50" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>356</v>
+        <v>256</v>
       </c>
       <c r="B51" t="s">
-        <v>357</v>
+        <v>257</v>
       </c>
       <c r="C51" t="s">
-        <v>379</v>
+        <v>273</v>
       </c>
       <c r="D51" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="E51" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -4913,170 +4713,170 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
         <v>77</v>
-      </c>
-      <c r="B7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
         <v>107</v>
-      </c>
-      <c r="B13" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
         <v>109</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
         <v>111</v>
-      </c>
-      <c r="B15" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
         <v>113</v>
-      </c>
-      <c r="B16" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
         <v>105</v>
-      </c>
-      <c r="B17" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
         <v>119</v>
-      </c>
-      <c r="B18" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" t="s">
         <v>121</v>
-      </c>
-      <c r="B19" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" t="s">
         <v>123</v>
-      </c>
-      <c r="B20" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -5091,7 +4891,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5103,232 +4903,232 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>297</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>303</v>
+        <v>349</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="9">
-        <v>637.32000000000005</v>
+        <v>73.2</v>
       </c>
       <c r="E2">
-        <v>5800</v>
+        <v>3500</v>
       </c>
       <c r="F2">
-        <v>1062.2</v>
+        <v>915</v>
       </c>
       <c r="G2">
-        <v>0.6</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B3" t="s">
-        <v>303</v>
+        <v>349</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D3" s="9">
-        <v>699.12</v>
+        <v>-649.70428266700003</v>
       </c>
       <c r="E3">
-        <v>5300</v>
+        <v>8700</v>
       </c>
       <c r="F3">
-        <v>1165.2</v>
+        <v>1112.5073333299999</v>
       </c>
       <c r="G3">
-        <v>0.6</v>
+        <v>-0.58399999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>350</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D4" s="9">
-        <v>717.35416666699996</v>
+        <v>467.265625</v>
       </c>
       <c r="E4">
-        <v>6500</v>
+        <v>6200</v>
       </c>
       <c r="F4">
-        <v>1229.75</v>
+        <v>1495.25</v>
       </c>
       <c r="G4">
-        <v>0.58333333333299997</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>350</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D5" s="9">
-        <v>593.9</v>
+        <v>623.25</v>
       </c>
       <c r="E5">
-        <v>3700</v>
+        <v>7800</v>
       </c>
       <c r="F5">
-        <v>1484.75</v>
+        <v>1246.5</v>
       </c>
       <c r="G5">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>324</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>350</v>
       </c>
       <c r="C6" t="s">
         <v>164</v>
       </c>
       <c r="D6" s="9">
-        <v>793.3125</v>
+        <v>572.625</v>
       </c>
       <c r="E6">
-        <v>7600</v>
+        <v>6400</v>
       </c>
       <c r="F6">
-        <v>1057.75</v>
+        <v>1145.25</v>
       </c>
       <c r="G6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>351</v>
       </c>
       <c r="C7" t="s">
         <v>165</v>
       </c>
       <c r="D7" s="9">
-        <v>832.125</v>
+        <v>459.2</v>
       </c>
       <c r="E7">
-        <v>6000</v>
+        <v>3900</v>
       </c>
       <c r="F7">
-        <v>1109.5</v>
+        <v>1435</v>
       </c>
       <c r="G7">
-        <v>0.75</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>351</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D8" s="9">
-        <v>824.72500000000002</v>
+        <v>464.30370370399999</v>
       </c>
       <c r="E8">
-        <v>7000</v>
+        <v>7400</v>
       </c>
       <c r="F8">
-        <v>1499.5</v>
+        <v>1099.66666667</v>
       </c>
       <c r="G8">
-        <v>0.55000000000000004</v>
+        <v>0.42222222222200001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>309</v>
+        <v>352</v>
       </c>
       <c r="B9" t="s">
-        <v>310</v>
+        <v>351</v>
       </c>
       <c r="C9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D9" s="9">
-        <v>-569.35913249999999</v>
+        <v>296.25</v>
       </c>
       <c r="E9">
-        <v>8600</v>
+        <v>3500</v>
       </c>
       <c r="F9">
-        <v>1133.0530000000001</v>
+        <v>1066.5</v>
       </c>
       <c r="G9">
-        <v>-0.50249999999999995</v>
+        <v>0.277777777778</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>311</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
-        <v>307</v>
+        <v>351</v>
       </c>
       <c r="C10" t="s">
         <v>164</v>
       </c>
       <c r="D10" s="9">
-        <v>409.64</v>
+        <v>492.1</v>
       </c>
       <c r="E10">
-        <v>3800</v>
+        <v>6000</v>
       </c>
       <c r="F10">
-        <v>877.8</v>
+        <v>1165.5</v>
       </c>
       <c r="G10">
-        <v>0.46666666666700002</v>
+        <v>0.42222222222200001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="9">
         <f>SUM(D2:D10)</f>
-        <v>4938.1375341670009</v>
+        <v>2798.490046037</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
@@ -5346,10 +5146,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5360,106 +5160,176 @@
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
       <c r="B2">
-        <v>3403.3</v>
+        <v>1329.8</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B3">
+        <v>1401.8</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3">
-        <v>1913.05</v>
-      </c>
-      <c r="C3">
-        <v>70</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="B4">
-        <v>1943.25</v>
+        <v>1654.2</v>
       </c>
       <c r="C4">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>315</v>
+        <v>357</v>
       </c>
       <c r="B5">
-        <v>1733.4</v>
+        <v>2037.85</v>
       </c>
       <c r="C5">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6">
+        <v>2175.0500000000002</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7">
+        <v>2902</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8">
+        <v>3214.625</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9">
+        <v>3704.5</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.fanduel.com/e/Game/11476?tableId=9922292&amp;fromLobby=true"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.fanduel.com/e/Game/11476?tableId=9922574&amp;fromLobby=true"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactored Update NHL data to be a little cleaner/modular
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Roster" sheetId="10" r:id="rId8"/>
     <sheet name="Best Contests" sheetId="12" r:id="rId9"/>
     <sheet name="Performance Monitoring" sheetId="13" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!#REF!</definedName>
@@ -36,13 +37,13 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="385">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -1155,6 +1156,48 @@
   </si>
   <si>
     <t>Programming Design Course</t>
+  </si>
+  <si>
+    <t>Brenden Dillon</t>
+  </si>
+  <si>
+    <t>Barclay Goodrow</t>
+  </si>
+  <si>
+    <t>Brent Burns</t>
+  </si>
+  <si>
+    <t>Ilya Bryzgalov</t>
+  </si>
+  <si>
+    <t>Matt Tennyson</t>
+  </si>
+  <si>
+    <t>Melker Karlsson</t>
+  </si>
+  <si>
+    <t>Tomas Hertl</t>
+  </si>
+  <si>
+    <t>Marc-Edouard Vlasic</t>
+  </si>
+  <si>
+    <t>Logan Couture</t>
+  </si>
+  <si>
+    <t>John Scott</t>
+  </si>
+  <si>
+    <t>Joe Thornton</t>
+  </si>
+  <si>
+    <t>James Sheppard</t>
+  </si>
+  <si>
+    <t>Joe Pavelski</t>
+  </si>
+  <si>
+    <t>Antti Niemi</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1647,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1629,6 +1672,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
@@ -1811,11 +1866,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="199844608"/>
-        <c:axId val="199846144"/>
+        <c:axId val="220680960"/>
+        <c:axId val="220682496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="199844608"/>
+        <c:axId val="220680960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1824,7 +1879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199846144"/>
+        <c:crossAx val="220682496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1832,7 +1887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199846144"/>
+        <c:axId val="220682496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1843,7 +1898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199844608"/>
+        <c:crossAx val="220680960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1956,11 +2011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199874432"/>
-        <c:axId val="199875968"/>
+        <c:axId val="220710784"/>
+        <c:axId val="220712320"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="199874432"/>
+        <c:axId val="220710784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,7 +2024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199875968"/>
+        <c:crossAx val="220712320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1977,7 +2032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199875968"/>
+        <c:axId val="220712320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1988,7 +2043,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199874432"/>
+        <c:crossAx val="220710784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2877,12 +2932,710 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15">
+        <v>52018</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="15">
+        <v>0</v>
+      </c>
+      <c r="G1" s="15">
+        <v>4</v>
+      </c>
+      <c r="H1" s="15">
+        <v>1</v>
+      </c>
+      <c r="I1" s="15">
+        <v>3</v>
+      </c>
+      <c r="J1" s="16">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="K1" s="15">
+        <v>1</v>
+      </c>
+      <c r="L1" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15">
+        <v>52035</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15">
+        <v>89</v>
+      </c>
+      <c r="H2" s="15">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="16">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="K2" s="15">
+        <v>0</v>
+      </c>
+      <c r="L2" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15">
+        <v>52034</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="15">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15">
+        <v>88</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15">
+        <v>2</v>
+      </c>
+      <c r="J3" s="17">
+        <v>1.117361111111111</v>
+      </c>
+      <c r="K3" s="15">
+        <v>1</v>
+      </c>
+      <c r="L3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15">
+        <v>52056</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="15">
+        <v>80</v>
+      </c>
+      <c r="G4" s="15">
+        <v>19</v>
+      </c>
+      <c r="H4" s="17">
+        <v>1.5048611111111112</v>
+      </c>
+      <c r="I4" s="15">
+        <v>6</v>
+      </c>
+      <c r="J4" s="15">
+        <v>25</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0.76</v>
+      </c>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15">
+        <v>52032</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15">
+        <v>80</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>2</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15">
+        <v>52031</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="D6" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15">
+        <v>68</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="K6" s="15">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15">
+        <v>52030</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>52</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15">
+        <v>3</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="K7" s="15">
+        <v>1</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15">
+        <v>52029</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15">
+        <v>48</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>1</v>
+      </c>
+      <c r="J8" s="16">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="K8" s="15">
+        <v>1</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15">
+        <v>52028</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="15">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>44</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0.9590277777777777</v>
+      </c>
+      <c r="K9" s="15">
+        <v>2</v>
+      </c>
+      <c r="L9" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15">
+        <v>52027</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+      <c r="G10" s="15">
+        <v>39</v>
+      </c>
+      <c r="H10" s="15">
+        <v>0</v>
+      </c>
+      <c r="I10" s="15">
+        <v>3</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.73888888888888893</v>
+      </c>
+      <c r="K10" s="15">
+        <v>2</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15">
+        <v>52026</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0</v>
+      </c>
+      <c r="G11" s="15">
+        <v>27</v>
+      </c>
+      <c r="H11" s="15">
+        <v>0</v>
+      </c>
+      <c r="I11" s="15">
+        <v>0</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="K11" s="15">
+        <v>-1</v>
+      </c>
+      <c r="L11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15">
+        <v>52025</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="15">
+        <v>0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>25</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0</v>
+      </c>
+      <c r="I12" s="15">
+        <v>2</v>
+      </c>
+      <c r="J12" s="16">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15">
+        <v>52024</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="D13" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>20</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1</v>
+      </c>
+      <c r="J13" s="16">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="K13" s="15">
+        <v>-1</v>
+      </c>
+      <c r="L13" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15">
+        <v>52023</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="D14" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2</v>
+      </c>
+      <c r="G14" s="15">
+        <v>19</v>
+      </c>
+      <c r="H14" s="15">
+        <v>0</v>
+      </c>
+      <c r="I14" s="15">
+        <v>1</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="K14" s="15">
+        <v>0</v>
+      </c>
+      <c r="L14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15">
+        <v>52022</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="15">
+        <v>15</v>
+      </c>
+      <c r="H15" s="15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="K15" s="15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15">
+        <v>52021</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1</v>
+      </c>
+      <c r="G16" s="15">
+        <v>12</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1</v>
+      </c>
+      <c r="I16" s="15">
+        <v>6</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0.7597222222222223</v>
+      </c>
+      <c r="K16" s="15">
+        <v>2</v>
+      </c>
+      <c r="L16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15">
+        <v>52020</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="D17" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="15">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>10</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0</v>
+      </c>
+      <c r="I17" s="15">
+        <v>1</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="K17" s="15">
+        <v>0</v>
+      </c>
+      <c r="L17" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15">
+        <v>52019</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="D18" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>8</v>
+      </c>
+      <c r="H18" s="15">
+        <v>1</v>
+      </c>
+      <c r="I18" s="15">
+        <v>4</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="K18" s="15">
+        <v>-1</v>
+      </c>
+      <c r="L18" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15">
+        <v>52036</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="D19" s="15">
+        <v>2014020721</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="15">
+        <v>31</v>
+      </c>
+      <c r="G19" s="15">
+        <v>25</v>
+      </c>
+      <c r="H19" s="17">
+        <v>2.4993055555555554</v>
+      </c>
+      <c r="I19" s="15">
+        <v>3</v>
+      </c>
+      <c r="J19" s="15">
+        <v>28</v>
+      </c>
+      <c r="K19" s="15">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="L19" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -3438,8 +4191,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
created config file and check for current user to pull parameters
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -3283,11 +3283,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="217229952"/>
-        <c:axId val="217244032"/>
+        <c:axId val="245598464"/>
+        <c:axId val="245604352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217229952"/>
+        <c:axId val="245598464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,7 +3296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217244032"/>
+        <c:crossAx val="245604352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217244032"/>
+        <c:axId val="245604352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,7 +3315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217229952"/>
+        <c:crossAx val="245598464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3428,11 +3428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217788416"/>
-        <c:axId val="217789952"/>
+        <c:axId val="246226304"/>
+        <c:axId val="246232192"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="217788416"/>
+        <c:axId val="246226304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3441,7 +3441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217789952"/>
+        <c:crossAx val="246232192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3449,7 +3449,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217789952"/>
+        <c:axId val="246232192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3460,7 +3460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217788416"/>
+        <c:crossAx val="246226304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8802,7 +8802,7 @@
         <v>61</v>
       </c>
       <c r="B3" s="3">
-        <v>1169</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added inning and event to BBSim
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="10320" windowHeight="9900" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="10320" windowHeight="9900" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -18,18 +18,32 @@
     <sheet name="Best Contests" sheetId="12" r:id="rId9"/>
     <sheet name="Performance Monitoring" sheetId="13" r:id="rId10"/>
     <sheet name="Output" sheetId="17" r:id="rId11"/>
+    <sheet name="Baseball Simulation" sheetId="18" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$H$22</definedName>
+    <definedName name="cl1st">'Baseball Simulation'!$F$8</definedName>
+    <definedName name="cl2nd">'Baseball Simulation'!$F$9</definedName>
+    <definedName name="cl3rd">'Baseball Simulation'!$F$10</definedName>
     <definedName name="cLastDataDate">Parameters!#REF!</definedName>
+    <definedName name="clAwayScore">'Baseball Simulation'!$H$2</definedName>
+    <definedName name="clBatter">'Baseball Simulation'!$F$7</definedName>
     <definedName name="clBCLastRow">Parameters!$B$7</definedName>
     <definedName name="clEntryLimit">Parameters!$B$5</definedName>
+    <definedName name="clEvent">'Baseball Simulation'!$F$11</definedName>
+    <definedName name="clEventDes">'Baseball Simulation'!#REF!</definedName>
+    <definedName name="clEventDesc">'Baseball Simulation'!$F$12</definedName>
+    <definedName name="clHomeScore">'Baseball Simulation'!$F$2</definedName>
     <definedName name="cLineUpURL">Parameters!$B$2</definedName>
+    <definedName name="clInning">'Baseball Simulation'!$F$4</definedName>
     <definedName name="clLastGameDataID">Parameters!$B$3</definedName>
     <definedName name="clLineupsCache">Parameters!$B$4</definedName>
     <definedName name="clMaxAvgWins">Parameters!$B$6</definedName>
     <definedName name="clMLBTeamsLocations">Parameters!#REF!</definedName>
+    <definedName name="clOut">'Baseball Simulation'!$F$13</definedName>
+    <definedName name="clPitch">'Baseball Simulation'!$F$5</definedName>
+    <definedName name="clPitcher">'Baseball Simulation'!$F$6</definedName>
     <definedName name="clPMLastRow">Parameters!$B$8</definedName>
     <definedName name="clUserWinsCache">Parameters!#REF!</definedName>
     <definedName name="cSalaryCap">Parameters!#REF!</definedName>
@@ -39,13 +53,13 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="871">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -2309,15 +2323,9 @@
     <t>Michal Neuvirth</t>
   </si>
   <si>
-    <t>Mikhail  Grigorenko</t>
-  </si>
-  <si>
     <t>Jason Demers</t>
   </si>
   <si>
-    <t>Jason Chimera</t>
-  </si>
-  <si>
     <t>Viktor Fasth</t>
   </si>
   <si>
@@ -2381,90 +2389,21 @@
     <t>Duncan Keith</t>
   </si>
   <si>
-    <t>Troy Grosenick</t>
-  </si>
-  <si>
-    <t>Erik Johnson</t>
-  </si>
-  <si>
-    <t>Jason LaBarbera</t>
-  </si>
-  <si>
-    <t>Calvin Pickard</t>
-  </si>
-  <si>
-    <t>Brad Winchester</t>
-  </si>
-  <si>
-    <t>Anthony Duclair</t>
-  </si>
-  <si>
-    <t>Anthony Peluso</t>
-  </si>
-  <si>
-    <t>Tim Jackman</t>
-  </si>
-  <si>
     <t>Barret Jackman</t>
   </si>
   <si>
-    <t>Ruslan Fedotenko</t>
-  </si>
-  <si>
-    <t>Martin Havlat</t>
-  </si>
-  <si>
     <t>Martin Marincin</t>
   </si>
   <si>
-    <t>Matt Tennyson</t>
-  </si>
-  <si>
-    <t>Matt Moulson</t>
-  </si>
-  <si>
     <t>Andrew Campbell</t>
   </si>
   <si>
-    <t>Jamie McGinn</t>
-  </si>
-  <si>
     <t>Tye McGinn</t>
   </si>
   <si>
-    <t>Ryane Clowe</t>
-  </si>
-  <si>
-    <t>Mike Weber</t>
-  </si>
-  <si>
-    <t>['MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL']</t>
-  </si>
-  <si>
-    <t>['CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI']</t>
-  </si>
-  <si>
     <t>Matthew Hackett</t>
   </si>
   <si>
-    <t>John Klingberg</t>
-  </si>
-  <si>
-    <t>['DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL']</t>
-  </si>
-  <si>
-    <t>Cody Eakin</t>
-  </si>
-  <si>
-    <t>['ANA', 'ANA', 'ANA', 'ANA', 'ANA', 'ANA', 'ANA']</t>
-  </si>
-  <si>
-    <t>['DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL']</t>
-  </si>
-  <si>
-    <t>['SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS']</t>
-  </si>
-  <si>
     <t>TeamOdds.py</t>
   </si>
   <si>
@@ -2480,45 +2419,30 @@
     <t>Columbus</t>
   </si>
   <si>
-    <t>[u'+137', u'-151']</t>
-  </si>
-  <si>
     <t>Detroit</t>
   </si>
   <si>
     <t>Minnesota</t>
   </si>
   <si>
-    <t>[u'+248', u'-280']</t>
-  </si>
-  <si>
     <t>Toronto</t>
   </si>
   <si>
     <t>Boston</t>
   </si>
   <si>
-    <t>[u'+216', u'-243']</t>
-  </si>
-  <si>
     <t>New Jersey</t>
   </si>
   <si>
     <t>NY Rangers</t>
   </si>
   <si>
-    <t>[u'+162', u'-180']</t>
-  </si>
-  <si>
     <t>Dallas</t>
   </si>
   <si>
     <t>Nashville</t>
   </si>
   <si>
-    <t>[u'-177', u'+160']</t>
-  </si>
-  <si>
     <t>Calgary</t>
   </si>
   <si>
@@ -2546,9 +2470,6 @@
     <t>Chicago</t>
   </si>
   <si>
-    <t>[u'+102', u'-113']</t>
-  </si>
-  <si>
     <t>Carolina</t>
   </si>
   <si>
@@ -2606,13 +2527,151 @@
     <t>[u'-200', u'+170']</t>
   </si>
   <si>
-    <t>{u'Dallas': 38.17, u'Minnesota': 60.16, u'Winnipeg': 53.49, u'Vancouver': 49.02, u'Calgary': 63.9, u'Carolina': 53.05, u'Columbus': 46.95, u'Arizona': 32.47, u'Tampa Bay': 55.75, u'Pittsburgh': 55.56, u'NY Islanders': 78.72, u'Nashville': 64.29, u'Los Angeles': 73.05, u'Toronto': 37.04, u'San Jose': 69.97, u'Florida': 46.73, u'Detroit': 42.19, u'Philadelphia': 49.5, u'Ottawa': 66.67, u'Buffalo': 23.7, u'St. Louis': 43.48, u'Colorado': 29.41, u'New Jersey': 31.65, u'Boston': 73.68, u'Edmonton': 38.46, u'Washington': 49.26, u'NY Rangers': 70.85, u'Chicago': 60.0}</t>
-  </si>
-  <si>
     <t>Vegas Odds</t>
   </si>
   <si>
     <t>Anaheim</t>
+  </si>
+  <si>
+    <t>{u'MIN': [['Zach Parise', 'Mikael Granlund', 'Jason Pominville'], ['Nino Niederreiter', 'Mikko Koivu', 'Chris Stewart'], ['Thomas Vanek', 'Charlie Coyle', 'Justin Fontaine'], ['Ryan Carter', 'Kyle Brodziak', 'Jordan Schroeder'], ['Ryan Suter', 'Jonas Brodin'], ['Marco Scandella', 'Jared Spurgeon'], ['Jordan Leopold', 'Mathew Dumba'], ['Zach Parise', 'Mikko Koivu', 'Jason Pominville', 'Ryan Suter', 'Mathew Dumba'], ['Thomas Vanek', 'Mikael Granlund', 'Chris Stewart', 'Marco Scandella', 'Jared Spurgeon']], u'TOR': [['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel'], ['Joakim Lindstrom', 'Nazem Kadri', 'Richard Panik'], ['Leo Komarov', 'Trevor Smith', 'Joffrey Lupul'], ['David Booth', 'Zach Sill', 'Casey Bailey'], ['Eric Brewer', 'Dion Phaneuf'], ['Jake Gardiner', 'Morgan Rielly'], ['Tim Erixon', 'T.J. Brennan'], ['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel', 'Morgan Rielly', 'Dion Phaneuf'], ['Joffrey Lupul', 'Nazem Kadri', 'Joakim Lindstrom', 'Jake Gardiner', 'T.J. Brennan']], u'WSH': [['Alex Ovechkin', 'Evgeny Kuznetsov', 'Joel Ward'], ['Marcus Johansson', 'Nicklas Backstrom', 'Troy Brouwer'], ['Curtis Glencross', 'Eric Fehr', 'Jason Chimera'], ['Brooks Laich', 'Michael Latta', 'Tom Wilson'], ['Brooks Orpik', 'John Carlson'], ['Karl Alzner', 'Matt Niskanen'], ['Tim Gleason', 'Mike Green'], ['Marcus Johansson', 'Nicklas Backstrom', 'Troy Brouwer', 'Alex Ovechkin', 'John Carlson'], ['Curtis Glencross', 'Evgeny Kuznetsov', 'Joel Ward', 'Matt Niskanen', 'Mike Green']], u'BOS': [['Brad Marchand', 'Patrice Bergeron', 'David Krejci'], ['Milan Lucic', 'Ryan Spooner', 'Brett Connolly'], ['Loui Eriksson', 'Carl Soderberg', 'Reilly Smith'], ['Chris Kelly', 'Gregory Campbell', 'David Pastrnak'], ['Zdeno Chara', 'Zach Trotman'], ['Torey Krug', 'Dennis Seidenberg'], ['Matt Bartkowski', 'Adam McQuaid'], ['Ryan Spooner', 'Patrice Bergeron', 'Loui Eriksson', 'Torey Krug', 'David Krejci'], ['Milan Lucic', 'Carl Soderberg', 'Brad Marchand', 'Zdeno Chara', 'Reilly Smith']], u'DET': [['Justin Abdelkader', 'Henrik Zetterberg', 'Gustav Nyquist'], ['Darren Helm', 'Pavel Datsyuk', 'Tomas Tatar'], ['Teemu Pulkkinen', 'Riley Sheahan', 'Stephen Weiss'], ['Drew Miller', 'Luke Glendening', 'Joakim Andersson'], ['Jonathan Ericsson', 'Niklas Kronwall'], ['Kyle Quincey', 'Dan DeKeyser'], ['Brendan Smith', 'Marek Zidlicky'], ['Gustav Nyquist', 'Henrik Zetterberg', 'Justin Abdelkader', 'Teemu Pulkkinen', 'Niklas Kronwall'], ['Tomas Tatar', 'Riley Sheahan', 'Stephen Weiss', 'Pavel Datsyuk', 'Marek Zidlicky']], u'NAS': [['Filip Forsberg', 'Mike Ribeiro', 'James Neal'], ['Colin Wilson', 'Mike Fisher', 'Craig Smith'], ['Viktor Stalberg', 'Matt Cullen', 'Mike Santorelli'], ['Gabriel Bourque', 'Calle Jarnkrok', 'Taylor Beck'], ['Roman Josi', 'Shea Weber'], ['Mattias Ekholm', 'Seth Jones'], ['Ryan Ellis', 'Cody Franson'], ['Colin Wilson', 'Mike Ribeiro', 'Craig Smith', 'Roman Josi', 'Shea Weber'], ['Filip Forsberg', 'Mike Fisher', 'James Neal', 'Seth Jones', 'Ryan Ellis']], u'NYI': [['Nikolay Kulemin', 'John Tavares', 'Ryan Strome'], ['Josh Bailey', 'Frans Nielsen', 'Kyle Okposo'], ['Anders Lee', 'Brock Nelson', 'Cal Clutterbuck'], ['Matt Martin', 'Casey Cizikas', 'Eric Boulton'], ['Nick Leddy', 'Johnny Boychuk'], ['Brian Strait', 'Travis Hamonic'], ['Thomas Hickey', 'Lubomir Visnovsky'], ['Anders Lee', 'John Tavares', 'Kyle Okposo', 'Nick Leddy', 'Frans Nielsen'], ['Josh Bailey', 'Brock Nelson', 'Ryan Strome', 'Lubomir Visnovsky', 'Johnny Boychuk']], u'FLA': [['Jonathan Huberdeau', 'Aleksander Barkov', 'Jaromir Jagr'], ['Brandon Pirri', 'Dave Bolland', 'Brad Boyes'], ['Jussi Jokinen', 'Vincent Trocheck', 'Jimmy Hayes'], ['Tomas Kopecky', 'Derek MacKenzie', 'Shawn Thornton'], ['Brian Campbell', 'Aaron Ekblad'], ['Willie Mitchell', 'Erik Gudbranson'], ['Dmitry Kulikov', 'Alex Petrovic'], ['Jimmy Hayes', 'Brandon Pirri', 'Brad Boyes', 'Brian Campbell', 'Jussi Jokinen'], ['Jonathan Huberdeau', 'Aleksander Barkov', 'Jaromir Jagr', 'Dmitry Kulikov', 'Aaron Ekblad']], u'COL': [['John Mitchell', 'Matt Duchene', 'Jarome Iginla'], ['Gabriel Landeskog', "Ryan O'Reilly", 'Alex Tanguay'], ['Cody McLeod', 'Marc-Andre Cliche', 'Dennis Everberg'], ['Jordan Caron', 'Freddie Hamilton', 'Joey Hishon'], ['Nate Guenin', 'Tyson Barrie'], ['Jan Hejda', 'Zach Redmond'], ['Brad Stuart', 'Nick Holden'], ['Gabriel Landeskog', "Ryan O'Reilly", 'Jarome Iginla', 'Alex Tanguay', 'Tyson Barrie'], ['John Mitchell', 'Matt Duchene', 'Joey Hishon', 'Zach Redmond', 'Nick Holden']], u'NJD': [['Reid Boucher', 'Scott Gomez', 'Steve Bernier'], ['Stefan Matteau', 'Travis Zajac', 'Michael Cammalleri'], ['Adam Henrique', 'Patrik Elias', 'Dainius Zubrus'], ['Tuomo Ruutu', 'Jacob Josefson', 'Jordin Tootoo'], ['Andy Greene', 'Adam Larsson'], ['Mark Fraser', 'Damon Severson'], ['Jon Merrill', 'Eric Gelinas'], ['Adam Henrique', 'Travis Zajac', 'Jordin Tootoo', 'Jacob Josefson', 'Damon Severson'], ['Michael Cammalleri', 'Patrik Elias', 'Steve Bernier', 'Jon Merrill', 'Eric Gelinas']], u'DAL': [['Jamie Benn', 'Cody Eakin', 'Tyler Seguin'], ['Patrick Eaves', 'Jason Spezza', 'Ales Hemsky'], ['Antoine Roussel', 'Vernon Fiddler', 'Ryan Garbutt'], ['Travis Moen', 'Colton Sceviour', 'Valeri Nichushkin'], ['Alex Goligoski', 'John Klingberg'], ['Patrik Nemeth', 'Trevor Daley'], ['Jordie Benn', 'Jason Demers'], ['Jamie Benn', 'Jason Spezza', 'Patrick Eaves', 'Tyler Seguin', 'John Klingberg'], ['Valeri Nichushkin', 'Colton Sceviour', 'Ales Hemsky', 'Trevor Daley', 'Alex Goligoski']], u'CGY': [['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler'], ['Lance Bouma', 'Mikael Backlund', 'David Jones'], ['Mason Raymond', 'Markus Granlund', 'Joe Colborne'], ['Brandon Bollig', 'Matt Stajan', 'Drew Shore'], ['Kris Russell', 'Dennis Wideman'], ['T.J. Brodie', 'Deryk Engelland'], ['David Schlemko', 'Corey Potter'], ['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler', 'Kris Russell', 'Dennis Wideman'], ['Mason Raymond', 'Mikael Backlund', 'Joe Colborne', 'T.J. Brodie', 'Corey Potter']], u'NYR': [['Rick Nash', 'Derick Brassard', 'Mats Zuccarello'], ['Chris Kreider', 'Derek Stepan', 'J.T. Miller'], ['Carl Hagelin', 'Kevin Hayes', 'Martin St. Louis'], ['Tanner Glass', 'Dominic Moore', 'Jesper Fast'], ['Ryan McDonagh', 'Dan Girardi'], ['Marc Staal', 'Dan Boyle'], ['Keith Yandle', 'Matt Hunwick'], ['Chris Kreider', 'Derek Stepan', 'Rick Nash', 'Martin St. Louis', 'Keith Yandle'], ['Kevin Hayes', 'Derick Brassard', 'Mats Zuccarello', 'Ryan McDonagh', 'Dan Boyle']], u'CAR': [['Eric Staal', 'Jordan Staal', 'Elias Lindholm'], ['Nathan Gerbe', 'Victor Rask', 'Chris Terry'], ['Jeff Skinner', 'Jay McClement', 'Alexander Semin'], ['Andrej Nestrasil', 'Brad Malone', 'Pat Dwyer'], ['Ron Hainsey', 'Justin Faulk'], ['John-Michael Liles', 'Ryan Murphy'], ['Michal Jordan', 'Danny Biega'], ['Andrej Nestrasil', 'Eric Staal', 'Elias Lindholm', 'Victor Rask', 'Justin Faulk'], ['Jeff Skinner', 'Jordan Staal', 'Chris Terry', 'John-Michael Liles', 'Ryan Murphy']], u'PIT': [['David Perron', 'Sidney Crosby', 'Patric Hornqvist'], ['Chris Kunitz', 'Evgeni Malkin', 'Blake Comeau'], ['Daniel Winnik', 'Brandon Sutter', 'Beau Bennett'], ['Nick Spaling', 'Maxim Lapierre', 'Craig Adams'], ['Paul Martin', 'Ben Lovejoy'], ['Rob Scuderi', 'Derrick Pouliot'], ['Ian Cole', 'Taylor Chorney'], ['Chris Kunitz', 'Sidney Crosby', 'Patric Hornqvist', 'Evgeni Malkin', 'Derrick Pouliot'], ['David Perron', 'Brandon Sutter', 'Blake Comeau', 'Paul Martin', 'Ian Cole']], u'VAN': [['Daniel Sedin', 'Henrik Sedin', 'Alexandre Burrows'], ['Chris Higgins', 'Nick Bonino', 'Radim Vrbata'], ['Shawn Matthias', 'Linden Vey', 'Derek Dorsett'], ['Ronalds Kenins', 'Bo Horvat', 'Jannik Hansen'], ['Alexander Edler', 'Chris Tanev'], ['Dan Hamhuis', 'Yannick Weber'], ['Kevin Bieksa', 'Luca Sbisa'], ['Daniel Sedin', 'Henrik Sedin', 'Radim Vrbata', 'Alexander Edler', 'Yannick Weber'], ['Chris Higgins', 'Nick Bonino', 'Alexandre Burrows', 'Dan Hamhuis', 'Chris Tanev']], u'STL': [['Jaden Schwartz', 'Paul Stastny', 'T.J. Oshie'], ['Dmitrij Jaskin', 'David Backes', 'Patrik Berglund'], ['Olli Jokinen', 'Jori Lehtera', 'Ty Rattie'], ['Steve Ott', 'Marcel Goc', 'Ryan Reaves'], ['Jay Bouwmeester', 'Alex Pietrangelo'], ['Zbynek Michalek', 'Kevin Shattenkirk'], ['Barret Jackman', 'Robert Bortuzzo'], ['Jaden Schwartz', 'David Backes', 'T.J. Oshie', 'Paul Stastny', 'Kevin Shattenkirk'], ['Dmitrij Jaskin', 'Jori Lehtera', 'Patrik Berglund', 'Jay Bouwmeester', 'Alex Pietrangelo']], u'CHI': [['Kris Versteeg', 'Jonathan Toews', 'Marian Hossa'], ['Patrick Sharp', 'Brad Richards', 'Antoine Vermette'], ['Bryan Bickell', 'Andrew Shaw', 'Brandon Saad'], ['Andrew Desjardins', 'Marcus Kruger', 'Teuvo Teravainen'], ['Kimmo Timonen', 'Brent Seabrook'], ['Duncan Keith', 'Michal Rozsival'], ['Johnny Oduya', 'Niklas Hjalmarsson'], ['Andrew Shaw', 'Jonathan Toews', 'Brandon Saad', 'Duncan Keith', 'Marian Hossa'], ['Teuvo Teravainen', 'Brad Richards', 'Kris Versteeg', 'Patrick Sharp', 'Brent Seabrook']], u'SJS': [['Joe Pavelski', 'Joe Thornton', 'Melker Karlsson'], ['Patrick Marleau', 'Logan Couture', 'Tomas Hertl'], ['Matthew Nieto', 'Chris Tierney', 'Tommy Wingels'], ['Mike Brown', 'Ben Smith', 'Barclay Goodrow'], ['Matt Irwin', 'Brent Burns'], ['Brenden Dillon', 'Justin Braun'], ['Karl Stollery', 'Taylor Fedun'], ['Patrick Marleau', 'Joe Thornton', 'Logan Couture', 'Joe Pavelski', 'Brent Burns'], ['Melker Karlsson', 'Chris Tierney', 'Tomas Hertl', 'Matt Irwin', 'Taylor Fedun']], u'MTL': [['Max Pacioretty', 'Tomas Plekanec', 'Brendan Gallagher'], ['Alex Galchenyuk', 'David Desharnais', 'P.A. Parenteau'], ['Brandon Prust', 'Lars Eller', 'Dale Weise'], ['Jacob De La Rose', 'Torrey Mitchell', 'Devante Smith-Pelly'], ['Alexei Emelin', 'P.K. Subban'], ['Nathan Beaulieu', 'Jeff Petry'], ['Sergei Gonchar', 'Tom Gilbert'], ['Max Pacioretty', 'David Desharnais', 'P.A. Parenteau', 'Nathan Beaulieu', 'P.K. Subban'], ['Alex Galchenyuk', 'Tomas Plekanec', 'Brendan Gallagher', 'Sergei Gonchar', 'Jeff Petry']], u'PHI': [['Michael Raffl', 'Claude Giroux', 'Jakub Voracek'], ['Brayden Schenn', 'Sean Couturier', 'Matt Read'], ['Zac Rinaldo', 'Nick Cousins', 'Ryan White'], ['Chris VandeVelde', 'Vincent Lecavalier'], ['Nicklas Grossmann', 'Mark Streit'], ['Michael Del Zotto', 'Nick Schultz'], ['Carlo Colaiacovo', 'Brandon Manning'], ['Brayden Schenn', 'Claude Giroux', 'Ryan White', 'Jakub Voracek', 'Mark Streit'], ['Michael Raffl', 'Sean Couturier', 'Matt Read', 'Michael Del Zotto', 'Vincent Lecavalier']], u'ANA': [['Tomas Fleischmann', 'Ryan Kesler', 'Kyle Palmieri'], ['Jiri Sekac', 'Rickard Rakell', 'Corey Perry'], ['Andrew Cogliano', 'Nate Thompson', 'Jakob Silfverberg'], ['Stefan Noesen', 'Chris Wagner', 'Emerson Etem'], ['Hampus Lindholm', 'Francois Beauchemin'], ['Cam Fowler', 'Sami Vatanen'], ['Simon Despres', 'James Wisniewski'], ['Tomas Fleischmann', 'Ryan Kesler', 'Kyle Palmieri', 'Francois Beauchemin', 'Sami Vatanen'], ['Jiri Sekac', 'Rickard Rakell', 'Corey Perry', 'Cam Fowler', 'James Wisniewski']], u'LAK': [['Marian Gaborik', 'Anze Kopitar', 'Justin Williams'], ['Dwight King', 'Jeff Carter', 'Tyler Toffoli'], ['Trevor Lewis', 'Jarret Stoll', 'Dustin Brown'], ['Kyle Clifford', 'Nick Shore', 'Jordan Nolan'], ['Jake Muzzin', 'Drew Doughty'], ['Alec Martinez', 'Robyn Regehr'], ['Brayden McNabb', 'Matt Greene'], ['Marian Gaborik', 'Anze Kopitar', 'Jeff Carter', 'Jake Muzzin', 'Drew Doughty'], ['Dustin Brown', 'Tyler Toffoli', 'Justin Williams', 'Brayden McNabb', 'Alec Martinez']], u'CBJ': [['Boone Jenner', 'Ryan Johansen', 'Cam Atkinson'], ['Brandon Dubinsky', 'Artem Anisimov', 'Nick Foligno'], ['Scott Hartnell', 'Alexander Wennberg', 'Marko Dano'], ['Matt Calvert', 'Mark Letestu', 'Jeremy Morin'], ['Jack Johnson', 'David Savard'], ['Fedor Tyutin', 'Dalton Prout'], ['Kevin Connauton', 'Cody Goloubef'], ['Scott Hartnell', 'Ryan Johansen', 'Nick Foligno', 'Kevin Connauton', 'Alexander Wennberg'], ['Boone Jenner', 'Brandon Dubinsky', 'Cam Atkinson', 'Jack Johnson', 'David Savard']], u'BUF': [['Matt Moulson', 'Johan Larsson', 'Tyler Ennis'], ['Marcus Foligno', 'Mikhail  Grigorenko', 'Brian Gionta'], ['Nicolas Deslauriers', 'Phil Varone', 'Patrick Kaleta'], ['Cody Hodgson', 'Matt Ellis', 'Zac Dalpe'], ['Zach Bogosian', 'Rasmus Ristolainen'], ['Andrej Meszaros', 'Tyson Strachan'], ['Andre Benoit', 'Nikita Zadorov'], ['Matt Moulson', 'Johan Larsson', 'Brian Gionta', 'Tyler Ennis', 'Rasmus Ristolainen'], ['Marcus Foligno', 'Mikhail  Grigorenko', 'Cody Hodgson', 'Zach Bogosian', 'Andrej Meszaros']], u'EDM': [['Benoit Pouliot', 'Ryan Nugent-Hopkins', 'Jordan Eberle'], ['Teddy Purcell', 'Derek Roy', 'Nail Yakupov'], ['Taylor Hall', 'Anton Lander', 'Andrew Miller'], ['Luke Gazdic', 'Rob Klinkhammer', 'Matt Fraser'], ['Oscar Klefbom', 'Justin Schultz'], ['Martin Marincin', 'David Musil'], ['Brandon Davidson', 'Keith Aulie'], ['Teddy Purcell', 'Ryan Nugent-Hopkins', 'Anton Lander', 'Jordan Eberle', 'Justin Schultz'], ['Taylor Hall', 'Derek Roy', 'Benoit Pouliot', 'Oscar Klefbom', 'Nail Yakupov']], u'TBL': [['Alex Killorn', 'Steven Stamkos', 'Ryan Callahan'], ['Ondrej Palat', 'Tyler Johnson', 'Nikita Kucherov'], ['Vladislav Namestnikov', 'Valtteri Filppula', 'Cedric Paquette'], ['Jonathan Drouin', 'Brian Boyle', 'J.T. Brown'], ['Nikita Nesterov', 'Anton Stralman'], ['Matt Carle', 'Slater Koekkoek'], ['Mark Barberio', 'Luke Witkowski'], ['Jonathan Drouin', 'Steven Stamkos', 'Ondrej Palat', 'Valtteri Filppula', 'Anton Stralman'], ['Vladislav Namestnikov', 'Tyler Johnson', 'Ryan Callahan', 'Nikita Nesterov', 'Nikita Kucherov']], u'WIN': [['Andrew Ladd', 'Bryan Little', 'Michael Frolik'], ['Drew Stafford', 'Mark Scheifele', 'Blake Wheeler'], ['Mathieu Perreault', 'Adam Lowry', 'Lee Stempniak'], ['Jiri Tlusty', 'Jim Slater', 'Chris Thorburn'], ['Tobias Enstrom', 'Tyler Myers'], ['Mark Stuart', 'Jacob Trouba'], ['Adam Pardy', 'Jay Harrison'], ['Andrew Ladd', 'Bryan Little', 'Blake Wheeler', 'Mathieu Perreault', 'Tyler Myers'], ['Drew Stafford', 'Mark Scheifele', 'Michael Frolik', 'Tobias Enstrom', 'Jacob Trouba']], u'ARI': [['Tobias Rieder', 'Mark Arcobello', 'Shane Doan'], ['Martin Erat', 'Sam Gagner', 'David Moss'], ['Craig Cunningham', 'Kyle Chipchura', 'Jordan Szwarz'], ['Tye McGinn', 'Joe Vitale', 'B.J. Crombeen'], ['Oliver Ekman-Larsson', 'Michael Stone'], ['Klas Dahlbeck', 'Connor Murphy'], ['Andrew Campbell', 'John Moore'], ['Tobias Rieder', 'Sam Gagner', 'Shane Doan', 'John Moore', 'Oliver Ekman-Larsson'], ['Martin Erat', 'Mark Arcobello', 'David Moss', 'Michael Stone', 'Connor Murphy']], u'OTT': [['Zack Smith', 'Mika Zibanejad', 'Bobby Ryan'], ['Clarke MacArthur', 'Kyle Turris', 'Mark Stone'], ['Erik Condra', 'Jean-Gabriel Pageau', 'Curtis Lazar'], ['Mike Hoffman', 'David Legwand', 'Alex Chiasson'], ['Marc Methot', 'Erik Karlsson'], ['Patrick Wiercioch', 'Cody Ceci'], ['Mark Borowiecki', 'Eric Gryba'], ['David Legwand', 'Mika Zibanejad', 'Bobby Ryan', 'Patrick Wiercioch', 'Erik Karlsson'], ['Clarke MacArthur', 'Kyle Turris', 'Mark Stone', 'Mike Hoffman', 'Cody Ceci']]}</t>
+  </si>
+  <si>
+    <t>David Musil</t>
+  </si>
+  <si>
+    <t>Todd Bertuzzi</t>
+  </si>
+  <si>
+    <t>Chris Neil</t>
+  </si>
+  <si>
+    <t>Robin Lehner</t>
+  </si>
+  <si>
+    <t>Jay Beagle</t>
+  </si>
+  <si>
+    <t>Nathan Horton</t>
+  </si>
+  <si>
+    <t>Jonathan Drouin</t>
+  </si>
+  <si>
+    <t>Jonas Gustavsson</t>
+  </si>
+  <si>
+    <t>Dmitry Kulikov</t>
+  </si>
+  <si>
+    <t>Andre Burakovsky</t>
+  </si>
+  <si>
+    <t>Bobby Butler</t>
+  </si>
+  <si>
+    <t>Andy Greene</t>
+  </si>
+  <si>
+    <t>Philipp Grubauer</t>
+  </si>
+  <si>
+    <t>Philip Varone</t>
+  </si>
+  <si>
+    <t>[u'+106', u'-117']</t>
+  </si>
+  <si>
+    <t>[u'-165', u'+149']</t>
+  </si>
+  <si>
+    <t>[u'+143', u'-158']</t>
+  </si>
+  <si>
+    <t>[u'+132', u'-146']</t>
+  </si>
+  <si>
+    <t>[u'-129', u'+117']</t>
+  </si>
+  <si>
+    <t>[u'-127', u'+115']</t>
+  </si>
+  <si>
+    <t>[u'+191', u'-213']</t>
+  </si>
+  <si>
+    <t>{u'PHI': 46.08, u'STL': 43.48, u'CHI': 60.0, u'MIN': 61.24, u'TOR': 37.04, u'WSH': 48.54, u'LAK': 55.56, u'DET': 53.92, u'OTT': 66.67, u'SJS': 59.35, u'WIN': 41.15, u'NYR': 68.05, u'DAL': 43.1, u'MTL': 55.95, u'CAR': 62.26, u'FLA': 46.51, u'VAN': 46.95, u'BUF': 40.16, u'CBJ': 34.36, u'PIT': 56.33}</t>
+  </si>
+  <si>
+    <t>['OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT']</t>
+  </si>
+  <si>
+    <t>['FLA', 'FLA', 'FLA', 'FLA', 'FLA', 'FLA', 'FLA', 'FLA']</t>
+  </si>
+  <si>
+    <t>['WSH', 'WSH', 'WSH', 'WSH', 'WSH', 'WSH', 'WSH']</t>
+  </si>
+  <si>
+    <t>John Carlson</t>
+  </si>
+  <si>
+    <t>['CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI']</t>
+  </si>
+  <si>
+    <t>['MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL']</t>
+  </si>
+  <si>
+    <t>['OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT']</t>
+  </si>
+  <si>
+    <t>BBSim.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Cole\Desktop\FanDuel\fanduel\modules\BBSim.py</t>
+  </si>
+  <si>
+    <t>script_name_5</t>
+  </si>
+  <si>
+    <t>script_path_5</t>
+  </si>
+  <si>
+    <t>Home Score:</t>
+  </si>
+  <si>
+    <t>Away Score:</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>Pitcher</t>
+  </si>
+  <si>
+    <t>Batter</t>
+  </si>
+  <si>
+    <t>Event:</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>Called Strike</t>
+  </si>
+  <si>
+    <t>Outs</t>
+  </si>
+  <si>
+    <t>Inning</t>
+  </si>
+  <si>
+    <t>Event Description</t>
   </si>
 </sst>
 </file>
@@ -3283,11 +3342,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245598464"/>
-        <c:axId val="245604352"/>
+        <c:axId val="233474304"/>
+        <c:axId val="233480192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245598464"/>
+        <c:axId val="233474304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,7 +3355,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245604352"/>
+        <c:crossAx val="233480192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245604352"/>
+        <c:axId val="233480192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,7 +3374,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245598464"/>
+        <c:crossAx val="233474304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3428,11 +3487,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="246226304"/>
-        <c:axId val="246232192"/>
+        <c:axId val="228855168"/>
+        <c:axId val="228861056"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="246226304"/>
+        <c:axId val="228855168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3441,7 +3500,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246232192"/>
+        <c:crossAx val="228861056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3449,7 +3508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246232192"/>
+        <c:axId val="228861056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3460,7 +3519,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246226304"/>
+        <c:crossAx val="228855168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4103,7 +4162,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4111,7 +4170,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4119,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4127,7 +4186,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>806</v>
+        <v>854</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4135,7 +4194,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>807</v>
+        <v>855</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4143,7 +4202,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>455</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4151,7 +4210,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>456</v>
+        <v>782</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4159,7 +4218,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4167,7 +4226,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4175,7 +4234,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4183,7 +4242,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4191,7 +4250,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4199,6 +4258,22 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>856</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>857</v>
+      </c>
+      <c r="B15" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4389,13 +4464,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B1" t="s">
-        <v>810</v>
+        <v>786</v>
       </c>
       <c r="C1" t="s">
-        <v>808</v>
+        <v>839</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4403,189 +4478,189 @@
         <v>812</v>
       </c>
       <c r="B2" t="s">
-        <v>813</v>
+        <v>788</v>
       </c>
       <c r="C2" t="s">
-        <v>811</v>
+        <v>821</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
       <c r="B3" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="C3" t="s">
-        <v>814</v>
+        <v>840</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>818</v>
+        <v>806</v>
       </c>
       <c r="B4" t="s">
-        <v>819</v>
+        <v>787</v>
       </c>
       <c r="C4" t="s">
-        <v>817</v>
+        <v>841</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>821</v>
+        <v>792</v>
       </c>
       <c r="B5" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="C5" t="s">
-        <v>820</v>
+        <v>842</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>824</v>
+        <v>784</v>
       </c>
       <c r="B6" t="s">
-        <v>825</v>
+        <v>797</v>
       </c>
       <c r="C6" t="s">
-        <v>823</v>
+        <v>843</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>809</v>
+        <v>798</v>
       </c>
       <c r="B7" t="s">
-        <v>827</v>
+        <v>799</v>
       </c>
       <c r="C7" t="s">
-        <v>826</v>
+        <v>844</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>828</v>
+        <v>801</v>
       </c>
       <c r="B8" t="s">
-        <v>829</v>
+        <v>802</v>
       </c>
       <c r="C8" t="s">
-        <v>826</v>
+        <v>800</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>831</v>
+        <v>785</v>
       </c>
       <c r="B9" t="s">
-        <v>832</v>
+        <v>791</v>
       </c>
       <c r="C9" t="s">
-        <v>830</v>
+        <v>845</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="B10" t="s">
-        <v>834</v>
+        <v>805</v>
       </c>
       <c r="C10" t="s">
-        <v>833</v>
+        <v>783</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
       <c r="B11" t="s">
-        <v>837</v>
+        <v>806</v>
       </c>
       <c r="C11" t="s">
-        <v>835</v>
+        <v>804</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>839</v>
+        <v>808</v>
       </c>
       <c r="B12" t="s">
-        <v>840</v>
+        <v>809</v>
       </c>
       <c r="C12" t="s">
-        <v>838</v>
+        <v>807</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
       <c r="B13" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="C13" t="s">
-        <v>841</v>
+        <v>810</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>845</v>
+        <v>814</v>
       </c>
       <c r="B14" t="s">
-        <v>829</v>
+        <v>799</v>
       </c>
       <c r="C14" t="s">
-        <v>844</v>
+        <v>813</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>847</v>
+        <v>816</v>
       </c>
       <c r="B15" t="s">
-        <v>848</v>
+        <v>817</v>
       </c>
       <c r="C15" t="s">
+        <v>815</v>
+      </c>
+      <c r="E15" t="s">
         <v>846</v>
-      </c>
-      <c r="E15" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>850</v>
+        <v>819</v>
       </c>
       <c r="B16" t="s">
-        <v>851</v>
+        <v>820</v>
       </c>
       <c r="C16" t="s">
-        <v>849</v>
+        <v>818</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
       <c r="B17" t="s">
-        <v>812</v>
+        <v>786</v>
       </c>
       <c r="C17" t="s">
-        <v>826</v>
+        <v>796</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="B18" t="s">
-        <v>815</v>
+        <v>788</v>
       </c>
       <c r="C18" t="s">
-        <v>852</v>
+        <v>821</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8141,6 +8216,107 @@
     <row r="729" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B729">
         <v>3100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>858</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>859</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>861</v>
+      </c>
+      <c r="F6">
+        <v>572020</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>862</v>
+      </c>
+      <c r="F7">
+        <v>543068</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>863</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>870</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>868</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8153,9 +8329,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8772,7 +8946,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -8809,7 +8983,9 @@
       <c r="A4" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -8899,7 +9075,7 @@
         <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>854</v>
+        <v>822</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8910,7 +9086,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>855</v>
+        <v>823</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8921,7 +9097,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>837</v>
+        <v>806</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -8932,7 +9108,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>816</v>
+        <v>789</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -8943,7 +9119,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>839</v>
+        <v>808</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -8954,7 +9130,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>824</v>
+        <v>794</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -8965,7 +9141,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>834</v>
+        <v>803</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -8976,7 +9152,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>832</v>
+        <v>802</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -8987,7 +9163,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>850</v>
+        <v>819</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -8998,7 +9174,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>810</v>
+        <v>785</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -9009,7 +9185,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>821</v>
+        <v>792</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -9020,7 +9196,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>812</v>
+        <v>786</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -9031,7 +9207,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>825</v>
+        <v>795</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -9042,7 +9218,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>829</v>
+        <v>799</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -9053,7 +9229,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>851</v>
+        <v>820</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -9064,7 +9240,7 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>813</v>
+        <v>787</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9075,7 +9251,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>828</v>
+        <v>798</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -9086,7 +9262,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>822</v>
+        <v>793</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -9097,7 +9273,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>818</v>
+        <v>790</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -9108,7 +9284,7 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>840</v>
+        <v>809</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -9119,7 +9295,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>819</v>
+        <v>791</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -9130,7 +9306,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -9141,7 +9317,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>827</v>
+        <v>797</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -9152,7 +9328,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>848</v>
+        <v>817</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -9163,7 +9339,7 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>809</v>
+        <v>784</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -9174,7 +9350,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>847</v>
+        <v>816</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -9185,7 +9361,7 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>831</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -9196,7 +9372,7 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>845</v>
+        <v>814</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9207,7 +9383,7 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>815</v>
+        <v>788</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -9218,7 +9394,7 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -9229,7 +9405,7 @@
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
     </row>
   </sheetData>
@@ -9260,7 +9436,7 @@
     <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>778</v>
+        <v>826</v>
       </c>
       <c r="B2" t="s">
         <v>544</v>
@@ -9295,42 +9471,42 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>767</v>
+        <v>827</v>
       </c>
       <c r="B3" t="s">
-        <v>768</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>769</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>558</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>559</v>
+        <v>725</v>
       </c>
       <c r="F3" t="s">
-        <v>560</v>
+        <v>467</v>
       </c>
       <c r="G3" t="s">
-        <v>237</v>
+        <v>471</v>
       </c>
       <c r="H3" t="s">
-        <v>561</v>
+        <v>468</v>
       </c>
       <c r="I3" t="s">
-        <v>562</v>
+        <v>472</v>
       </c>
       <c r="J3" t="s">
-        <v>272</v>
+        <v>213</v>
       </c>
       <c r="K3" t="s">
-        <v>474</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="B4" t="s">
         <v>223</v>
@@ -9365,13 +9541,13 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>828</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>722</v>
       </c>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>543</v>
       </c>
       <c r="D5" t="s">
         <v>503</v>
@@ -9430,13 +9606,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>779</v>
+        <v>759</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>462</v>
       </c>
       <c r="C6" t="s">
-        <v>503</v>
+        <v>423</v>
       </c>
       <c r="D6" t="s">
         <v>758</v>
@@ -9465,51 +9641,51 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>766</v>
       </c>
       <c r="C7" t="s">
-        <v>423</v>
+        <v>767</v>
       </c>
       <c r="D7" t="s">
-        <v>760</v>
+        <v>558</v>
       </c>
       <c r="E7" t="s">
-        <v>256</v>
+        <v>559</v>
       </c>
       <c r="F7" t="s">
-        <v>420</v>
+        <v>560</v>
       </c>
       <c r="G7" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
-        <v>258</v>
+        <v>561</v>
       </c>
       <c r="I7" t="s">
-        <v>260</v>
+        <v>562</v>
       </c>
       <c r="J7" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="K7" t="s">
-        <v>179</v>
+        <v>474</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>780</v>
+        <v>829</v>
       </c>
       <c r="B8" t="s">
-        <v>756</v>
+        <v>734</v>
       </c>
       <c r="C8" t="s">
         <v>254</v>
       </c>
       <c r="D8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E8" t="s">
         <v>463</v>
@@ -9532,16 +9708,16 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>716</v>
       </c>
       <c r="B9" t="s">
-        <v>756</v>
+        <v>669</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>640</v>
       </c>
       <c r="D9" t="s">
-        <v>760</v>
+        <v>419</v>
       </c>
       <c r="E9" t="s">
         <v>269</v>
@@ -9567,13 +9743,13 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="B10" t="s">
-        <v>763</v>
+        <v>521</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>769</v>
       </c>
       <c r="D10" t="s">
         <v>75</v>
@@ -9602,13 +9778,13 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
       <c r="B11" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C11" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D11" t="s">
         <v>475</v>
@@ -9637,13 +9813,13 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>782</v>
+        <v>485</v>
       </c>
       <c r="B12" t="s">
-        <v>255</v>
+        <v>486</v>
       </c>
       <c r="C12" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="D12" t="s">
         <v>183</v>
@@ -9672,22 +9848,22 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>783</v>
+        <v>830</v>
       </c>
       <c r="B13" t="s">
-        <v>784</v>
+        <v>723</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>831</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
-        <v>269</v>
+        <v>185</v>
       </c>
       <c r="F13" t="s">
-        <v>270</v>
+        <v>186</v>
       </c>
       <c r="G13" t="s">
         <v>219</v>
@@ -9707,10 +9883,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>785</v>
+        <v>530</v>
       </c>
       <c r="B14" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
       <c r="C14" t="s">
         <v>190</v>
@@ -9742,13 +9918,13 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>787</v>
+        <v>832</v>
       </c>
       <c r="B15" t="s">
-        <v>786</v>
+        <v>669</v>
       </c>
       <c r="C15" t="s">
-        <v>733</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
         <v>183</v>
@@ -9777,16 +9953,16 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>490</v>
+        <v>524</v>
       </c>
       <c r="B16" t="s">
-        <v>788</v>
+        <v>833</v>
       </c>
       <c r="C16" t="s">
         <v>423</v>
       </c>
       <c r="D16" t="s">
-        <v>789</v>
+        <v>777</v>
       </c>
       <c r="E16" t="s">
         <v>462</v>
@@ -9812,7 +9988,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>549</v>
+        <v>771</v>
       </c>
       <c r="B17" t="s">
         <v>218</v>
@@ -9847,22 +10023,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>790</v>
+        <v>834</v>
       </c>
       <c r="B18" t="s">
-        <v>791</v>
+        <v>502</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>752</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>504</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>478</v>
       </c>
       <c r="G18" t="s">
         <v>219</v>
@@ -9882,13 +10058,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B19" t="s">
         <v>526</v>
       </c>
       <c r="C19" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="D19" t="s">
         <v>241</v>
@@ -9917,13 +10093,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>529</v>
+        <v>242</v>
       </c>
       <c r="B20" t="s">
         <v>526</v>
       </c>
       <c r="C20" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="D20" t="s">
         <v>241</v>
@@ -9952,10 +10128,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>793</v>
+        <v>686</v>
       </c>
       <c r="B21" t="s">
-        <v>794</v>
+        <v>779</v>
       </c>
       <c r="C21" t="s">
         <v>500</v>
@@ -9987,22 +10163,22 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>795</v>
+        <v>549</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>489</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>217</v>
+        <v>69</v>
       </c>
       <c r="F22" t="s">
-        <v>459</v>
+        <v>197</v>
       </c>
       <c r="G22" t="s">
         <v>219</v>
@@ -10022,7 +10198,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>706</v>
+        <v>835</v>
       </c>
       <c r="B23" t="s">
         <v>214</v>
@@ -10057,22 +10233,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>518</v>
+        <v>273</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>274</v>
       </c>
       <c r="C24" t="s">
-        <v>519</v>
+        <v>275</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>276</v>
       </c>
       <c r="E24" t="s">
-        <v>421</v>
+        <v>277</v>
       </c>
       <c r="F24" t="s">
-        <v>457</v>
+        <v>278</v>
       </c>
       <c r="G24" t="s">
         <v>240</v>
@@ -10080,10 +10256,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>510</v>
       </c>
       <c r="C25" t="s">
         <v>519</v>
@@ -10115,13 +10291,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>485</v>
+        <v>707</v>
       </c>
       <c r="B26" t="s">
-        <v>486</v>
+        <v>703</v>
       </c>
       <c r="C26" t="s">
-        <v>259</v>
+        <v>836</v>
       </c>
       <c r="D26" t="s">
         <v>113</v>
@@ -10150,16 +10326,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>509</v>
+        <v>837</v>
       </c>
       <c r="B27" t="s">
-        <v>510</v>
+        <v>838</v>
       </c>
       <c r="C27" t="s">
-        <v>259</v>
+        <v>733</v>
       </c>
       <c r="D27" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E27" t="s">
         <v>256</v>
@@ -10185,37 +10361,37 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>460</v>
+        <v>528</v>
       </c>
       <c r="B28" t="s">
-        <v>796</v>
+        <v>725</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>467</v>
       </c>
       <c r="D28" t="s">
-        <v>282</v>
+        <v>476</v>
       </c>
       <c r="E28" t="s">
-        <v>264</v>
+        <v>468</v>
       </c>
       <c r="F28" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="G28" t="s">
-        <v>703</v>
+        <v>189</v>
       </c>
       <c r="H28" t="s">
-        <v>556</v>
+        <v>190</v>
       </c>
       <c r="I28" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="J28" t="s">
-        <v>180</v>
+        <v>257</v>
       </c>
       <c r="K28" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -10360,13 +10536,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B33" t="s">
         <v>521</v>
       </c>
       <c r="C33" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D33" t="s">
         <v>752</v>
@@ -10395,13 +10571,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B34" t="s">
         <v>521</v>
       </c>
       <c r="C34" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D34" t="s">
         <v>476</v>
@@ -10436,7 +10612,7 @@
         <v>272</v>
       </c>
       <c r="C35" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D35" t="s">
         <v>218</v>
@@ -10506,7 +10682,7 @@
         <v>521</v>
       </c>
       <c r="C37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D37" t="s">
         <v>216</v>
@@ -10535,7 +10711,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>799</v>
+        <v>780</v>
       </c>
       <c r="B38" t="s">
         <v>243</v>
@@ -10570,7 +10746,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B39" t="s">
         <v>493</v>
@@ -10666,7 +10842,7 @@
         <v>557</v>
       </c>
       <c r="B42" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C42" t="s">
         <v>269</v>
@@ -10698,13 +10874,13 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>765</v>
+      </c>
+      <c r="B43" t="s">
+        <v>766</v>
+      </c>
+      <c r="C43" t="s">
         <v>767</v>
-      </c>
-      <c r="B43" t="s">
-        <v>768</v>
-      </c>
-      <c r="C43" t="s">
-        <v>769</v>
       </c>
       <c r="D43" t="s">
         <v>558</v>
@@ -10861,19 +11037,19 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B48" t="s">
         <v>521</v>
       </c>
       <c r="C48" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D48" t="s">
         <v>571</v>
       </c>
       <c r="E48" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F48" t="s">
         <v>624</v>
@@ -10896,7 +11072,7 @@
         <v>565</v>
       </c>
       <c r="B49" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C49" t="s">
         <v>223</v>
@@ -11001,10 +11177,10 @@
         <v>523</v>
       </c>
       <c r="B52" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C52" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D52" t="s">
         <v>558</v>
@@ -11033,7 +11209,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B53" t="s">
         <v>462</v>
@@ -11161,7 +11337,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B57" t="s">
         <v>726</v>
@@ -11196,7 +11372,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B58" t="s">
         <v>498</v>
@@ -11251,16 +11427,16 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B60" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C60" t="s">
         <v>735</v>
       </c>
       <c r="D60" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E60" t="s">
         <v>239</v>
@@ -11367,7 +11543,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B64" t="s">
         <v>214</v>
@@ -11494,7 +11670,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B69" t="s">
         <v>726</v>
@@ -11514,7 +11690,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B70" t="s">
         <v>498</v>
@@ -11580,16 +11756,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B73" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C73" t="s">
         <v>735</v>
       </c>
       <c r="D73" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E73" t="s">
         <v>277</v>
@@ -13731,7 +13907,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -13742,7 +13918,7 @@
         <v>505</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>754</v>
+        <v>825</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -15881,7 +16057,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15910,155 +16086,155 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>650</v>
       </c>
       <c r="B2" t="s">
-        <v>803</v>
+        <v>852</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D2" s="9">
-        <v>-1188.9992594600001</v>
+        <v>426.65625</v>
       </c>
       <c r="E2">
-        <v>7700</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>802</v>
+        <v>422</v>
       </c>
       <c r="B3" t="s">
-        <v>804</v>
+        <v>847</v>
       </c>
       <c r="C3" t="s">
         <v>159</v>
       </c>
       <c r="D3" s="9">
-        <v>392.62666666699999</v>
+        <v>435.796875</v>
       </c>
       <c r="E3">
-        <v>4500</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>615</v>
+        <v>692</v>
       </c>
       <c r="B4" t="s">
-        <v>804</v>
+        <v>853</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D4" s="9">
-        <v>436.62666666699999</v>
+        <v>-1080.16961528</v>
       </c>
       <c r="E4">
-        <v>8500</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>651</v>
+        <v>478</v>
       </c>
       <c r="B5" t="s">
-        <v>797</v>
+        <v>848</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="9">
-        <v>388.24517906300002</v>
+        <v>430.875</v>
       </c>
       <c r="E5">
-        <v>5700</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="B6" t="s">
-        <v>797</v>
+        <v>849</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D6" s="9">
-        <v>446.04683195600001</v>
+        <v>627.299319728</v>
       </c>
       <c r="E6">
-        <v>5600</v>
+        <v>9800</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>650</v>
+        <v>589</v>
       </c>
       <c r="B7" t="s">
-        <v>797</v>
+        <v>849</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D7" s="9">
-        <v>458.50964187300002</v>
+        <v>470.68027210899999</v>
       </c>
       <c r="E7">
-        <v>9300</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>777</v>
+        <v>850</v>
       </c>
       <c r="B8" t="s">
-        <v>798</v>
+        <v>849</v>
       </c>
       <c r="C8" t="s">
         <v>160</v>
       </c>
       <c r="D8" s="9">
-        <v>486</v>
+        <v>401.95918367299998</v>
       </c>
       <c r="E8">
-        <v>5300</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>514</v>
+        <v>587</v>
       </c>
       <c r="B9" t="s">
-        <v>805</v>
+        <v>849</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="9">
-        <v>279.89999999999998</v>
+        <v>482.05442176899999</v>
       </c>
       <c r="E9">
-        <v>3800</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>800</v>
+        <v>775</v>
       </c>
       <c r="B10" t="s">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C10" t="s">
         <v>160</v>
       </c>
       <c r="D10" s="9">
-        <v>456.583809524</v>
+        <v>499.49387755100003</v>
       </c>
       <c r="E10">
-        <v>4500</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated excel workbook with BBSim sheet
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="10320" windowHeight="9900" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="10320" windowHeight="9900" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -18,18 +18,32 @@
     <sheet name="Best Contests" sheetId="12" r:id="rId9"/>
     <sheet name="Performance Monitoring" sheetId="13" r:id="rId10"/>
     <sheet name="Output" sheetId="17" r:id="rId11"/>
+    <sheet name="Baseball Simulation" sheetId="18" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Player Mapping'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'To Do'!$A$1:$H$22</definedName>
+    <definedName name="cl1st">'Baseball Simulation'!$F$8</definedName>
+    <definedName name="cl2nd">'Baseball Simulation'!$F$9</definedName>
+    <definedName name="cl3rd">'Baseball Simulation'!$F$10</definedName>
     <definedName name="cLastDataDate">Parameters!#REF!</definedName>
+    <definedName name="clAwayScore">'Baseball Simulation'!$H$2</definedName>
+    <definedName name="clBatter">'Baseball Simulation'!$F$7</definedName>
     <definedName name="clBCLastRow">Parameters!$B$7</definedName>
     <definedName name="clEntryLimit">Parameters!$B$5</definedName>
+    <definedName name="clEvent">'Baseball Simulation'!$F$11</definedName>
+    <definedName name="clEventDes">'Baseball Simulation'!#REF!</definedName>
+    <definedName name="clEventDesc">'Baseball Simulation'!$F$12</definedName>
+    <definedName name="clHomeScore">'Baseball Simulation'!$F$2</definedName>
     <definedName name="cLineUpURL">Parameters!$B$2</definedName>
+    <definedName name="clInning">'Baseball Simulation'!$F$4</definedName>
     <definedName name="clLastGameDataID">Parameters!$B$3</definedName>
     <definedName name="clLineupsCache">Parameters!$B$4</definedName>
     <definedName name="clMaxAvgWins">Parameters!$B$6</definedName>
     <definedName name="clMLBTeamsLocations">Parameters!#REF!</definedName>
+    <definedName name="clOut">'Baseball Simulation'!$F$13</definedName>
+    <definedName name="clPitch">'Baseball Simulation'!$F$5</definedName>
+    <definedName name="clPitcher">'Baseball Simulation'!$F$6</definedName>
     <definedName name="clPMLastRow">Parameters!$B$8</definedName>
     <definedName name="clUserWinsCache">Parameters!#REF!</definedName>
     <definedName name="cSalaryCap">Parameters!#REF!</definedName>
@@ -39,13 +53,13 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId13"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="873">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -2309,15 +2323,9 @@
     <t>Michal Neuvirth</t>
   </si>
   <si>
-    <t>Mikhail  Grigorenko</t>
-  </si>
-  <si>
     <t>Jason Demers</t>
   </si>
   <si>
-    <t>Jason Chimera</t>
-  </si>
-  <si>
     <t>Viktor Fasth</t>
   </si>
   <si>
@@ -2381,90 +2389,21 @@
     <t>Duncan Keith</t>
   </si>
   <si>
-    <t>Troy Grosenick</t>
-  </si>
-  <si>
-    <t>Erik Johnson</t>
-  </si>
-  <si>
-    <t>Jason LaBarbera</t>
-  </si>
-  <si>
-    <t>Calvin Pickard</t>
-  </si>
-  <si>
-    <t>Brad Winchester</t>
-  </si>
-  <si>
-    <t>Anthony Duclair</t>
-  </si>
-  <si>
-    <t>Anthony Peluso</t>
-  </si>
-  <si>
-    <t>Tim Jackman</t>
-  </si>
-  <si>
     <t>Barret Jackman</t>
   </si>
   <si>
-    <t>Ruslan Fedotenko</t>
-  </si>
-  <si>
-    <t>Martin Havlat</t>
-  </si>
-  <si>
     <t>Martin Marincin</t>
   </si>
   <si>
-    <t>Matt Tennyson</t>
-  </si>
-  <si>
-    <t>Matt Moulson</t>
-  </si>
-  <si>
     <t>Andrew Campbell</t>
   </si>
   <si>
-    <t>Jamie McGinn</t>
-  </si>
-  <si>
     <t>Tye McGinn</t>
   </si>
   <si>
-    <t>Ryane Clowe</t>
-  </si>
-  <si>
-    <t>Mike Weber</t>
-  </si>
-  <si>
-    <t>['MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL']</t>
-  </si>
-  <si>
-    <t>['CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI']</t>
-  </si>
-  <si>
     <t>Matthew Hackett</t>
   </si>
   <si>
-    <t>John Klingberg</t>
-  </si>
-  <si>
-    <t>['DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL']</t>
-  </si>
-  <si>
-    <t>Cody Eakin</t>
-  </si>
-  <si>
-    <t>['ANA', 'ANA', 'ANA', 'ANA', 'ANA', 'ANA', 'ANA']</t>
-  </si>
-  <si>
-    <t>['DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL', 'DAL']</t>
-  </si>
-  <si>
-    <t>['SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS', 'SJS']</t>
-  </si>
-  <si>
     <t>TeamOdds.py</t>
   </si>
   <si>
@@ -2480,45 +2419,30 @@
     <t>Columbus</t>
   </si>
   <si>
-    <t>[u'+137', u'-151']</t>
-  </si>
-  <si>
     <t>Detroit</t>
   </si>
   <si>
     <t>Minnesota</t>
   </si>
   <si>
-    <t>[u'+248', u'-280']</t>
-  </si>
-  <si>
     <t>Toronto</t>
   </si>
   <si>
     <t>Boston</t>
   </si>
   <si>
-    <t>[u'+216', u'-243']</t>
-  </si>
-  <si>
     <t>New Jersey</t>
   </si>
   <si>
     <t>NY Rangers</t>
   </si>
   <si>
-    <t>[u'+162', u'-180']</t>
-  </si>
-  <si>
     <t>Dallas</t>
   </si>
   <si>
     <t>Nashville</t>
   </si>
   <si>
-    <t>[u'-177', u'+160']</t>
-  </si>
-  <si>
     <t>Calgary</t>
   </si>
   <si>
@@ -2546,9 +2470,6 @@
     <t>Chicago</t>
   </si>
   <si>
-    <t>[u'+102', u'-113']</t>
-  </si>
-  <si>
     <t>Carolina</t>
   </si>
   <si>
@@ -2606,13 +2527,157 @@
     <t>[u'-200', u'+170']</t>
   </si>
   <si>
-    <t>{u'Dallas': 38.17, u'Minnesota': 60.16, u'Winnipeg': 53.49, u'Vancouver': 49.02, u'Calgary': 63.9, u'Carolina': 53.05, u'Columbus': 46.95, u'Arizona': 32.47, u'Tampa Bay': 55.75, u'Pittsburgh': 55.56, u'NY Islanders': 78.72, u'Nashville': 64.29, u'Los Angeles': 73.05, u'Toronto': 37.04, u'San Jose': 69.97, u'Florida': 46.73, u'Detroit': 42.19, u'Philadelphia': 49.5, u'Ottawa': 66.67, u'Buffalo': 23.7, u'St. Louis': 43.48, u'Colorado': 29.41, u'New Jersey': 31.65, u'Boston': 73.68, u'Edmonton': 38.46, u'Washington': 49.26, u'NY Rangers': 70.85, u'Chicago': 60.0}</t>
-  </si>
-  <si>
     <t>Vegas Odds</t>
   </si>
   <si>
     <t>Anaheim</t>
+  </si>
+  <si>
+    <t>{u'MIN': [['Zach Parise', 'Mikael Granlund', 'Jason Pominville'], ['Nino Niederreiter', 'Mikko Koivu', 'Chris Stewart'], ['Thomas Vanek', 'Charlie Coyle', 'Justin Fontaine'], ['Ryan Carter', 'Kyle Brodziak', 'Jordan Schroeder'], ['Ryan Suter', 'Jonas Brodin'], ['Marco Scandella', 'Jared Spurgeon'], ['Jordan Leopold', 'Mathew Dumba'], ['Zach Parise', 'Mikko Koivu', 'Jason Pominville', 'Ryan Suter', 'Mathew Dumba'], ['Thomas Vanek', 'Mikael Granlund', 'Chris Stewart', 'Marco Scandella', 'Jared Spurgeon']], u'TOR': [['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel'], ['Joakim Lindstrom', 'Nazem Kadri', 'Richard Panik'], ['Leo Komarov', 'Trevor Smith', 'Joffrey Lupul'], ['David Booth', 'Zach Sill', 'Casey Bailey'], ['Eric Brewer', 'Dion Phaneuf'], ['Jake Gardiner', 'Morgan Rielly'], ['Tim Erixon', 'T.J. Brennan'], ['James van Riemsdyk', 'Tyler Bozak', 'Phil Kessel', 'Morgan Rielly', 'Dion Phaneuf'], ['Joffrey Lupul', 'Nazem Kadri', 'Joakim Lindstrom', 'Jake Gardiner', 'T.J. Brennan']], u'WSH': [['Alex Ovechkin', 'Evgeny Kuznetsov', 'Joel Ward'], ['Marcus Johansson', 'Nicklas Backstrom', 'Troy Brouwer'], ['Curtis Glencross', 'Eric Fehr', 'Jason Chimera'], ['Brooks Laich', 'Michael Latta', 'Tom Wilson'], ['Brooks Orpik', 'John Carlson'], ['Karl Alzner', 'Matt Niskanen'], ['Tim Gleason', 'Mike Green'], ['Marcus Johansson', 'Nicklas Backstrom', 'Troy Brouwer', 'Alex Ovechkin', 'John Carlson'], ['Curtis Glencross', 'Evgeny Kuznetsov', 'Joel Ward', 'Matt Niskanen', 'Mike Green']], u'BOS': [['Brad Marchand', 'Patrice Bergeron', 'David Krejci'], ['Milan Lucic', 'Ryan Spooner', 'Brett Connolly'], ['Loui Eriksson', 'Carl Soderberg', 'Reilly Smith'], ['Chris Kelly', 'Gregory Campbell', 'David Pastrnak'], ['Zdeno Chara', 'Zach Trotman'], ['Torey Krug', 'Dennis Seidenberg'], ['Matt Bartkowski', 'Adam McQuaid'], ['Ryan Spooner', 'Patrice Bergeron', 'Loui Eriksson', 'Torey Krug', 'David Krejci'], ['Milan Lucic', 'Carl Soderberg', 'Brad Marchand', 'Zdeno Chara', 'Reilly Smith']], u'DET': [['Justin Abdelkader', 'Henrik Zetterberg', 'Gustav Nyquist'], ['Darren Helm', 'Pavel Datsyuk', 'Tomas Tatar'], ['Teemu Pulkkinen', 'Riley Sheahan', 'Stephen Weiss'], ['Drew Miller', 'Luke Glendening', 'Joakim Andersson'], ['Jonathan Ericsson', 'Niklas Kronwall'], ['Kyle Quincey', 'Dan DeKeyser'], ['Brendan Smith', 'Marek Zidlicky'], ['Gustav Nyquist', 'Henrik Zetterberg', 'Justin Abdelkader', 'Teemu Pulkkinen', 'Niklas Kronwall'], ['Tomas Tatar', 'Riley Sheahan', 'Stephen Weiss', 'Pavel Datsyuk', 'Marek Zidlicky']], u'NAS': [['Filip Forsberg', 'Mike Ribeiro', 'James Neal'], ['Colin Wilson', 'Mike Fisher', 'Craig Smith'], ['Viktor Stalberg', 'Matt Cullen', 'Mike Santorelli'], ['Gabriel Bourque', 'Calle Jarnkrok', 'Taylor Beck'], ['Roman Josi', 'Shea Weber'], ['Mattias Ekholm', 'Seth Jones'], ['Ryan Ellis', 'Cody Franson'], ['Colin Wilson', 'Mike Ribeiro', 'Craig Smith', 'Roman Josi', 'Shea Weber'], ['Filip Forsberg', 'Mike Fisher', 'James Neal', 'Seth Jones', 'Ryan Ellis']], u'NYI': [['Nikolay Kulemin', 'John Tavares', 'Ryan Strome'], ['Josh Bailey', 'Frans Nielsen', 'Kyle Okposo'], ['Anders Lee', 'Brock Nelson', 'Cal Clutterbuck'], ['Matt Martin', 'Casey Cizikas', 'Eric Boulton'], ['Nick Leddy', 'Johnny Boychuk'], ['Brian Strait', 'Travis Hamonic'], ['Thomas Hickey', 'Lubomir Visnovsky'], ['Anders Lee', 'John Tavares', 'Kyle Okposo', 'Nick Leddy', 'Frans Nielsen'], ['Josh Bailey', 'Brock Nelson', 'Ryan Strome', 'Lubomir Visnovsky', 'Johnny Boychuk']], u'FLA': [['Jonathan Huberdeau', 'Aleksander Barkov', 'Jaromir Jagr'], ['Brandon Pirri', 'Dave Bolland', 'Brad Boyes'], ['Jussi Jokinen', 'Vincent Trocheck', 'Jimmy Hayes'], ['Tomas Kopecky', 'Derek MacKenzie', 'Shawn Thornton'], ['Brian Campbell', 'Aaron Ekblad'], ['Willie Mitchell', 'Erik Gudbranson'], ['Dmitry Kulikov', 'Alex Petrovic'], ['Jimmy Hayes', 'Brandon Pirri', 'Brad Boyes', 'Brian Campbell', 'Jussi Jokinen'], ['Jonathan Huberdeau', 'Aleksander Barkov', 'Jaromir Jagr', 'Dmitry Kulikov', 'Aaron Ekblad']], u'COL': [['John Mitchell', 'Matt Duchene', 'Jarome Iginla'], ['Gabriel Landeskog', "Ryan O'Reilly", 'Alex Tanguay'], ['Cody McLeod', 'Marc-Andre Cliche', 'Dennis Everberg'], ['Jordan Caron', 'Freddie Hamilton', 'Joey Hishon'], ['Nate Guenin', 'Tyson Barrie'], ['Jan Hejda', 'Zach Redmond'], ['Brad Stuart', 'Nick Holden'], ['Gabriel Landeskog', "Ryan O'Reilly", 'Jarome Iginla', 'Alex Tanguay', 'Tyson Barrie'], ['John Mitchell', 'Matt Duchene', 'Joey Hishon', 'Zach Redmond', 'Nick Holden']], u'NJD': [['Reid Boucher', 'Scott Gomez', 'Steve Bernier'], ['Stefan Matteau', 'Travis Zajac', 'Michael Cammalleri'], ['Adam Henrique', 'Patrik Elias', 'Dainius Zubrus'], ['Tuomo Ruutu', 'Jacob Josefson', 'Jordin Tootoo'], ['Andy Greene', 'Adam Larsson'], ['Mark Fraser', 'Damon Severson'], ['Jon Merrill', 'Eric Gelinas'], ['Adam Henrique', 'Travis Zajac', 'Jordin Tootoo', 'Jacob Josefson', 'Damon Severson'], ['Michael Cammalleri', 'Patrik Elias', 'Steve Bernier', 'Jon Merrill', 'Eric Gelinas']], u'DAL': [['Jamie Benn', 'Cody Eakin', 'Tyler Seguin'], ['Patrick Eaves', 'Jason Spezza', 'Ales Hemsky'], ['Antoine Roussel', 'Vernon Fiddler', 'Ryan Garbutt'], ['Travis Moen', 'Colton Sceviour', 'Valeri Nichushkin'], ['Alex Goligoski', 'John Klingberg'], ['Patrik Nemeth', 'Trevor Daley'], ['Jordie Benn', 'Jason Demers'], ['Jamie Benn', 'Jason Spezza', 'Patrick Eaves', 'Tyler Seguin', 'John Klingberg'], ['Valeri Nichushkin', 'Colton Sceviour', 'Ales Hemsky', 'Trevor Daley', 'Alex Goligoski']], u'CGY': [['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler'], ['Lance Bouma', 'Mikael Backlund', 'David Jones'], ['Mason Raymond', 'Markus Granlund', 'Joe Colborne'], ['Brandon Bollig', 'Matt Stajan', 'Drew Shore'], ['Kris Russell', 'Dennis Wideman'], ['T.J. Brodie', 'Deryk Engelland'], ['David Schlemko', 'Corey Potter'], ['Johnny Gaudreau', 'Sean Monahan', 'Jiri Hudler', 'Kris Russell', 'Dennis Wideman'], ['Mason Raymond', 'Mikael Backlund', 'Joe Colborne', 'T.J. Brodie', 'Corey Potter']], u'NYR': [['Rick Nash', 'Derick Brassard', 'Mats Zuccarello'], ['Chris Kreider', 'Derek Stepan', 'J.T. Miller'], ['Carl Hagelin', 'Kevin Hayes', 'Martin St. Louis'], ['Tanner Glass', 'Dominic Moore', 'Jesper Fast'], ['Ryan McDonagh', 'Dan Girardi'], ['Marc Staal', 'Dan Boyle'], ['Keith Yandle', 'Matt Hunwick'], ['Chris Kreider', 'Derek Stepan', 'Rick Nash', 'Martin St. Louis', 'Keith Yandle'], ['Kevin Hayes', 'Derick Brassard', 'Mats Zuccarello', 'Ryan McDonagh', 'Dan Boyle']], u'CAR': [['Eric Staal', 'Jordan Staal', 'Elias Lindholm'], ['Nathan Gerbe', 'Victor Rask', 'Chris Terry'], ['Jeff Skinner', 'Jay McClement', 'Alexander Semin'], ['Andrej Nestrasil', 'Brad Malone', 'Pat Dwyer'], ['Ron Hainsey', 'Justin Faulk'], ['John-Michael Liles', 'Ryan Murphy'], ['Michal Jordan', 'Danny Biega'], ['Andrej Nestrasil', 'Eric Staal', 'Elias Lindholm', 'Victor Rask', 'Justin Faulk'], ['Jeff Skinner', 'Jordan Staal', 'Chris Terry', 'John-Michael Liles', 'Ryan Murphy']], u'PIT': [['David Perron', 'Sidney Crosby', 'Patric Hornqvist'], ['Chris Kunitz', 'Evgeni Malkin', 'Blake Comeau'], ['Daniel Winnik', 'Brandon Sutter', 'Beau Bennett'], ['Nick Spaling', 'Maxim Lapierre', 'Craig Adams'], ['Paul Martin', 'Ben Lovejoy'], ['Rob Scuderi', 'Derrick Pouliot'], ['Ian Cole', 'Taylor Chorney'], ['Chris Kunitz', 'Sidney Crosby', 'Patric Hornqvist', 'Evgeni Malkin', 'Derrick Pouliot'], ['David Perron', 'Brandon Sutter', 'Blake Comeau', 'Paul Martin', 'Ian Cole']], u'VAN': [['Daniel Sedin', 'Henrik Sedin', 'Alexandre Burrows'], ['Chris Higgins', 'Nick Bonino', 'Radim Vrbata'], ['Shawn Matthias', 'Linden Vey', 'Derek Dorsett'], ['Ronalds Kenins', 'Bo Horvat', 'Jannik Hansen'], ['Alexander Edler', 'Chris Tanev'], ['Dan Hamhuis', 'Yannick Weber'], ['Kevin Bieksa', 'Luca Sbisa'], ['Daniel Sedin', 'Henrik Sedin', 'Radim Vrbata', 'Alexander Edler', 'Yannick Weber'], ['Chris Higgins', 'Nick Bonino', 'Alexandre Burrows', 'Dan Hamhuis', 'Chris Tanev']], u'STL': [['Jaden Schwartz', 'Paul Stastny', 'T.J. Oshie'], ['Dmitrij Jaskin', 'David Backes', 'Patrik Berglund'], ['Olli Jokinen', 'Jori Lehtera', 'Ty Rattie'], ['Steve Ott', 'Marcel Goc', 'Ryan Reaves'], ['Jay Bouwmeester', 'Alex Pietrangelo'], ['Zbynek Michalek', 'Kevin Shattenkirk'], ['Barret Jackman', 'Robert Bortuzzo'], ['Jaden Schwartz', 'David Backes', 'T.J. Oshie', 'Paul Stastny', 'Kevin Shattenkirk'], ['Dmitrij Jaskin', 'Jori Lehtera', 'Patrik Berglund', 'Jay Bouwmeester', 'Alex Pietrangelo']], u'CHI': [['Kris Versteeg', 'Jonathan Toews', 'Marian Hossa'], ['Patrick Sharp', 'Brad Richards', 'Antoine Vermette'], ['Bryan Bickell', 'Andrew Shaw', 'Brandon Saad'], ['Andrew Desjardins', 'Marcus Kruger', 'Teuvo Teravainen'], ['Kimmo Timonen', 'Brent Seabrook'], ['Duncan Keith', 'Michal Rozsival'], ['Johnny Oduya', 'Niklas Hjalmarsson'], ['Andrew Shaw', 'Jonathan Toews', 'Brandon Saad', 'Duncan Keith', 'Marian Hossa'], ['Teuvo Teravainen', 'Brad Richards', 'Kris Versteeg', 'Patrick Sharp', 'Brent Seabrook']], u'SJS': [['Joe Pavelski', 'Joe Thornton', 'Melker Karlsson'], ['Patrick Marleau', 'Logan Couture', 'Tomas Hertl'], ['Matthew Nieto', 'Chris Tierney', 'Tommy Wingels'], ['Mike Brown', 'Ben Smith', 'Barclay Goodrow'], ['Matt Irwin', 'Brent Burns'], ['Brenden Dillon', 'Justin Braun'], ['Karl Stollery', 'Taylor Fedun'], ['Patrick Marleau', 'Joe Thornton', 'Logan Couture', 'Joe Pavelski', 'Brent Burns'], ['Melker Karlsson', 'Chris Tierney', 'Tomas Hertl', 'Matt Irwin', 'Taylor Fedun']], u'MTL': [['Max Pacioretty', 'Tomas Plekanec', 'Brendan Gallagher'], ['Alex Galchenyuk', 'David Desharnais', 'P.A. Parenteau'], ['Brandon Prust', 'Lars Eller', 'Dale Weise'], ['Jacob De La Rose', 'Torrey Mitchell', 'Devante Smith-Pelly'], ['Alexei Emelin', 'P.K. Subban'], ['Nathan Beaulieu', 'Jeff Petry'], ['Sergei Gonchar', 'Tom Gilbert'], ['Max Pacioretty', 'David Desharnais', 'P.A. Parenteau', 'Nathan Beaulieu', 'P.K. Subban'], ['Alex Galchenyuk', 'Tomas Plekanec', 'Brendan Gallagher', 'Sergei Gonchar', 'Jeff Petry']], u'PHI': [['Michael Raffl', 'Claude Giroux', 'Jakub Voracek'], ['Brayden Schenn', 'Sean Couturier', 'Matt Read'], ['Zac Rinaldo', 'Nick Cousins', 'Ryan White'], ['Chris VandeVelde', 'Vincent Lecavalier'], ['Nicklas Grossmann', 'Mark Streit'], ['Michael Del Zotto', 'Nick Schultz'], ['Carlo Colaiacovo', 'Brandon Manning'], ['Brayden Schenn', 'Claude Giroux', 'Ryan White', 'Jakub Voracek', 'Mark Streit'], ['Michael Raffl', 'Sean Couturier', 'Matt Read', 'Michael Del Zotto', 'Vincent Lecavalier']], u'ANA': [['Tomas Fleischmann', 'Ryan Kesler', 'Kyle Palmieri'], ['Jiri Sekac', 'Rickard Rakell', 'Corey Perry'], ['Andrew Cogliano', 'Nate Thompson', 'Jakob Silfverberg'], ['Stefan Noesen', 'Chris Wagner', 'Emerson Etem'], ['Hampus Lindholm', 'Francois Beauchemin'], ['Cam Fowler', 'Sami Vatanen'], ['Simon Despres', 'James Wisniewski'], ['Tomas Fleischmann', 'Ryan Kesler', 'Kyle Palmieri', 'Francois Beauchemin', 'Sami Vatanen'], ['Jiri Sekac', 'Rickard Rakell', 'Corey Perry', 'Cam Fowler', 'James Wisniewski']], u'LAK': [['Marian Gaborik', 'Anze Kopitar', 'Justin Williams'], ['Dwight King', 'Jeff Carter', 'Tyler Toffoli'], ['Trevor Lewis', 'Jarret Stoll', 'Dustin Brown'], ['Kyle Clifford', 'Nick Shore', 'Jordan Nolan'], ['Jake Muzzin', 'Drew Doughty'], ['Alec Martinez', 'Robyn Regehr'], ['Brayden McNabb', 'Matt Greene'], ['Marian Gaborik', 'Anze Kopitar', 'Jeff Carter', 'Jake Muzzin', 'Drew Doughty'], ['Dustin Brown', 'Tyler Toffoli', 'Justin Williams', 'Brayden McNabb', 'Alec Martinez']], u'CBJ': [['Boone Jenner', 'Ryan Johansen', 'Cam Atkinson'], ['Brandon Dubinsky', 'Artem Anisimov', 'Nick Foligno'], ['Scott Hartnell', 'Alexander Wennberg', 'Marko Dano'], ['Matt Calvert', 'Mark Letestu', 'Jeremy Morin'], ['Jack Johnson', 'David Savard'], ['Fedor Tyutin', 'Dalton Prout'], ['Kevin Connauton', 'Cody Goloubef'], ['Scott Hartnell', 'Ryan Johansen', 'Nick Foligno', 'Kevin Connauton', 'Alexander Wennberg'], ['Boone Jenner', 'Brandon Dubinsky', 'Cam Atkinson', 'Jack Johnson', 'David Savard']], u'BUF': [['Matt Moulson', 'Johan Larsson', 'Tyler Ennis'], ['Marcus Foligno', 'Mikhail  Grigorenko', 'Brian Gionta'], ['Nicolas Deslauriers', 'Phil Varone', 'Patrick Kaleta'], ['Cody Hodgson', 'Matt Ellis', 'Zac Dalpe'], ['Zach Bogosian', 'Rasmus Ristolainen'], ['Andrej Meszaros', 'Tyson Strachan'], ['Andre Benoit', 'Nikita Zadorov'], ['Matt Moulson', 'Johan Larsson', 'Brian Gionta', 'Tyler Ennis', 'Rasmus Ristolainen'], ['Marcus Foligno', 'Mikhail  Grigorenko', 'Cody Hodgson', 'Zach Bogosian', 'Andrej Meszaros']], u'EDM': [['Benoit Pouliot', 'Ryan Nugent-Hopkins', 'Jordan Eberle'], ['Teddy Purcell', 'Derek Roy', 'Nail Yakupov'], ['Taylor Hall', 'Anton Lander', 'Andrew Miller'], ['Luke Gazdic', 'Rob Klinkhammer', 'Matt Fraser'], ['Oscar Klefbom', 'Justin Schultz'], ['Martin Marincin', 'David Musil'], ['Brandon Davidson', 'Keith Aulie'], ['Teddy Purcell', 'Ryan Nugent-Hopkins', 'Anton Lander', 'Jordan Eberle', 'Justin Schultz'], ['Taylor Hall', 'Derek Roy', 'Benoit Pouliot', 'Oscar Klefbom', 'Nail Yakupov']], u'TBL': [['Alex Killorn', 'Steven Stamkos', 'Ryan Callahan'], ['Ondrej Palat', 'Tyler Johnson', 'Nikita Kucherov'], ['Vladislav Namestnikov', 'Valtteri Filppula', 'Cedric Paquette'], ['Jonathan Drouin', 'Brian Boyle', 'J.T. Brown'], ['Nikita Nesterov', 'Anton Stralman'], ['Matt Carle', 'Slater Koekkoek'], ['Mark Barberio', 'Luke Witkowski'], ['Jonathan Drouin', 'Steven Stamkos', 'Ondrej Palat', 'Valtteri Filppula', 'Anton Stralman'], ['Vladislav Namestnikov', 'Tyler Johnson', 'Ryan Callahan', 'Nikita Nesterov', 'Nikita Kucherov']], u'WIN': [['Andrew Ladd', 'Bryan Little', 'Michael Frolik'], ['Drew Stafford', 'Mark Scheifele', 'Blake Wheeler'], ['Mathieu Perreault', 'Adam Lowry', 'Lee Stempniak'], ['Jiri Tlusty', 'Jim Slater', 'Chris Thorburn'], ['Tobias Enstrom', 'Tyler Myers'], ['Mark Stuart', 'Jacob Trouba'], ['Adam Pardy', 'Jay Harrison'], ['Andrew Ladd', 'Bryan Little', 'Blake Wheeler', 'Mathieu Perreault', 'Tyler Myers'], ['Drew Stafford', 'Mark Scheifele', 'Michael Frolik', 'Tobias Enstrom', 'Jacob Trouba']], u'ARI': [['Tobias Rieder', 'Mark Arcobello', 'Shane Doan'], ['Martin Erat', 'Sam Gagner', 'David Moss'], ['Craig Cunningham', 'Kyle Chipchura', 'Jordan Szwarz'], ['Tye McGinn', 'Joe Vitale', 'B.J. Crombeen'], ['Oliver Ekman-Larsson', 'Michael Stone'], ['Klas Dahlbeck', 'Connor Murphy'], ['Andrew Campbell', 'John Moore'], ['Tobias Rieder', 'Sam Gagner', 'Shane Doan', 'John Moore', 'Oliver Ekman-Larsson'], ['Martin Erat', 'Mark Arcobello', 'David Moss', 'Michael Stone', 'Connor Murphy']], u'OTT': [['Zack Smith', 'Mika Zibanejad', 'Bobby Ryan'], ['Clarke MacArthur', 'Kyle Turris', 'Mark Stone'], ['Erik Condra', 'Jean-Gabriel Pageau', 'Curtis Lazar'], ['Mike Hoffman', 'David Legwand', 'Alex Chiasson'], ['Marc Methot', 'Erik Karlsson'], ['Patrick Wiercioch', 'Cody Ceci'], ['Mark Borowiecki', 'Eric Gryba'], ['David Legwand', 'Mika Zibanejad', 'Bobby Ryan', 'Patrick Wiercioch', 'Erik Karlsson'], ['Clarke MacArthur', 'Kyle Turris', 'Mark Stone', 'Mike Hoffman', 'Cody Ceci']]}</t>
+  </si>
+  <si>
+    <t>David Musil</t>
+  </si>
+  <si>
+    <t>Todd Bertuzzi</t>
+  </si>
+  <si>
+    <t>Chris Neil</t>
+  </si>
+  <si>
+    <t>Robin Lehner</t>
+  </si>
+  <si>
+    <t>Jay Beagle</t>
+  </si>
+  <si>
+    <t>Nathan Horton</t>
+  </si>
+  <si>
+    <t>Jonathan Drouin</t>
+  </si>
+  <si>
+    <t>Jonas Gustavsson</t>
+  </si>
+  <si>
+    <t>Dmitry Kulikov</t>
+  </si>
+  <si>
+    <t>Andre Burakovsky</t>
+  </si>
+  <si>
+    <t>Bobby Butler</t>
+  </si>
+  <si>
+    <t>Andy Greene</t>
+  </si>
+  <si>
+    <t>Philipp Grubauer</t>
+  </si>
+  <si>
+    <t>Philip Varone</t>
+  </si>
+  <si>
+    <t>[u'+106', u'-117']</t>
+  </si>
+  <si>
+    <t>[u'-165', u'+149']</t>
+  </si>
+  <si>
+    <t>[u'+143', u'-158']</t>
+  </si>
+  <si>
+    <t>[u'+132', u'-146']</t>
+  </si>
+  <si>
+    <t>[u'-129', u'+117']</t>
+  </si>
+  <si>
+    <t>[u'-127', u'+115']</t>
+  </si>
+  <si>
+    <t>[u'+191', u'-213']</t>
+  </si>
+  <si>
+    <t>{u'PHI': 46.08, u'STL': 43.48, u'CHI': 60.0, u'MIN': 61.24, u'TOR': 37.04, u'WSH': 48.54, u'LAK': 55.56, u'DET': 53.92, u'OTT': 66.67, u'SJS': 59.35, u'WIN': 41.15, u'NYR': 68.05, u'DAL': 43.1, u'MTL': 55.95, u'CAR': 62.26, u'FLA': 46.51, u'VAN': 46.95, u'BUF': 40.16, u'CBJ': 34.36, u'PIT': 56.33}</t>
+  </si>
+  <si>
+    <t>['OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT']</t>
+  </si>
+  <si>
+    <t>['FLA', 'FLA', 'FLA', 'FLA', 'FLA', 'FLA', 'FLA', 'FLA']</t>
+  </si>
+  <si>
+    <t>['WSH', 'WSH', 'WSH', 'WSH', 'WSH', 'WSH', 'WSH']</t>
+  </si>
+  <si>
+    <t>John Carlson</t>
+  </si>
+  <si>
+    <t>['CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI', 'CHI']</t>
+  </si>
+  <si>
+    <t>['MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL', 'MTL']</t>
+  </si>
+  <si>
+    <t>['OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT']</t>
+  </si>
+  <si>
+    <t>BBSim.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Cole\Desktop\FanDuel\fanduel\modules\BBSim.py</t>
+  </si>
+  <si>
+    <t>script_name_5</t>
+  </si>
+  <si>
+    <t>script_path_5</t>
+  </si>
+  <si>
+    <t>Home Score:</t>
+  </si>
+  <si>
+    <t>Away Score:</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>Pitcher</t>
+  </si>
+  <si>
+    <t>Batter</t>
+  </si>
+  <si>
+    <t>Event:</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>Outs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robinson Cano grounds out, pitcher C.  J.   Wilson to first baseman Albert Pujols.  </t>
+  </si>
+  <si>
+    <t>Inning</t>
+  </si>
+  <si>
+    <t>Event Description</t>
+  </si>
+  <si>
+    <t>Groundout</t>
   </si>
 </sst>
 </file>
@@ -3283,11 +3348,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="245598464"/>
-        <c:axId val="245604352"/>
+        <c:axId val="233474304"/>
+        <c:axId val="233480192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245598464"/>
+        <c:axId val="233474304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,7 +3361,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245604352"/>
+        <c:crossAx val="233480192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3369,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245604352"/>
+        <c:axId val="233480192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,7 +3380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="245598464"/>
+        <c:crossAx val="233474304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3428,11 +3493,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="246226304"/>
-        <c:axId val="246232192"/>
+        <c:axId val="228855168"/>
+        <c:axId val="228861056"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="246226304"/>
+        <c:axId val="228855168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3441,7 +3506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246232192"/>
+        <c:crossAx val="228861056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3449,7 +3514,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246232192"/>
+        <c:axId val="228861056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3460,7 +3525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246226304"/>
+        <c:crossAx val="228855168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4103,7 +4168,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4111,7 +4176,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4119,7 +4184,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4127,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>806</v>
+        <v>854</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4135,7 +4200,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>807</v>
+        <v>855</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4143,7 +4208,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>455</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4151,7 +4216,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>456</v>
+        <v>782</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4159,7 +4224,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>226</v>
+        <v>455</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4167,7 +4232,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4175,7 +4240,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4183,7 +4248,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4191,7 +4256,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4199,6 +4264,22 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>856</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>857</v>
+      </c>
+      <c r="B15" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4389,13 +4470,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B1" t="s">
-        <v>810</v>
+        <v>786</v>
       </c>
       <c r="C1" t="s">
-        <v>808</v>
+        <v>839</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4403,189 +4484,189 @@
         <v>812</v>
       </c>
       <c r="B2" t="s">
-        <v>813</v>
+        <v>788</v>
       </c>
       <c r="C2" t="s">
-        <v>811</v>
+        <v>821</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>815</v>
+        <v>803</v>
       </c>
       <c r="B3" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="C3" t="s">
-        <v>814</v>
+        <v>840</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>818</v>
+        <v>806</v>
       </c>
       <c r="B4" t="s">
-        <v>819</v>
+        <v>787</v>
       </c>
       <c r="C4" t="s">
-        <v>817</v>
+        <v>841</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>821</v>
+        <v>792</v>
       </c>
       <c r="B5" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="C5" t="s">
-        <v>820</v>
+        <v>842</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>824</v>
+        <v>784</v>
       </c>
       <c r="B6" t="s">
-        <v>825</v>
+        <v>797</v>
       </c>
       <c r="C6" t="s">
-        <v>823</v>
+        <v>843</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>809</v>
+        <v>798</v>
       </c>
       <c r="B7" t="s">
-        <v>827</v>
+        <v>799</v>
       </c>
       <c r="C7" t="s">
-        <v>826</v>
+        <v>844</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>828</v>
+        <v>801</v>
       </c>
       <c r="B8" t="s">
-        <v>829</v>
+        <v>802</v>
       </c>
       <c r="C8" t="s">
-        <v>826</v>
+        <v>800</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>831</v>
+        <v>785</v>
       </c>
       <c r="B9" t="s">
-        <v>832</v>
+        <v>791</v>
       </c>
       <c r="C9" t="s">
-        <v>830</v>
+        <v>845</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="B10" t="s">
-        <v>834</v>
+        <v>805</v>
       </c>
       <c r="C10" t="s">
-        <v>833</v>
+        <v>783</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
       <c r="B11" t="s">
-        <v>837</v>
+        <v>806</v>
       </c>
       <c r="C11" t="s">
-        <v>835</v>
+        <v>804</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>839</v>
+        <v>808</v>
       </c>
       <c r="B12" t="s">
-        <v>840</v>
+        <v>809</v>
       </c>
       <c r="C12" t="s">
-        <v>838</v>
+        <v>807</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
       <c r="B13" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="C13" t="s">
-        <v>841</v>
+        <v>810</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>845</v>
+        <v>814</v>
       </c>
       <c r="B14" t="s">
-        <v>829</v>
+        <v>799</v>
       </c>
       <c r="C14" t="s">
-        <v>844</v>
+        <v>813</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>847</v>
+        <v>816</v>
       </c>
       <c r="B15" t="s">
-        <v>848</v>
+        <v>817</v>
       </c>
       <c r="C15" t="s">
+        <v>815</v>
+      </c>
+      <c r="E15" t="s">
         <v>846</v>
-      </c>
-      <c r="E15" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>850</v>
+        <v>819</v>
       </c>
       <c r="B16" t="s">
-        <v>851</v>
+        <v>820</v>
       </c>
       <c r="C16" t="s">
-        <v>849</v>
+        <v>818</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
       <c r="B17" t="s">
-        <v>812</v>
+        <v>786</v>
       </c>
       <c r="C17" t="s">
-        <v>826</v>
+        <v>796</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
       <c r="B18" t="s">
-        <v>815</v>
+        <v>788</v>
       </c>
       <c r="C18" t="s">
-        <v>852</v>
+        <v>821</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8141,6 +8222,111 @@
     <row r="729" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B729">
         <v>3100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>858</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>859</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="5:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="5:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>861</v>
+      </c>
+      <c r="F6">
+        <v>572020</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>862</v>
+      </c>
+      <c r="F7">
+        <v>545361</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>863</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>871</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>868</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8153,9 +8339,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8772,7 +8956,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -8809,7 +8993,9 @@
       <c r="A4" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -8899,7 +9085,7 @@
         <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>854</v>
+        <v>822</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8910,7 +9096,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>855</v>
+        <v>823</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8921,7 +9107,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>837</v>
+        <v>806</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -8932,7 +9118,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>816</v>
+        <v>789</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -8943,7 +9129,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>839</v>
+        <v>808</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -8954,7 +9140,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>824</v>
+        <v>794</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -8965,7 +9151,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>834</v>
+        <v>803</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -8976,7 +9162,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>832</v>
+        <v>802</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -8987,7 +9173,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>850</v>
+        <v>819</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -8998,7 +9184,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>810</v>
+        <v>785</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -9009,7 +9195,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>821</v>
+        <v>792</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -9020,7 +9206,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>812</v>
+        <v>786</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -9031,7 +9217,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>825</v>
+        <v>795</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -9042,7 +9228,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>829</v>
+        <v>799</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -9053,7 +9239,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>851</v>
+        <v>820</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -9064,7 +9250,7 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>813</v>
+        <v>787</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9075,7 +9261,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>828</v>
+        <v>798</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -9086,7 +9272,7 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>822</v>
+        <v>793</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -9097,7 +9283,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>818</v>
+        <v>790</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -9108,7 +9294,7 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>840</v>
+        <v>809</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -9119,7 +9305,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>819</v>
+        <v>791</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -9130,7 +9316,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>843</v>
+        <v>812</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -9141,7 +9327,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>827</v>
+        <v>797</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -9152,7 +9338,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>848</v>
+        <v>817</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -9163,7 +9349,7 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>809</v>
+        <v>784</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -9174,7 +9360,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>847</v>
+        <v>816</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -9185,7 +9371,7 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>831</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -9196,7 +9382,7 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>845</v>
+        <v>814</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9207,7 +9393,7 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>815</v>
+        <v>788</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -9218,7 +9404,7 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>836</v>
+        <v>805</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -9229,7 +9415,7 @@
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>842</v>
+        <v>811</v>
       </c>
     </row>
   </sheetData>
@@ -9260,7 +9446,7 @@
     <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>778</v>
+        <v>826</v>
       </c>
       <c r="B2" t="s">
         <v>544</v>
@@ -9295,42 +9481,42 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>767</v>
+        <v>827</v>
       </c>
       <c r="B3" t="s">
-        <v>768</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>769</v>
+        <v>190</v>
       </c>
       <c r="D3" t="s">
-        <v>558</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>559</v>
+        <v>725</v>
       </c>
       <c r="F3" t="s">
-        <v>560</v>
+        <v>467</v>
       </c>
       <c r="G3" t="s">
-        <v>237</v>
+        <v>471</v>
       </c>
       <c r="H3" t="s">
-        <v>561</v>
+        <v>468</v>
       </c>
       <c r="I3" t="s">
-        <v>562</v>
+        <v>472</v>
       </c>
       <c r="J3" t="s">
-        <v>272</v>
+        <v>213</v>
       </c>
       <c r="K3" t="s">
-        <v>474</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="B4" t="s">
         <v>223</v>
@@ -9365,13 +9551,13 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>828</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>722</v>
       </c>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>543</v>
       </c>
       <c r="D5" t="s">
         <v>503</v>
@@ -9430,13 +9616,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>779</v>
+        <v>759</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>462</v>
       </c>
       <c r="C6" t="s">
-        <v>503</v>
+        <v>423</v>
       </c>
       <c r="D6" t="s">
         <v>758</v>
@@ -9465,51 +9651,51 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>766</v>
       </c>
       <c r="C7" t="s">
-        <v>423</v>
+        <v>767</v>
       </c>
       <c r="D7" t="s">
-        <v>760</v>
+        <v>558</v>
       </c>
       <c r="E7" t="s">
-        <v>256</v>
+        <v>559</v>
       </c>
       <c r="F7" t="s">
-        <v>420</v>
+        <v>560</v>
       </c>
       <c r="G7" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
-        <v>258</v>
+        <v>561</v>
       </c>
       <c r="I7" t="s">
-        <v>260</v>
+        <v>562</v>
       </c>
       <c r="J7" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="K7" t="s">
-        <v>179</v>
+        <v>474</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>780</v>
+        <v>829</v>
       </c>
       <c r="B8" t="s">
-        <v>756</v>
+        <v>734</v>
       </c>
       <c r="C8" t="s">
         <v>254</v>
       </c>
       <c r="D8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E8" t="s">
         <v>463</v>
@@ -9532,16 +9718,16 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>716</v>
       </c>
       <c r="B9" t="s">
-        <v>756</v>
+        <v>669</v>
       </c>
       <c r="C9" t="s">
-        <v>254</v>
+        <v>640</v>
       </c>
       <c r="D9" t="s">
-        <v>760</v>
+        <v>419</v>
       </c>
       <c r="E9" t="s">
         <v>269</v>
@@ -9567,13 +9753,13 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="B10" t="s">
-        <v>763</v>
+        <v>521</v>
       </c>
       <c r="C10" t="s">
-        <v>254</v>
+        <v>769</v>
       </c>
       <c r="D10" t="s">
         <v>75</v>
@@ -9602,13 +9788,13 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
       <c r="B11" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C11" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D11" t="s">
         <v>475</v>
@@ -9637,13 +9823,13 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>782</v>
+        <v>485</v>
       </c>
       <c r="B12" t="s">
-        <v>255</v>
+        <v>486</v>
       </c>
       <c r="C12" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="D12" t="s">
         <v>183</v>
@@ -9672,22 +9858,22 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>783</v>
+        <v>830</v>
       </c>
       <c r="B13" t="s">
-        <v>784</v>
+        <v>723</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>831</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
-        <v>269</v>
+        <v>185</v>
       </c>
       <c r="F13" t="s">
-        <v>270</v>
+        <v>186</v>
       </c>
       <c r="G13" t="s">
         <v>219</v>
@@ -9707,10 +9893,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>785</v>
+        <v>530</v>
       </c>
       <c r="B14" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
       <c r="C14" t="s">
         <v>190</v>
@@ -9742,13 +9928,13 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>787</v>
+        <v>832</v>
       </c>
       <c r="B15" t="s">
-        <v>786</v>
+        <v>669</v>
       </c>
       <c r="C15" t="s">
-        <v>733</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
         <v>183</v>
@@ -9777,16 +9963,16 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>490</v>
+        <v>524</v>
       </c>
       <c r="B16" t="s">
-        <v>788</v>
+        <v>833</v>
       </c>
       <c r="C16" t="s">
         <v>423</v>
       </c>
       <c r="D16" t="s">
-        <v>789</v>
+        <v>777</v>
       </c>
       <c r="E16" t="s">
         <v>462</v>
@@ -9812,7 +9998,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>549</v>
+        <v>771</v>
       </c>
       <c r="B17" t="s">
         <v>218</v>
@@ -9847,22 +10033,22 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>790</v>
+        <v>834</v>
       </c>
       <c r="B18" t="s">
-        <v>791</v>
+        <v>502</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>752</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>504</v>
       </c>
       <c r="F18" t="s">
-        <v>197</v>
+        <v>478</v>
       </c>
       <c r="G18" t="s">
         <v>219</v>
@@ -9882,13 +10068,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B19" t="s">
         <v>526</v>
       </c>
       <c r="C19" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="D19" t="s">
         <v>241</v>
@@ -9917,13 +10103,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>529</v>
+        <v>242</v>
       </c>
       <c r="B20" t="s">
         <v>526</v>
       </c>
       <c r="C20" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="D20" t="s">
         <v>241</v>
@@ -9952,10 +10138,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>793</v>
+        <v>686</v>
       </c>
       <c r="B21" t="s">
-        <v>794</v>
+        <v>779</v>
       </c>
       <c r="C21" t="s">
         <v>500</v>
@@ -9987,22 +10173,22 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>795</v>
+        <v>549</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>489</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>113</v>
       </c>
       <c r="E22" t="s">
-        <v>217</v>
+        <v>69</v>
       </c>
       <c r="F22" t="s">
-        <v>459</v>
+        <v>197</v>
       </c>
       <c r="G22" t="s">
         <v>219</v>
@@ -10022,7 +10208,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>706</v>
+        <v>835</v>
       </c>
       <c r="B23" t="s">
         <v>214</v>
@@ -10057,22 +10243,22 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>518</v>
+        <v>273</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>274</v>
       </c>
       <c r="C24" t="s">
-        <v>519</v>
+        <v>275</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>276</v>
       </c>
       <c r="E24" t="s">
-        <v>421</v>
+        <v>277</v>
       </c>
       <c r="F24" t="s">
-        <v>457</v>
+        <v>278</v>
       </c>
       <c r="G24" t="s">
         <v>240</v>
@@ -10080,10 +10266,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>510</v>
       </c>
       <c r="C25" t="s">
         <v>519</v>
@@ -10115,13 +10301,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>485</v>
+        <v>707</v>
       </c>
       <c r="B26" t="s">
-        <v>486</v>
+        <v>703</v>
       </c>
       <c r="C26" t="s">
-        <v>259</v>
+        <v>836</v>
       </c>
       <c r="D26" t="s">
         <v>113</v>
@@ -10150,16 +10336,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>509</v>
+        <v>837</v>
       </c>
       <c r="B27" t="s">
-        <v>510</v>
+        <v>838</v>
       </c>
       <c r="C27" t="s">
-        <v>259</v>
+        <v>733</v>
       </c>
       <c r="D27" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E27" t="s">
         <v>256</v>
@@ -10185,37 +10371,37 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>460</v>
+        <v>528</v>
       </c>
       <c r="B28" t="s">
-        <v>796</v>
+        <v>725</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>467</v>
       </c>
       <c r="D28" t="s">
-        <v>282</v>
+        <v>476</v>
       </c>
       <c r="E28" t="s">
-        <v>264</v>
+        <v>468</v>
       </c>
       <c r="F28" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="G28" t="s">
-        <v>703</v>
+        <v>189</v>
       </c>
       <c r="H28" t="s">
-        <v>556</v>
+        <v>190</v>
       </c>
       <c r="I28" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="J28" t="s">
-        <v>180</v>
+        <v>257</v>
       </c>
       <c r="K28" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -10360,13 +10546,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B33" t="s">
         <v>521</v>
       </c>
       <c r="C33" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D33" t="s">
         <v>752</v>
@@ -10395,13 +10581,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B34" t="s">
         <v>521</v>
       </c>
       <c r="C34" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D34" t="s">
         <v>476</v>
@@ -10436,7 +10622,7 @@
         <v>272</v>
       </c>
       <c r="C35" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D35" t="s">
         <v>218</v>
@@ -10506,7 +10692,7 @@
         <v>521</v>
       </c>
       <c r="C37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D37" t="s">
         <v>216</v>
@@ -10535,7 +10721,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>799</v>
+        <v>780</v>
       </c>
       <c r="B38" t="s">
         <v>243</v>
@@ -10570,7 +10756,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B39" t="s">
         <v>493</v>
@@ -10666,7 +10852,7 @@
         <v>557</v>
       </c>
       <c r="B42" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C42" t="s">
         <v>269</v>
@@ -10698,13 +10884,13 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>765</v>
+      </c>
+      <c r="B43" t="s">
+        <v>766</v>
+      </c>
+      <c r="C43" t="s">
         <v>767</v>
-      </c>
-      <c r="B43" t="s">
-        <v>768</v>
-      </c>
-      <c r="C43" t="s">
-        <v>769</v>
       </c>
       <c r="D43" t="s">
         <v>558</v>
@@ -10861,19 +11047,19 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B48" t="s">
         <v>521</v>
       </c>
       <c r="C48" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D48" t="s">
         <v>571</v>
       </c>
       <c r="E48" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="F48" t="s">
         <v>624</v>
@@ -10896,7 +11082,7 @@
         <v>565</v>
       </c>
       <c r="B49" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C49" t="s">
         <v>223</v>
@@ -11001,10 +11187,10 @@
         <v>523</v>
       </c>
       <c r="B52" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C52" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D52" t="s">
         <v>558</v>
@@ -11033,7 +11219,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B53" t="s">
         <v>462</v>
@@ -11161,7 +11347,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B57" t="s">
         <v>726</v>
@@ -11196,7 +11382,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B58" t="s">
         <v>498</v>
@@ -11251,16 +11437,16 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B60" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C60" t="s">
         <v>735</v>
       </c>
       <c r="D60" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E60" t="s">
         <v>239</v>
@@ -11367,7 +11553,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B64" t="s">
         <v>214</v>
@@ -11494,7 +11680,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B69" t="s">
         <v>726</v>
@@ -11514,7 +11700,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B70" t="s">
         <v>498</v>
@@ -11580,16 +11766,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B73" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C73" t="s">
         <v>735</v>
       </c>
       <c r="D73" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E73" t="s">
         <v>277</v>
@@ -13731,7 +13917,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -13742,7 +13928,7 @@
         <v>505</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>754</v>
+        <v>825</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -15881,7 +16067,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15910,155 +16096,155 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>650</v>
       </c>
       <c r="B2" t="s">
-        <v>803</v>
+        <v>852</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D2" s="9">
-        <v>-1188.9992594600001</v>
+        <v>426.65625</v>
       </c>
       <c r="E2">
-        <v>7700</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>802</v>
+        <v>422</v>
       </c>
       <c r="B3" t="s">
-        <v>804</v>
+        <v>847</v>
       </c>
       <c r="C3" t="s">
         <v>159</v>
       </c>
       <c r="D3" s="9">
-        <v>392.62666666699999</v>
+        <v>435.796875</v>
       </c>
       <c r="E3">
-        <v>4500</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>615</v>
+        <v>692</v>
       </c>
       <c r="B4" t="s">
-        <v>804</v>
+        <v>853</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D4" s="9">
-        <v>436.62666666699999</v>
+        <v>-1080.16961528</v>
       </c>
       <c r="E4">
-        <v>8500</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>651</v>
+        <v>478</v>
       </c>
       <c r="B5" t="s">
-        <v>797</v>
+        <v>848</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="9">
-        <v>388.24517906300002</v>
+        <v>430.875</v>
       </c>
       <c r="E5">
-        <v>5700</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
       <c r="B6" t="s">
-        <v>797</v>
+        <v>849</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D6" s="9">
-        <v>446.04683195600001</v>
+        <v>627.299319728</v>
       </c>
       <c r="E6">
-        <v>5600</v>
+        <v>9800</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>650</v>
+        <v>589</v>
       </c>
       <c r="B7" t="s">
-        <v>797</v>
+        <v>849</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D7" s="9">
-        <v>458.50964187300002</v>
+        <v>470.68027210899999</v>
       </c>
       <c r="E7">
-        <v>9300</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>777</v>
+        <v>850</v>
       </c>
       <c r="B8" t="s">
-        <v>798</v>
+        <v>849</v>
       </c>
       <c r="C8" t="s">
         <v>160</v>
       </c>
       <c r="D8" s="9">
-        <v>486</v>
+        <v>401.95918367299998</v>
       </c>
       <c r="E8">
-        <v>5300</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>514</v>
+        <v>587</v>
       </c>
       <c r="B9" t="s">
-        <v>805</v>
+        <v>849</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="9">
-        <v>279.89999999999998</v>
+        <v>482.05442176899999</v>
       </c>
       <c r="E9">
-        <v>3800</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>800</v>
+        <v>775</v>
       </c>
       <c r="B10" t="s">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C10" t="s">
         <v>160</v>
       </c>
       <c r="D10" s="9">
-        <v>456.583809524</v>
+        <v>499.49387755100003</v>
       </c>
       <c r="E10">
-        <v>4500</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add cells to parameters sheet in fanduel.xlsx
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="10320" windowHeight="9900" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="10320" windowHeight="9840" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <definedName name="clAwayScore">'Baseball Simulation'!$H$2</definedName>
     <definedName name="clBatter">'Baseball Simulation'!$F$7</definedName>
     <definedName name="clBCLastRow">Parameters!$B$7</definedName>
+    <definedName name="clDFNNBA">Parameters!$B$13</definedName>
     <definedName name="clEntryLimit">Parameters!$B$5</definedName>
     <definedName name="clEvent">'Baseball Simulation'!$F$11</definedName>
     <definedName name="clEventDes">'Baseball Simulation'!#REF!</definedName>
@@ -37,6 +38,7 @@
     <definedName name="clHomeScore">'Baseball Simulation'!$F$2</definedName>
     <definedName name="cLineUpURL">Parameters!$B$2</definedName>
     <definedName name="clInning">'Baseball Simulation'!$F$4</definedName>
+    <definedName name="clLastDate">Parameters!$B$12</definedName>
     <definedName name="clLastGameDataID">Parameters!$B$3</definedName>
     <definedName name="clLineupsCache">Parameters!$B$4</definedName>
     <definedName name="clMaxAvgWins">Parameters!$B$6</definedName>
@@ -45,11 +47,14 @@
     <definedName name="clPitch">'Baseball Simulation'!$F$5</definedName>
     <definedName name="clPitcher">'Baseball Simulation'!$F$6</definedName>
     <definedName name="clPMLastRow">Parameters!$B$8</definedName>
+    <definedName name="clRWMLB">Parameters!$B$15</definedName>
+    <definedName name="clRWNBA">Parameters!$B$14</definedName>
     <definedName name="clUserWinsCache">Parameters!#REF!</definedName>
     <definedName name="cSalaryCap">Parameters!#REF!</definedName>
     <definedName name="cStatsURL">Parameters!#REF!</definedName>
     <definedName name="cTeamLocationDict">Parameters!#REF!</definedName>
     <definedName name="cUserWinsCache">Parameters!#REF!</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
@@ -59,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="878">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -2672,15 +2677,37 @@
   </si>
   <si>
     <t>Event Description</t>
+  </si>
+  <si>
+    <t>Backtest Historizing</t>
+  </si>
+  <si>
+    <t>Dailyfantasynerd NBA</t>
+  </si>
+  <si>
+    <t>Ty Lawson, Michael Carter-Williams, James Harden, Randy Foye, Danilo Gallinari, Tim Duncan, Thaddeus Young, Bismack Biyombo</t>
+  </si>
+  <si>
+    <t>Rotowire NBA</t>
+  </si>
+  <si>
+    <t>Kemba Walker, Devin Harris, James Harden, Monta Ellis, LeBron James, Dirk Nowitzki, Carl Landry, Tyson Chandler</t>
+  </si>
+  <si>
+    <t>Rotowire MLB</t>
+  </si>
+  <si>
+    <t>Chris Sale, Derek Norris, David Ortiz, Brian Dozier, Brett Lawrie, Charlie Blackmon, Michael Cuddyer, Khristopher Davis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -3126,7 +3153,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3159,6 +3186,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
@@ -3206,8 +3235,36 @@
     <cellStyle name="Total 2" xfId="42"/>
     <cellStyle name="Warning Text" xfId="3" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3342,11 +3399,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="233256448"/>
-        <c:axId val="233257984"/>
+        <c:axId val="81543552"/>
+        <c:axId val="81545088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="233256448"/>
+        <c:axId val="81543552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3355,7 +3412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233257984"/>
+        <c:crossAx val="81545088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3363,7 +3420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233257984"/>
+        <c:axId val="81545088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3374,7 +3431,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233256448"/>
+        <c:crossAx val="81543552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3487,11 +3544,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233294464"/>
-        <c:axId val="233300352"/>
+        <c:axId val="81569280"/>
+        <c:axId val="81570816"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="233294464"/>
+        <c:axId val="81569280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3500,7 +3557,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233300352"/>
+        <c:crossAx val="81570816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3508,7 +3565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233300352"/>
+        <c:axId val="81570816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3519,7 +3576,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233294464"/>
+        <c:crossAx val="81569280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8227,7 +8284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -8946,8 +9003,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9028,16 +9085,36 @@
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
+      <c r="A12" s="18" t="s">
+        <v>871</v>
+      </c>
+      <c r="B12" s="19">
+        <v>42106</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>875</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>

</xml_diff>

<commit_message>
fix bug in BBSim that resulted from not deleting correcting line in get_connection_cursor after merge conflit (always returns a regular cursor)
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="10320" windowHeight="9840" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="10320" windowHeight="9840" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="880">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -2698,6 +2698,12 @@
   </si>
   <si>
     <t>Chris Sale, Derek Norris, David Ortiz, Brian Dozier, Brett Lawrie, Charlie Blackmon, Michael Cuddyer, Khristopher Davis</t>
+  </si>
+  <si>
+    <t>Flyout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Trout flies out to right fielder Nelson Cruz.  </t>
   </si>
 </sst>
 </file>
@@ -3399,11 +3405,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="81543552"/>
-        <c:axId val="81545088"/>
+        <c:axId val="229890688"/>
+        <c:axId val="229896576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81543552"/>
+        <c:axId val="229890688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3412,7 +3418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81545088"/>
+        <c:crossAx val="229896576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3420,7 +3426,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81545088"/>
+        <c:axId val="229896576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3431,7 +3437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81543552"/>
+        <c:crossAx val="229890688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3544,11 +3550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81569280"/>
-        <c:axId val="81570816"/>
+        <c:axId val="230449152"/>
+        <c:axId val="230450688"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="81569280"/>
+        <c:axId val="230449152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3557,7 +3563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81570816"/>
+        <c:crossAx val="230450688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3565,7 +3571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81570816"/>
+        <c:axId val="230450688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3576,7 +3582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81569280"/>
+        <c:crossAx val="230449152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8284,7 +8290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -8338,7 +8344,7 @@
         <v>862</v>
       </c>
       <c r="F7">
-        <v>543068</v>
+        <v>405395</v>
       </c>
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.25">
@@ -8360,20 +8366,24 @@
       <c r="E11" t="s">
         <v>863</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>870</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>879</v>
+      </c>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>868</v>
       </c>
       <c r="F13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -9003,7 +9013,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Solid Sport Class framework started. API calls to XMSStats built, next step need to store data in database
</commit_message>
<xml_diff>
--- a/Fanduel.xlsx
+++ b/Fanduel.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="881">
   <si>
     <t>n_scripts_list</t>
   </si>
@@ -2583,30 +2583,18 @@
     <t>Philip Varone</t>
   </si>
   <si>
-    <t>[u'+106', u'-117']</t>
-  </si>
-  <si>
     <t>[u'-165', u'+149']</t>
   </si>
   <si>
     <t>[u'+143', u'-158']</t>
   </si>
   <si>
-    <t>[u'+132', u'-146']</t>
-  </si>
-  <si>
-    <t>[u'-129', u'+117']</t>
-  </si>
-  <si>
     <t>[u'-127', u'+115']</t>
   </si>
   <si>
     <t>[u'+191', u'-213']</t>
   </si>
   <si>
-    <t>{u'PHI': 46.08, u'STL': 43.48, u'CHI': 60.0, u'MIN': 61.24, u'TOR': 37.04, u'WSH': 48.54, u'LAK': 55.56, u'DET': 53.92, u'OTT': 66.67, u'SJS': 59.35, u'WIN': 41.15, u'NYR': 68.05, u'DAL': 43.1, u'MTL': 55.95, u'CAR': 62.26, u'FLA': 46.51, u'VAN': 46.95, u'BUF': 40.16, u'CBJ': 34.36, u'PIT': 56.33}</t>
-  </si>
-  <si>
     <t>['OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT', 'OTT']</t>
   </si>
   <si>
@@ -2704,6 +2692,21 @@
   </si>
   <si>
     <t xml:space="preserve">Mike Trout flies out to right fielder Nelson Cruz.  </t>
+  </si>
+  <si>
+    <t>[u'+130', u'-144']</t>
+  </si>
+  <si>
+    <t>[u'+128', u'-141']</t>
+  </si>
+  <si>
+    <t>[u'+116', u'-128']</t>
+  </si>
+  <si>
+    <t>[u'+105', u'-116']</t>
+  </si>
+  <si>
+    <t>{u'VAN': 58.51, u'WSH': 59.02, u'CGY': 43.86, u'NAS': 53.7, u'NYI': 43.48, u'MTL': 56.14, u'CHI': 48.78, u'OTT': 46.3}</t>
   </si>
 </sst>
 </file>
@@ -3159,7 +3162,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3194,6 +3197,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
@@ -3405,11 +3409,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="229890688"/>
-        <c:axId val="229896576"/>
+        <c:axId val="212944384"/>
+        <c:axId val="212945920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="229890688"/>
+        <c:axId val="212944384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3418,7 +3422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229896576"/>
+        <c:crossAx val="212945920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3426,7 +3430,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="229896576"/>
+        <c:axId val="212945920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3437,7 +3441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="229890688"/>
+        <c:crossAx val="212944384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3550,11 +3554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="230449152"/>
-        <c:axId val="230450688"/>
+        <c:axId val="212982400"/>
+        <c:axId val="212988288"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="230449152"/>
+        <c:axId val="212982400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3563,7 +3567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230450688"/>
+        <c:crossAx val="212988288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3571,7 +3575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230450688"/>
+        <c:axId val="212988288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,7 +3586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230449152"/>
+        <c:crossAx val="212982400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4249,7 +4253,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4257,7 +4261,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4326,7 +4330,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -4334,7 +4338,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B15" t="s">
         <v>210</v>
@@ -4527,24 +4531,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B1" t="s">
         <v>811</v>
       </c>
-      <c r="B1" t="s">
-        <v>786</v>
-      </c>
       <c r="C1" t="s">
-        <v>839</v>
+        <v>876</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>812</v>
+        <v>794</v>
       </c>
       <c r="B2" t="s">
-        <v>788</v>
+        <v>805</v>
       </c>
       <c r="C2" t="s">
-        <v>821</v>
+        <v>877</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4555,7 +4559,7 @@
         <v>808</v>
       </c>
       <c r="C3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4566,29 +4570,29 @@
         <v>787</v>
       </c>
       <c r="C4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>792</v>
+        <v>812</v>
       </c>
       <c r="B5" t="s">
-        <v>816</v>
+        <v>798</v>
       </c>
       <c r="C5" t="s">
-        <v>842</v>
+        <v>878</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>784</v>
+        <v>802</v>
       </c>
       <c r="B6" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="C6" t="s">
-        <v>843</v>
+        <v>879</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -4599,7 +4603,7 @@
         <v>799</v>
       </c>
       <c r="C7" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4621,7 +4625,7 @@
         <v>791</v>
       </c>
       <c r="C9" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4690,7 +4694,7 @@
         <v>815</v>
       </c>
       <c r="E15" t="s">
-        <v>846</v>
+        <v>880</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -8288,10 +8292,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E2:H13"/>
+  <dimension ref="E2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8299,17 +8303,18 @@
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -8317,7 +8322,7 @@
     </row>
     <row r="4" spans="5:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E4" s="5" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="F4" s="5">
         <v>1</v>
@@ -8325,15 +8330,15 @@
     </row>
     <row r="5" spans="5:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E5" s="5" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="F6">
         <v>572020</v>
@@ -8341,7 +8346,7 @@
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="F7">
         <v>405395</v>
@@ -8349,41 +8354,47 @@
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="F13">
         <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="20">
+        <f ca="1">NOW()</f>
+        <v>42107.74542835648</v>
       </c>
     </row>
   </sheetData>
@@ -9096,7 +9107,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="B12" s="19">
         <v>42106</v>
@@ -9104,26 +9115,26 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -16176,7 +16187,7 @@
         <v>650</v>
       </c>
       <c r="B2" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="C2" t="s">
         <v>158</v>
@@ -16193,7 +16204,7 @@
         <v>422</v>
       </c>
       <c r="B3" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="C3" t="s">
         <v>159</v>
@@ -16210,7 +16221,7 @@
         <v>692</v>
       </c>
       <c r="B4" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="C4" t="s">
         <v>161</v>
@@ -16227,7 +16238,7 @@
         <v>478</v>
       </c>
       <c r="B5" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="C5" t="s">
         <v>157</v>
@@ -16244,7 +16255,7 @@
         <v>505</v>
       </c>
       <c r="B6" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="C6" t="s">
         <v>158</v>
@@ -16261,7 +16272,7 @@
         <v>589</v>
       </c>
       <c r="B7" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="C7" t="s">
         <v>159</v>
@@ -16275,10 +16286,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B8" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="C8" t="s">
         <v>160</v>
@@ -16295,7 +16306,7 @@
         <v>587</v>
       </c>
       <c r="B9" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="C9" t="s">
         <v>157</v>
@@ -16312,7 +16323,7 @@
         <v>775</v>
       </c>
       <c r="B10" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C10" t="s">
         <v>160</v>

</xml_diff>